<commit_message>
Implemented new test data 102 and 103
</commit_message>
<xml_diff>
--- a/resources/test_data/VM_TestData_Sample1.xlsx
+++ b/resources/test_data/VM_TestData_Sample1.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22223"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_1520\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\praneethm\git\VMSeleniumFramework\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="135" documentId="8_{99F63481-3AA7-4202-BA2E-1971EFDF920A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E4AF0BC1-DEC3-423C-A10C-76C9F644C132}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LogInPage" sheetId="22" r:id="rId1"/>
     <sheet name="IndexPage" sheetId="23" r:id="rId2"/>
     <sheet name="NewSubmissionPage" sheetId="24" r:id="rId3"/>
+    <sheet name="SubmissionSummaryPage" sheetId="25" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
     <definedName name="Abc">#REF!</definedName>
@@ -28,7 +28,7 @@
     <definedName name="State">[1]Selectlists!$C$2:$C$52</definedName>
     <definedName name="waivsub">[1]Selectlists!$J$2:$J$6</definedName>
   </definedNames>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="67">
   <si>
     <t>TestCaseNumber</t>
   </si>
@@ -76,12 +76,6 @@
     <t>P@ssw0rd</t>
   </si>
   <si>
-    <t>Richard</t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
     <t>NewSubmission</t>
   </si>
   <si>
@@ -103,6 +97,9 @@
     <t>Apt</t>
   </si>
   <si>
+    <t>MailingAddress</t>
+  </si>
+  <si>
     <t>LegalEntityType</t>
   </si>
   <si>
@@ -112,9 +109,6 @@
     <t>SubIndustryType</t>
   </si>
   <si>
-    <t>BussinessPhone</t>
-  </si>
-  <si>
     <t>EmailId</t>
   </si>
   <si>
@@ -136,12 +130,12 @@
     <t>Madison</t>
   </si>
   <si>
-    <t>Wisconsin</t>
-  </si>
-  <si>
     <t>123 New Street</t>
   </si>
   <si>
+    <t>click</t>
+  </si>
+  <si>
     <t>Individual</t>
   </si>
   <si>
@@ -166,9 +160,6 @@
     <t>edw982347-Edward Bella</t>
   </si>
   <si>
-    <t>click</t>
-  </si>
-  <si>
     <t>John miller</t>
   </si>
   <si>
@@ -178,21 +169,12 @@
     <t>Belgium</t>
   </si>
   <si>
-    <t>Limburg</t>
-  </si>
-  <si>
     <t>jhgfugfgb</t>
   </si>
   <si>
     <t>Zinkare zoth</t>
   </si>
   <si>
-    <t>42-Wholesale Trade</t>
-  </si>
-  <si>
-    <t>423210-Furniture Merchan</t>
-  </si>
-  <si>
     <t>(121)212-1212</t>
   </si>
   <si>
@@ -203,13 +185,73 @@
   </si>
   <si>
     <t xml:space="preserve">edw982347-Edward Bella		</t>
+  </si>
+  <si>
+    <t>Thomas Submission</t>
+  </si>
+  <si>
+    <t>Bountiful</t>
+  </si>
+  <si>
+    <t>86 East White Street Chicopee</t>
+  </si>
+  <si>
+    <t>77 S. Hartford Ave. South Portland</t>
+  </si>
+  <si>
+    <t>Association</t>
+  </si>
+  <si>
+    <t>111140 - Wheat Farming</t>
+  </si>
+  <si>
+    <t>(456) 489 - 7879</t>
+  </si>
+  <si>
+    <t>thomas@mailinator.com</t>
+  </si>
+  <si>
+    <t>Back</t>
+  </si>
+  <si>
+    <t>BusinessPhone</t>
+  </si>
+  <si>
+    <t>CommercialAuto</t>
+  </si>
+  <si>
+    <t>SSN</t>
+  </si>
+  <si>
+    <t>654-98-8797</t>
+  </si>
+  <si>
+    <t>SelectUser</t>
+  </si>
+  <si>
+    <t>SelectAndProceed</t>
+  </si>
+  <si>
+    <t>CreateSubmission1</t>
+  </si>
+  <si>
+    <t>42 -Wholesale Trade</t>
+  </si>
+  <si>
+    <t>423210 - Furniture Merchant Wholesalers</t>
+  </si>
+  <si>
+    <t>FEIN</t>
+  </si>
+  <si>
+    <t>31-5151365</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,6 +283,12 @@
       <sz val="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF393939"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -260,16 +308,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF505050"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF505050"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF505050"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF505050"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -278,28 +326,69 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -960,96 +1049,97 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE9F756-70FA-49A6-8EFC-F2E5D2624C1B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
         <v>101</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="2">
+      <c r="F2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
         <v>102</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="2">
+      <c r="F3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
         <v>103</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1059,50 +1149,72 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54FC45A2-B671-4782-8528-E34EC00CFD7D}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>101</v>
       </c>
       <c r="B2" s="1">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>102</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>103</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>103</v>
+      </c>
+      <c r="B5" s="1">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1112,192 +1224,456 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4736F30D-6BC0-4A5B-8AEF-44942C7CDE4B}">
-  <dimension ref="A1:Q3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1"/>
-    <col min="10" max="10" width="38.28515625" customWidth="1"/>
-    <col min="11" max="12" width="16.42578125" customWidth="1"/>
-    <col min="13" max="13" width="17.28515625" customWidth="1"/>
-    <col min="14" max="15" width="21.28515625" customWidth="1"/>
-    <col min="16" max="16" width="26" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="28" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="38.28515625" customWidth="1"/>
+    <col min="12" max="12" width="48.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="16.42578125" customWidth="1"/>
+    <col min="16" max="16" width="17.28515625" customWidth="1"/>
+    <col min="17" max="19" width="21.28515625" customWidth="1"/>
+    <col min="20" max="20" width="26" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.140625" customWidth="1"/>
+    <col min="22" max="22" width="15.5703125" customWidth="1"/>
+    <col min="23" max="23" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
-      <c r="A1" t="s">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="L1" t="s">
+      <c r="Q1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="M1" t="s">
+      <c r="R1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="S1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="N1" t="s">
+      <c r="T1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="O1" t="s">
+      <c r="U1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="P1" t="s">
+      <c r="V1" t="s">
+        <v>60</v>
+      </c>
+      <c r="W1" t="s">
+        <v>61</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>101</v>
+      </c>
+      <c r="B2" s="3">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="D2" s="3">
+        <v>53704</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:17">
-      <c r="A2" s="1">
-        <v>101</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="N2" s="4"/>
+      <c r="O2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>102</v>
+      </c>
+      <c r="B3" s="3">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="N3" s="4"/>
+      <c r="O3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>103</v>
+      </c>
+      <c r="B4" s="3">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="3">
+        <v>53704</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D2">
-        <v>53704</v>
-      </c>
-      <c r="E2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="H4" s="3"/>
+      <c r="I4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G2" t="s">
+      <c r="K4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I2" t="s">
+      <c r="L4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="J2" t="s">
+      <c r="M4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="N4" s="4"/>
+      <c r="O4" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="P4" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="Q4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="R4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="S4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="T4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="O2" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
-      <c r="A3">
-        <v>102</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="H3" t="s">
-        <v>46</v>
-      </c>
-      <c r="I3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J3" s="5" t="s">
+      <c r="U4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>103</v>
+      </c>
+      <c r="B5" s="3">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="D5" s="3">
+        <v>84010</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="F5" s="3"/>
+      <c r="G5" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="H5" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="I5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="O3" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="P3" s="5" t="s">
+      <c r="K5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="Q3" t="s">
-        <v>40</v>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="P5" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="D3:E3 G3 J3 L2:M3" xr:uid="{D4273C39-AEEA-4B3B-B9E8-E6E79339CF6E}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="D3:E3 G3 K3 O2:P4"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" display="random123@gmail.com" xr:uid="{12A744AB-7DF7-4981-8D89-14F426B34CD8}"/>
-    <hyperlink ref="E3" r:id="rId2" display="random123@gmail.com" xr:uid="{7D077161-16F4-4D69-BE58-DA8B165A9AEA}"/>
+    <hyperlink ref="D3" r:id="rId1" display="random123@gmail.com"/>
+    <hyperlink ref="E3" r:id="rId2" display="random123@gmail.com"/>
+    <hyperlink ref="P5" r:id="rId3"/>
   </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>101</v>
+      </c>
+      <c r="B2" s="3">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>102</v>
+      </c>
+      <c r="B3" s="3">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>103</v>
+      </c>
+      <c r="B4" s="3">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert and CheckIn tested code.
</commit_message>
<xml_diff>
--- a/resources/test_data/VM_TestData_Sample1.xlsx
+++ b/resources/test_data/VM_TestData_Sample1.xlsx
@@ -1,24 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22223"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22229"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_1520\AC\Temp\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="135" documentId="8_{99F63481-3AA7-4202-BA2E-1971EFDF920A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E4AF0BC1-DEC3-423C-A10C-76C9F644C132}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{87F0D541-E322-4912-ABEB-F64AFEFF021B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="6060" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LogInPage" sheetId="22" r:id="rId1"/>
     <sheet name="IndexPage" sheetId="23" r:id="rId2"/>
     <sheet name="NewSubmissionPage" sheetId="24" r:id="rId3"/>
+    <sheet name="SubmissionSummaryPage" sheetId="25" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
     <definedName name="Abc">#REF!</definedName>
@@ -44,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="76">
   <si>
     <t>TestCaseNumber</t>
   </si>
@@ -103,6 +99,9 @@
     <t>Apt</t>
   </si>
   <si>
+    <t>MailingAddress</t>
+  </si>
+  <si>
     <t>LegalEntityType</t>
   </si>
   <si>
@@ -112,7 +111,10 @@
     <t>SubIndustryType</t>
   </si>
   <si>
-    <t>BussinessPhone</t>
+    <t>SSN</t>
+  </si>
+  <si>
+    <t>BusinessPhone</t>
   </si>
   <si>
     <t>EmailId</t>
@@ -121,6 +123,9 @@
     <t>SelectProduct</t>
   </si>
   <si>
+    <t>CommercialAuto</t>
+  </si>
+  <si>
     <t>AgencyName</t>
   </si>
   <si>
@@ -130,15 +135,18 @@
     <t>CreateSubmission</t>
   </si>
   <si>
+    <t>SelectUser</t>
+  </si>
+  <si>
+    <t>SelectAndProceed</t>
+  </si>
+  <si>
     <t>Jack</t>
   </si>
   <si>
     <t>Madison</t>
   </si>
   <si>
-    <t>Wisconsin</t>
-  </si>
-  <si>
     <t>123 New Street</t>
   </si>
   <si>
@@ -151,10 +159,13 @@
     <t>111160 - Rice Farming</t>
   </si>
   <si>
+    <t>654-98-7987</t>
+  </si>
+  <si>
     <t>(654) 987 - 9798</t>
   </si>
   <si>
-    <t>jack@gmail.com</t>
+    <t>jack123@gmail.com</t>
   </si>
   <si>
     <t>Commercial Auto</t>
@@ -166,49 +177,103 @@
     <t>edw982347-Edward Bella</t>
   </si>
   <si>
+    <t>John miller</t>
+  </si>
+  <si>
+    <t>53004</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>jhgfugfgb</t>
+  </si>
+  <si>
+    <t>Zinkare zoth</t>
+  </si>
+  <si>
+    <t>42-Wholesale Trade</t>
+  </si>
+  <si>
+    <t>423210-Furniture Merchan</t>
+  </si>
+  <si>
+    <t>(121)212-1212</t>
+  </si>
+  <si>
+    <t>john@gmail.com</t>
+  </si>
+  <si>
+    <t>Commercial Property</t>
+  </si>
+  <si>
+    <t xml:space="preserve">edw982347-Edward Bella		</t>
+  </si>
+  <si>
+    <t>JohnKristin</t>
+  </si>
+  <si>
+    <t>SaltLakeCity</t>
+  </si>
+  <si>
+    <t>Alaska</t>
+  </si>
+  <si>
+    <t>Ameklari</t>
+  </si>
+  <si>
+    <t>Foreign Limited Liability</t>
+  </si>
+  <si>
+    <t>32 - Manufacturing-Wood, paper, printing, chemical, plastics, non-metallic minerals</t>
+  </si>
+  <si>
+    <t>321219 - Reconstituted Wood Product Manufacturing</t>
+  </si>
+  <si>
+    <t>(565) 865 - 6856</t>
+  </si>
+  <si>
+    <t>ashdkjhskjdh@fshgdf.com</t>
+  </si>
+  <si>
+    <t>General Liability</t>
+  </si>
+  <si>
+    <t>Thomas Submission</t>
+  </si>
+  <si>
+    <t>Bountiful</t>
+  </si>
+  <si>
+    <t>86 East White Street Chicopee</t>
+  </si>
+  <si>
+    <t>77 S. Hartford Ave. South Portland</t>
+  </si>
+  <si>
+    <t>Association</t>
+  </si>
+  <si>
+    <t>111140 - Wheat Farming</t>
+  </si>
+  <si>
+    <t>(456) 489 - 7879</t>
+  </si>
+  <si>
+    <t>thomas@mailinator.com</t>
+  </si>
+  <si>
+    <t>Back</t>
+  </si>
+  <si>
     <t>click</t>
-  </si>
-  <si>
-    <t>John miller</t>
-  </si>
-  <si>
-    <t>53004</t>
-  </si>
-  <si>
-    <t>Belgium</t>
-  </si>
-  <si>
-    <t>Limburg</t>
-  </si>
-  <si>
-    <t>jhgfugfgb</t>
-  </si>
-  <si>
-    <t>Zinkare zoth</t>
-  </si>
-  <si>
-    <t>42-Wholesale Trade</t>
-  </si>
-  <si>
-    <t>423210-Furniture Merchan</t>
-  </si>
-  <si>
-    <t>(121)212-1212</t>
-  </si>
-  <si>
-    <t>john@gmail.com</t>
-  </si>
-  <si>
-    <t>Commercial Property</t>
-  </si>
-  <si>
-    <t xml:space="preserve">edw982347-Edward Bella		</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -250,7 +315,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -260,16 +325,31 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF505050"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF505050"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF505050"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF505050"/>
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -278,28 +358,75 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -960,11 +1087,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE9F756-70FA-49A6-8EFC-F2E5D2624C1B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -974,82 +1101,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="2">
+      <c r="A2" s="4">
         <v>101</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="2">
+      <c r="A3" s="4">
         <v>102</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="2">
+      <c r="A4" s="4">
         <v>103</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1059,11 +1186,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54FC45A2-B671-4782-8528-E34EC00CFD7D}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1074,13 +1201,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1091,7 +1218,7 @@
       <c r="B2" s="1">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1102,7 +1229,29 @@
       <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
+        <v>103</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
+        <v>103</v>
+      </c>
+      <c r="B5" s="1">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1112,11 +1261,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4736F30D-6BC0-4A5B-8AEF-44942C7CDE4B}">
-  <dimension ref="A1:Q3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="U3" sqref="A1:W5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1125,179 +1274,436 @@
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1"/>
-    <col min="10" max="10" width="38.28515625" customWidth="1"/>
-    <col min="11" max="12" width="16.42578125" customWidth="1"/>
-    <col min="13" max="13" width="17.28515625" customWidth="1"/>
-    <col min="14" max="15" width="21.28515625" customWidth="1"/>
-    <col min="16" max="16" width="26" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="28" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" customWidth="1"/>
+    <col min="11" max="11" width="38.28515625" customWidth="1"/>
+    <col min="12" max="12" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="16.42578125" customWidth="1"/>
+    <col min="15" max="15" width="25.140625" customWidth="1"/>
+    <col min="16" max="18" width="21.28515625" customWidth="1"/>
+    <col min="19" max="19" width="26" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
-      <c r="A1" t="s">
+    <row r="1" spans="1:23">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="R1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="2" spans="1:17">
-      <c r="A2" s="1">
+    <row r="2" spans="1:23">
+      <c r="A2" s="5">
         <v>101</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="5">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2">
+      <c r="C2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="5">
         <v>53704</v>
       </c>
-      <c r="E2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J2" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" s="3" t="s">
+      <c r="E2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="F2" s="5"/>
+      <c r="G2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="H2" s="5"/>
+      <c r="I2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="L2" s="7" t="s">
         <v>38</v>
       </c>
+      <c r="M2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>41</v>
+      </c>
       <c r="P2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="W2" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23">
+      <c r="A3" s="5">
+        <v>102</v>
+      </c>
+      <c r="B3" s="5">
+        <v>3</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="M3" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="Q2" t="s">
-        <v>40</v>
+      <c r="N3" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
-      <c r="A3">
-        <v>102</v>
-      </c>
-      <c r="B3">
+    <row r="4" spans="1:23">
+      <c r="A4" s="5">
+        <v>103</v>
+      </c>
+      <c r="B4" s="5">
         <v>3</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="7" t="s">
+      <c r="C4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="5">
+        <v>84101</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S4" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="T4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="U4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="V4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="W4" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23">
+      <c r="A5" s="5">
+        <v>103</v>
+      </c>
+      <c r="B5" s="5">
+        <v>6</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="5">
+        <v>84010</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O5" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="P5" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="Q5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="R5" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F3" t="s">
+      <c r="S5" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="H3" t="s">
-        <v>46</v>
-      </c>
-      <c r="I3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>40</v>
+      <c r="T5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="U5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="V5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="W5" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="D3:E3 G3 J3 L2:M3" xr:uid="{D4273C39-AEEA-4B3B-B9E8-E6E79339CF6E}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="D3:E3 G3 K3 N2:O3" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" display="random123@gmail.com" xr:uid="{12A744AB-7DF7-4981-8D89-14F426B34CD8}"/>
-    <hyperlink ref="E3" r:id="rId2" display="random123@gmail.com" xr:uid="{7D077161-16F4-4D69-BE58-DA8B165A9AEA}"/>
+    <hyperlink ref="D3" r:id="rId1" display="random123@gmail.com" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" display="random123@gmail.com" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="O4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="O5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="O2" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="3">
+        <v>101</v>
+      </c>
+      <c r="B2" s="3">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3">
+        <v>102</v>
+      </c>
+      <c r="B3" s="3">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3">
+        <v>103</v>
+      </c>
+      <c r="B4" s="3">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated the test data of 103 test case
</commit_message>
<xml_diff>
--- a/resources/test_data/VM_TestData_Sample1.xlsx
+++ b/resources/test_data/VM_TestData_Sample1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="6060" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="6060" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LogInPage" sheetId="22" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="80">
   <si>
     <t>TestCaseNumber</t>
   </si>
@@ -215,18 +215,12 @@
     <t>JohnKristin</t>
   </si>
   <si>
-    <t>SaltLakeCity</t>
-  </si>
-  <si>
     <t>Alaska</t>
   </si>
   <si>
     <t>Ameklari</t>
   </si>
   <si>
-    <t>Foreign Limited Liability</t>
-  </si>
-  <si>
     <t>32 - Manufacturing-Wood, paper, printing, chemical, plastics, non-metallic minerals</t>
   </si>
   <si>
@@ -279,13 +273,25 @@
   </si>
   <si>
     <t>ServicePolicy</t>
+  </si>
+  <si>
+    <t>Salt Lake City</t>
+  </si>
+  <si>
+    <t>Foreign Limited Liability Company</t>
+  </si>
+  <si>
+    <t>FEIN</t>
+  </si>
+  <si>
+    <t>21-3113154</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -316,6 +322,12 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF393939"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -380,7 +392,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -417,6 +429,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1234,8 +1247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1257,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1324,10 +1337,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W5"/>
+  <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1336,20 +1349,23 @@
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.28515625" customWidth="1"/>
     <col min="7" max="7" width="28" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" customWidth="1"/>
     <col min="11" max="11" width="38.28515625" customWidth="1"/>
     <col min="12" max="12" width="48.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="16.42578125" customWidth="1"/>
-    <col min="15" max="15" width="25.140625" customWidth="1"/>
-    <col min="16" max="18" width="21.28515625" customWidth="1"/>
-    <col min="19" max="19" width="26" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="15.5703125" customWidth="1"/>
-    <col min="23" max="23" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="16.42578125" customWidth="1"/>
+    <col min="16" max="16" width="25.140625" customWidth="1"/>
+    <col min="17" max="19" width="21.28515625" customWidth="1"/>
+    <col min="20" max="20" width="26" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="15.5703125" customWidth="1"/>
+    <col min="23" max="23" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1389,38 +1405,41 @@
       <c r="M1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="O1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="V1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="W1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>101</v>
       </c>
@@ -1456,27 +1475,25 @@
       <c r="M2" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="N2" s="7"/>
+      <c r="O2" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="P2" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="Q2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="Q2" s="5" t="s">
-        <v>8</v>
-      </c>
       <c r="R2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="S2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="T2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="T2" s="5" t="s">
-        <v>8</v>
-      </c>
       <c r="U2" s="5" t="s">
         <v>8</v>
       </c>
@@ -1486,8 +1503,11 @@
       <c r="W2" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X2" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>102</v>
       </c>
@@ -1525,27 +1545,25 @@
       <c r="M3" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="N3" s="7"/>
+      <c r="O3" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="P3" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="Q3" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="Q3" s="5" t="s">
-        <v>8</v>
-      </c>
       <c r="R3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="S3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="S3" s="5" t="s">
+      <c r="T3" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="T3" s="5" t="s">
-        <v>8</v>
-      </c>
       <c r="U3" s="5" t="s">
         <v>8</v>
       </c>
@@ -1555,8 +1573,11 @@
       <c r="W3" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X3" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>103</v>
       </c>
@@ -1570,51 +1591,49 @@
         <v>84101</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="K4" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="M4" s="5"/>
+      <c r="N4" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="O4" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="P4" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="M4" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="N4" s="5" t="s">
+      <c r="Q4" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="O4" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="P4" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q4" s="5" t="s">
-        <v>8</v>
-      </c>
       <c r="R4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="S4" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="S4" s="5" t="s">
+      <c r="T4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="T4" s="5" t="s">
-        <v>8</v>
-      </c>
       <c r="U4" s="5" t="s">
         <v>8</v>
       </c>
@@ -1624,8 +1643,11 @@
       <c r="W4" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X4" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>103</v>
       </c>
@@ -1633,57 +1655,55 @@
         <v>6</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D5" s="5">
         <v>84010</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="K5" s="5" t="s">
         <v>36</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M5" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="N5" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="O5" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="P5" s="5" t="s">
+      <c r="N5" s="5"/>
+      <c r="O5" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="P5" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q5" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="Q5" s="5" t="s">
-        <v>8</v>
-      </c>
       <c r="R5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="S5" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="S5" s="5" t="s">
+      <c r="T5" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="T5" s="5" t="s">
-        <v>8</v>
-      </c>
       <c r="U5" s="5" t="s">
         <v>8</v>
       </c>
@@ -1691,21 +1711,25 @@
         <v>8</v>
       </c>
       <c r="W5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="X5" s="5" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="D3:E3 G3 K3 N2:O3"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="D3:E3 G3 K3 O2:P3"/>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" display="random123@gmail.com"/>
     <hyperlink ref="E3" r:id="rId2" display="random123@gmail.com"/>
-    <hyperlink ref="O4" r:id="rId3"/>
-    <hyperlink ref="O5" r:id="rId4"/>
-    <hyperlink ref="O2" r:id="rId5"/>
+    <hyperlink ref="P4" r:id="rId3"/>
+    <hyperlink ref="P5" r:id="rId4"/>
+    <hyperlink ref="P2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -1735,10 +1759,10 @@
         <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1782,7 +1806,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1793,7 +1817,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1804,7 +1828,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1815,7 +1839,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update for Task 27
</commit_message>
<xml_diff>
--- a/resources/test_data/VM_TestData_Sample1.xlsx
+++ b/resources/test_data/VM_TestData_Sample1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22229"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\praneethm\git\VMSeleniumFramework\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1FC30A6F-ACD7-4C53-8719-EE7A70C284BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="6060" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="6060" firstSheet="2" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LogInPage" sheetId="22" r:id="rId1"/>
@@ -29,7 +30,7 @@
     <definedName name="State">[1]Selectlists!$C$2:$C$52</definedName>
     <definedName name="waivsub">[1]Selectlists!$J$2:$J$6</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -45,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="82">
   <si>
     <t>TestCaseNumber</t>
   </si>
@@ -77,9 +80,18 @@
     <t>P@ssw0rd</t>
   </si>
   <si>
+    <t>VerifyUser</t>
+  </si>
+  <si>
     <t>NewSubmission</t>
   </si>
   <si>
+    <t>ServicePolicy</t>
+  </si>
+  <si>
+    <t>AreEqual&gt;Thomas Charles</t>
+  </si>
+  <si>
     <t>CustomerAccountName</t>
   </si>
   <si>
@@ -113,6 +125,9 @@
     <t>SSN</t>
   </si>
   <si>
+    <t>FEIN</t>
+  </si>
+  <si>
     <t>BusinessPhone</t>
   </si>
   <si>
@@ -215,18 +230,27 @@
     <t>JohnKristin</t>
   </si>
   <si>
+    <t>Salt Lake City</t>
+  </si>
+  <si>
     <t>Alaska</t>
   </si>
   <si>
     <t>Ameklari</t>
   </si>
   <si>
+    <t>Foreign Limited Liability Company</t>
+  </si>
+  <si>
     <t>32 - Manufacturing-Wood, paper, printing, chemical, plastics, non-metallic minerals</t>
   </si>
   <si>
     <t>321219 - Reconstituted Wood Product Manufacturing</t>
   </si>
   <si>
+    <t>21-3113154</t>
+  </si>
+  <si>
     <t>(565) 865 - 6856</t>
   </si>
   <si>
@@ -260,38 +284,23 @@
     <t>thomas@mailinator.com</t>
   </si>
   <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>Actions</t>
+  </si>
+  <si>
     <t>Back</t>
   </si>
   <si>
     <t>click</t>
-  </si>
-  <si>
-    <t>Search</t>
-  </si>
-  <si>
-    <t>Actions</t>
-  </si>
-  <si>
-    <t>ServicePolicy</t>
-  </si>
-  <si>
-    <t>Salt Lake City</t>
-  </si>
-  <si>
-    <t>Foreign Limited Liability Company</t>
-  </si>
-  <si>
-    <t>FEIN</t>
-  </si>
-  <si>
-    <t>21-3113154</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -460,7 +469,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -1125,20 +1134,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1158,7 +1167,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="4">
         <v>101</v>
       </c>
@@ -1178,7 +1187,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="4">
         <v>102</v>
       </c>
@@ -1198,7 +1207,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="4">
         <v>103</v>
       </c>
@@ -1218,7 +1227,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="13">
         <v>104</v>
       </c>
@@ -1244,22 +1253,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1269,11 +1279,14 @@
       <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>101</v>
       </c>
@@ -1281,44 +1294,50 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>102</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>103</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>103</v>
       </c>
       <c r="B5" s="1">
         <v>5</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>104</v>
       </c>
@@ -1326,7 +1345,8 @@
         <v>2</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1336,14 +1356,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
@@ -1365,7 +1385,7 @@
     <col min="24" max="24" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1373,73 +1393,73 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="N1" s="14" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T1" s="5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="U1" s="5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="V1" s="6" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="W1" s="6" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="X1" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
       <c r="A2" s="5">
         <v>101</v>
       </c>
@@ -1447,52 +1467,52 @@
         <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D2" s="5">
         <v>53704</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="N2" s="7"/>
       <c r="O2" s="8" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="P2" s="9" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="R2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="U2" s="5" t="s">
         <v>8</v>
@@ -1507,7 +1527,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24">
       <c r="A3" s="5">
         <v>102</v>
       </c>
@@ -1515,54 +1535,54 @@
         <v>3</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="10" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="N3" s="7"/>
       <c r="O3" s="8" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="R3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="S3" s="5" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="T3" s="5" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="U3" s="5" t="s">
         <v>8</v>
@@ -1577,7 +1597,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24">
       <c r="A4" s="5">
         <v>103</v>
       </c>
@@ -1585,54 +1605,54 @@
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D4" s="5">
         <v>84101</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="M4" s="5"/>
       <c r="N4" s="5" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="P4" s="12" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="R4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="S4" s="5" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="T4" s="5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="U4" s="5" t="s">
         <v>8</v>
@@ -1647,7 +1667,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24">
       <c r="A5" s="5">
         <v>103</v>
       </c>
@@ -1655,54 +1675,54 @@
         <v>6</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="D5" s="5">
         <v>84010</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>8</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="N5" s="5"/>
       <c r="O5" s="5" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="P5" s="12" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="R5" s="5" t="s">
         <v>8</v>
       </c>
       <c r="S5" s="5" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="T5" s="5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="U5" s="5" t="s">
         <v>8</v>
@@ -1719,14 +1739,14 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="D3:E3 G3 K3 O2:P3"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="D3:E3 G3 K3 O2:P3" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" display="random123@gmail.com"/>
-    <hyperlink ref="E3" r:id="rId2" display="random123@gmail.com"/>
-    <hyperlink ref="P4" r:id="rId3"/>
-    <hyperlink ref="P5" r:id="rId4"/>
-    <hyperlink ref="P2" r:id="rId5"/>
+    <hyperlink ref="D3" r:id="rId1" display="random123@gmail.com" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" display="random123@gmail.com" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="P4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="P5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="P2" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
@@ -1734,21 +1754,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.28515625" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1756,16 +1776,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="E1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>104</v>
       </c>
@@ -1773,7 +1793,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -1788,17 +1808,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1806,10 +1826,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="3">
         <v>101</v>
       </c>
@@ -1817,10 +1837,10 @@
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="3">
         <v>102</v>
       </c>
@@ -1828,10 +1848,10 @@
         <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="3">
         <v>103</v>
       </c>
@@ -1839,7 +1859,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update for Task 26
</commit_message>
<xml_diff>
--- a/resources/test_data/VM_TestData_Sample1.xlsx
+++ b/resources/test_data/VM_TestData_Sample1.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\praneethm\git\VMSeleniumFramework\resources\test_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1FC30A6F-ACD7-4C53-8719-EE7A70C284BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="6060" firstSheet="2" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="6060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LogInPage" sheetId="22" r:id="rId1"/>
     <sheet name="IndexPage" sheetId="23" r:id="rId2"/>
     <sheet name="NewSubmissionPage" sheetId="24" r:id="rId3"/>
     <sheet name="ServicePolicy" sheetId="26" r:id="rId4"/>
-    <sheet name="SubmissionSummaryPage" sheetId="25" r:id="rId5"/>
+    <sheet name="CustomerInformationPage" sheetId="27" r:id="rId5"/>
+    <sheet name="SubmissionSummaryPage" sheetId="25" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
     <definedName name="Abc">#REF!</definedName>
@@ -30,7 +30,7 @@
     <definedName name="State">[1]Selectlists!$C$2:$C$52</definedName>
     <definedName name="waivsub">[1]Selectlists!$J$2:$J$6</definedName>
   </definedNames>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,9 +38,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -48,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="86">
   <si>
     <t>TestCaseNumber</t>
   </si>
@@ -80,227 +78,239 @@
     <t>P@ssw0rd</t>
   </si>
   <si>
+    <t>NewSubmission</t>
+  </si>
+  <si>
+    <t>CustomerAccountName</t>
+  </si>
+  <si>
+    <t>ZipCode</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>StreetAddress</t>
+  </si>
+  <si>
+    <t>Apt</t>
+  </si>
+  <si>
+    <t>MailingAddress</t>
+  </si>
+  <si>
+    <t>LegalEntityType</t>
+  </si>
+  <si>
+    <t>IndustryType</t>
+  </si>
+  <si>
+    <t>SubIndustryType</t>
+  </si>
+  <si>
+    <t>SSN</t>
+  </si>
+  <si>
+    <t>BusinessPhone</t>
+  </si>
+  <si>
+    <t>EmailId</t>
+  </si>
+  <si>
+    <t>SelectProduct</t>
+  </si>
+  <si>
+    <t>CommercialAuto</t>
+  </si>
+  <si>
+    <t>AgencyName</t>
+  </si>
+  <si>
+    <t>AgentName</t>
+  </si>
+  <si>
+    <t>CreateSubmission</t>
+  </si>
+  <si>
+    <t>SelectUser</t>
+  </si>
+  <si>
+    <t>SelectAndProceed</t>
+  </si>
+  <si>
+    <t>CreateSubmission1</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>Madison</t>
+  </si>
+  <si>
+    <t>123 New Street</t>
+  </si>
+  <si>
+    <t>Individual</t>
+  </si>
+  <si>
+    <t>11 - Agriculture, Forestry, Fishing and Hunting</t>
+  </si>
+  <si>
+    <t>111160 - Rice Farming</t>
+  </si>
+  <si>
+    <t>654-98-7987</t>
+  </si>
+  <si>
+    <t>(654) 987 - 9798</t>
+  </si>
+  <si>
+    <t>jack123@gmail.com</t>
+  </si>
+  <si>
+    <t>Commercial Auto</t>
+  </si>
+  <si>
+    <t>pix3473-Pixel Groups</t>
+  </si>
+  <si>
+    <t>edw982347-Edward Bella</t>
+  </si>
+  <si>
+    <t>John miller</t>
+  </si>
+  <si>
+    <t>53004</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>jhgfugfgb</t>
+  </si>
+  <si>
+    <t>Zinkare zoth</t>
+  </si>
+  <si>
+    <t>42 -Wholesale Trade</t>
+  </si>
+  <si>
+    <t>423210 - Furniture Merchant Wholesalers</t>
+  </si>
+  <si>
+    <t>(121)212-1212</t>
+  </si>
+  <si>
+    <t>john@gmail.com</t>
+  </si>
+  <si>
+    <t>Commercial Property</t>
+  </si>
+  <si>
+    <t xml:space="preserve">edw982347-Edward Bella		</t>
+  </si>
+  <si>
+    <t>JohnKristin</t>
+  </si>
+  <si>
+    <t>Alaska</t>
+  </si>
+  <si>
+    <t>Ameklari</t>
+  </si>
+  <si>
+    <t>32 - Manufacturing-Wood, paper, printing, chemical, plastics, non-metallic minerals</t>
+  </si>
+  <si>
+    <t>321219 - Reconstituted Wood Product Manufacturing</t>
+  </si>
+  <si>
+    <t>(565) 865 - 6856</t>
+  </si>
+  <si>
+    <t>ashdkjhskjdh@fshgdf.com</t>
+  </si>
+  <si>
+    <t>General Liability</t>
+  </si>
+  <si>
+    <t>Thomas Submission</t>
+  </si>
+  <si>
+    <t>Bountiful</t>
+  </si>
+  <si>
+    <t>86 East White Street Chicopee</t>
+  </si>
+  <si>
+    <t>77 S. Hartford Ave. South Portland</t>
+  </si>
+  <si>
+    <t>Association</t>
+  </si>
+  <si>
+    <t>111140 - Wheat Farming</t>
+  </si>
+  <si>
+    <t>(456) 489 - 7879</t>
+  </si>
+  <si>
+    <t>thomas@mailinator.com</t>
+  </si>
+  <si>
+    <t>Back</t>
+  </si>
+  <si>
+    <t>click</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>Actions</t>
+  </si>
+  <si>
+    <t>ServicePolicy</t>
+  </si>
+  <si>
+    <t>Salt Lake City</t>
+  </si>
+  <si>
+    <t>Foreign Limited Liability Company</t>
+  </si>
+  <si>
+    <t>FEIN</t>
+  </si>
+  <si>
+    <t>21-3113154</t>
+  </si>
+  <si>
+    <t>Submissions</t>
+  </si>
+  <si>
+    <t>AddNewSubmission</t>
+  </si>
+  <si>
+    <t>Charles Submission</t>
+  </si>
+  <si>
+    <t>SelectAndProceed1</t>
+  </si>
+  <si>
     <t>VerifyUser</t>
   </si>
   <si>
-    <t>NewSubmission</t>
-  </si>
-  <si>
-    <t>ServicePolicy</t>
-  </si>
-  <si>
     <t>AreEqual&gt;Thomas Charles</t>
-  </si>
-  <si>
-    <t>CustomerAccountName</t>
-  </si>
-  <si>
-    <t>ZipCode</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>StreetAddress</t>
-  </si>
-  <si>
-    <t>Apt</t>
-  </si>
-  <si>
-    <t>MailingAddress</t>
-  </si>
-  <si>
-    <t>LegalEntityType</t>
-  </si>
-  <si>
-    <t>IndustryType</t>
-  </si>
-  <si>
-    <t>SubIndustryType</t>
-  </si>
-  <si>
-    <t>SSN</t>
-  </si>
-  <si>
-    <t>FEIN</t>
-  </si>
-  <si>
-    <t>BusinessPhone</t>
-  </si>
-  <si>
-    <t>EmailId</t>
-  </si>
-  <si>
-    <t>SelectProduct</t>
-  </si>
-  <si>
-    <t>CommercialAuto</t>
-  </si>
-  <si>
-    <t>AgencyName</t>
-  </si>
-  <si>
-    <t>AgentName</t>
-  </si>
-  <si>
-    <t>CreateSubmission</t>
-  </si>
-  <si>
-    <t>SelectUser</t>
-  </si>
-  <si>
-    <t>SelectAndProceed</t>
-  </si>
-  <si>
-    <t>CreateSubmission1</t>
-  </si>
-  <si>
-    <t>Jack</t>
-  </si>
-  <si>
-    <t>Madison</t>
-  </si>
-  <si>
-    <t>123 New Street</t>
-  </si>
-  <si>
-    <t>Individual</t>
-  </si>
-  <si>
-    <t>11 - Agriculture, Forestry, Fishing and Hunting</t>
-  </si>
-  <si>
-    <t>111160 - Rice Farming</t>
-  </si>
-  <si>
-    <t>654-98-7987</t>
-  </si>
-  <si>
-    <t>(654) 987 - 9798</t>
-  </si>
-  <si>
-    <t>jack123@gmail.com</t>
-  </si>
-  <si>
-    <t>Commercial Auto</t>
-  </si>
-  <si>
-    <t>pix3473-Pixel Groups</t>
-  </si>
-  <si>
-    <t>edw982347-Edward Bella</t>
-  </si>
-  <si>
-    <t>John miller</t>
-  </si>
-  <si>
-    <t>53004</t>
-  </si>
-  <si>
-    <t>Belgium</t>
-  </si>
-  <si>
-    <t>jhgfugfgb</t>
-  </si>
-  <si>
-    <t>Zinkare zoth</t>
-  </si>
-  <si>
-    <t>42 -Wholesale Trade</t>
-  </si>
-  <si>
-    <t>423210 - Furniture Merchant Wholesalers</t>
-  </si>
-  <si>
-    <t>(121)212-1212</t>
-  </si>
-  <si>
-    <t>john@gmail.com</t>
-  </si>
-  <si>
-    <t>Commercial Property</t>
-  </si>
-  <si>
-    <t xml:space="preserve">edw982347-Edward Bella		</t>
-  </si>
-  <si>
-    <t>JohnKristin</t>
-  </si>
-  <si>
-    <t>Salt Lake City</t>
-  </si>
-  <si>
-    <t>Alaska</t>
-  </si>
-  <si>
-    <t>Ameklari</t>
-  </si>
-  <si>
-    <t>Foreign Limited Liability Company</t>
-  </si>
-  <si>
-    <t>32 - Manufacturing-Wood, paper, printing, chemical, plastics, non-metallic minerals</t>
-  </si>
-  <si>
-    <t>321219 - Reconstituted Wood Product Manufacturing</t>
-  </si>
-  <si>
-    <t>21-3113154</t>
-  </si>
-  <si>
-    <t>(565) 865 - 6856</t>
-  </si>
-  <si>
-    <t>ashdkjhskjdh@fshgdf.com</t>
-  </si>
-  <si>
-    <t>General Liability</t>
-  </si>
-  <si>
-    <t>Thomas Submission</t>
-  </si>
-  <si>
-    <t>Bountiful</t>
-  </si>
-  <si>
-    <t>86 East White Street Chicopee</t>
-  </si>
-  <si>
-    <t>77 S. Hartford Ave. South Portland</t>
-  </si>
-  <si>
-    <t>Association</t>
-  </si>
-  <si>
-    <t>111140 - Wheat Farming</t>
-  </si>
-  <si>
-    <t>(456) 489 - 7879</t>
-  </si>
-  <si>
-    <t>thomas@mailinator.com</t>
-  </si>
-  <si>
-    <t>Search</t>
-  </si>
-  <si>
-    <t>Actions</t>
-  </si>
-  <si>
-    <t>Back</t>
-  </si>
-  <si>
-    <t>click</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -347,7 +357,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -396,12 +406,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -439,6 +460,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -469,7 +493,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -1134,20 +1158,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1167,7 +1191,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>101</v>
       </c>
@@ -1187,7 +1211,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>102</v>
       </c>
@@ -1207,7 +1231,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>103</v>
       </c>
@@ -1227,7 +1251,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>104</v>
       </c>
@@ -1253,14 +1277,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
@@ -1269,7 +1293,7 @@
     <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1277,16 +1301,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="E1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>101</v>
       </c>
@@ -1294,13 +1318,13 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>85</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>102</v>
       </c>
@@ -1312,7 +1336,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>103</v>
       </c>
@@ -1324,7 +1348,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>103</v>
       </c>
@@ -1337,7 +1361,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>104</v>
       </c>
@@ -1356,36 +1380,37 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:X5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.28515625" customWidth="1"/>
-    <col min="7" max="7" width="28" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" customWidth="1"/>
-    <col min="11" max="11" width="38.28515625" customWidth="1"/>
-    <col min="12" max="12" width="48.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="16.42578125" customWidth="1"/>
-    <col min="16" max="16" width="25.140625" customWidth="1"/>
-    <col min="17" max="19" width="21.28515625" customWidth="1"/>
-    <col min="20" max="20" width="26" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="15.5703125" customWidth="1"/>
-    <col min="23" max="23" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.28515625" customWidth="1"/>
+    <col min="8" max="8" width="28" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1"/>
+    <col min="12" max="12" width="38.28515625" customWidth="1"/>
+    <col min="13" max="13" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="16.42578125" customWidth="1"/>
+    <col min="17" max="17" width="25.140625" customWidth="1"/>
+    <col min="18" max="20" width="21.28515625" customWidth="1"/>
+    <col min="21" max="21" width="26" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="15.5703125" customWidth="1"/>
+    <col min="24" max="24" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1393,73 +1418,76 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="O1" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="P1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="S1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="W1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="X1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="U1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="V1" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="W1" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24">
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>101</v>
       </c>
@@ -1467,56 +1495,54 @@
         <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5">
+        <v>53704</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="5">
-        <v>53704</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="M2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5" t="s">
+      <c r="N2" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="5" t="s">
+      <c r="O2" s="7"/>
+      <c r="P2" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="Q2" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="R2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="S2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="T2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="N2" s="7"/>
-      <c r="O2" s="8" t="s">
+      <c r="U2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="P2" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="R2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="S2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="T2" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="U2" s="5" t="s">
-        <v>8</v>
-      </c>
       <c r="V2" s="5" t="s">
         <v>8</v>
       </c>
@@ -1526,8 +1552,11 @@
       <c r="X2" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:24">
+      <c r="Y2" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>102</v>
       </c>
@@ -1535,58 +1564,56 @@
         <v>3</v>
       </c>
       <c r="C3" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="J3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="M3" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="10" t="s">
+      <c r="N3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" s="7"/>
+      <c r="P3" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="Q3" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="K3" s="5" t="s">
+      <c r="R3" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="S3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="U3" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="M3" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="N3" s="7"/>
-      <c r="O3" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="R3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="S3" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="T3" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="U3" s="5" t="s">
-        <v>8</v>
-      </c>
       <c r="V3" s="5" t="s">
         <v>8</v>
       </c>
@@ -1596,8 +1623,11 @@
       <c r="X3" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:24">
+      <c r="Y3" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>103</v>
       </c>
@@ -1605,57 +1635,55 @@
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5">
+        <v>84101</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="M4" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="5">
-        <v>84101</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="N4" s="5"/>
+      <c r="O4" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="P4" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5" t="s">
+      <c r="Q4" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="R4" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="P4" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q4" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="R4" s="5" t="s">
-        <v>8</v>
-      </c>
       <c r="S4" s="5" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="T4" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="U4" s="5" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="V4" s="5" t="s">
         <v>8</v>
@@ -1666,8 +1694,11 @@
       <c r="X4" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:24">
+      <c r="Y4" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>103</v>
       </c>
@@ -1675,57 +1706,55 @@
         <v>6</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5">
+        <v>84010</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q5" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="D5" s="5">
-        <v>84010</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="M5" s="5" t="s">
+      <c r="R5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="S5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="T5" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="P5" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q5" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="R5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="S5" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="T5" s="5" t="s">
-        <v>47</v>
-      </c>
       <c r="U5" s="5" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="V5" s="5" t="s">
         <v>8</v>
@@ -1734,19 +1763,51 @@
         <v>8</v>
       </c>
       <c r="X5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y5" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A6" s="15">
+        <v>104</v>
+      </c>
+      <c r="B6" s="15">
+        <v>5</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="R6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="S6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="T6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="U6" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="V6" s="5" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="D3:E3 G3 K3 O2:P3" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="E3:F3 H3 L3 P2:Q3"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" display="random123@gmail.com" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="E3" r:id="rId2" display="random123@gmail.com" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="P4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="P5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="P2" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="E3" r:id="rId1" display="random123@gmail.com"/>
+    <hyperlink ref="F3" r:id="rId2" display="random123@gmail.com"/>
+    <hyperlink ref="Q4" r:id="rId3"/>
+    <hyperlink ref="Q5" r:id="rId4"/>
+    <hyperlink ref="Q2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
@@ -1754,21 +1815,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.28515625" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1776,16 +1837,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>104</v>
       </c>
@@ -1793,7 +1854,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -1808,17 +1869,65 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>104</v>
+      </c>
+      <c r="B2" s="1">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1826,10 +1935,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>101</v>
       </c>
@@ -1837,10 +1946,10 @@
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>102</v>
       </c>
@@ -1848,10 +1957,10 @@
         <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>103</v>
       </c>
@@ -1859,7 +1968,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update for the Assertions Task 40
</commit_message>
<xml_diff>
--- a/resources/test_data/VM_TestData_Sample1.xlsx
+++ b/resources/test_data/VM_TestData_Sample1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\praneethm\git\VMSeleniumFramework\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="6060" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="2055" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LogInPage" sheetId="22" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <definedName name="State">[1]Selectlists!$C$2:$C$52</definedName>
     <definedName name="waivsub">[1]Selectlists!$J$2:$J$6</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="115">
   <si>
     <t>TestCaseNumber</t>
   </si>
@@ -304,6 +304,97 @@
   </si>
   <si>
     <t>AreEqual&gt;Thomas Charles</t>
+  </si>
+  <si>
+    <t>VerifyCustomerAccountID</t>
+  </si>
+  <si>
+    <t>AreEqual&gt;ACC0000212</t>
+  </si>
+  <si>
+    <t>VerifyCustomerSince</t>
+  </si>
+  <si>
+    <t>VerifyLegalEntityType</t>
+  </si>
+  <si>
+    <t>VerifySSN</t>
+  </si>
+  <si>
+    <t>VerifyPhone</t>
+  </si>
+  <si>
+    <t>VerifyEmailID</t>
+  </si>
+  <si>
+    <t>VerifyPhysicalAddress</t>
+  </si>
+  <si>
+    <t>VerifyMailingAddress</t>
+  </si>
+  <si>
+    <t>AreEqual&gt;09/04/2019</t>
+  </si>
+  <si>
+    <t>AreEqual&gt;Individual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AreEqual&gt;65-4987879
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AreEqual&gt;(654) 987 - 9798
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AreEqual&gt;jack@gmail.com
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AreEqual&gt;123 New Street, Madison, WI- 53704
+</t>
+  </si>
+  <si>
+    <t>VerifyCustomerAccountName1</t>
+  </si>
+  <si>
+    <t>IsEnable&gt;true</t>
+  </si>
+  <si>
+    <t>CheckMultipleValues&gt;Select||Madison||Maple Bluff</t>
+  </si>
+  <si>
+    <t>Verifycity1</t>
+  </si>
+  <si>
+    <t>Verifystate1</t>
+  </si>
+  <si>
+    <t>IsEnable&gt;false</t>
+  </si>
+  <si>
+    <t>VerifyMailingAddress1</t>
+  </si>
+  <si>
+    <t>IsSelected&gt;true</t>
+  </si>
+  <si>
+    <t>VerifyLegalEntityType1</t>
+  </si>
+  <si>
+    <t>IsVisible&gt;true</t>
+  </si>
+  <si>
+    <t>VerifySSN1</t>
+  </si>
+  <si>
+    <t>VerifyFEIN1</t>
+  </si>
+  <si>
+    <t>VerifyColourofCS</t>
+  </si>
+  <si>
+    <t>CheckColor&gt;#48c157</t>
   </si>
 </sst>
 </file>
@@ -357,7 +448,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -417,12 +508,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -461,6 +561,18 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1159,10 +1271,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C5" sqref="C5:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1271,6 +1383,26 @@
         <v>8</v>
       </c>
     </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
+        <v>105</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1278,10 +1410,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1374,6 +1506,17 @@
         <v>8</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>105</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1381,36 +1524,46 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y6"/>
+  <dimension ref="A1:AG7"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.28515625" customWidth="1"/>
-    <col min="8" max="8" width="28" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" customWidth="1"/>
-    <col min="12" max="12" width="38.28515625" customWidth="1"/>
-    <col min="13" max="13" width="48.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="16.42578125" customWidth="1"/>
-    <col min="17" max="17" width="25.140625" customWidth="1"/>
-    <col min="18" max="20" width="21.28515625" customWidth="1"/>
-    <col min="21" max="21" width="26" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="15.5703125" customWidth="1"/>
-    <col min="24" max="24" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="49.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.28515625" customWidth="1"/>
+    <col min="11" max="11" width="28" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.140625" customWidth="1"/>
+    <col min="17" max="17" width="38.28515625" customWidth="1"/>
+    <col min="18" max="19" width="19.7109375" customWidth="1"/>
+    <col min="20" max="21" width="16.42578125" customWidth="1"/>
+    <col min="22" max="22" width="6.42578125" customWidth="1"/>
+    <col min="23" max="23" width="16.42578125" customWidth="1"/>
+    <col min="24" max="24" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="21.28515625" customWidth="1"/>
+    <col min="28" max="29" width="22.85546875" customWidth="1"/>
+    <col min="30" max="31" width="15.5703125" customWidth="1"/>
+    <col min="32" max="32" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1418,396 +1571,546 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="I1" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="M1" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="O1" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="P1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="S1" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="T1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="U1" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="V1" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="Z1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="AC1" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="AE1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="AF1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="AG1" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>101</v>
       </c>
       <c r="B2" s="5">
         <v>3</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5">
+      <c r="E2" s="5"/>
+      <c r="F2" s="5">
         <v>53704</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>33</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="Q2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="R2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="S2" s="7"/>
+      <c r="T2" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="O2" s="7"/>
-      <c r="P2" s="8" t="s">
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="X2" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="Y2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="S2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="T2" s="5" t="s">
+      <c r="Z2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="AB2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="V2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="W2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="X2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y2" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG2" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>102</v>
       </c>
       <c r="B3" s="5">
         <v>3</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="5"/>
+      <c r="F3" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="G3" s="11"/>
+      <c r="H3" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="10" t="s">
+      <c r="I3" s="11"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="J3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="K3" s="5" t="s">
+      <c r="M3" s="5"/>
+      <c r="N3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="Q3" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="R3" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="S3" s="7"/>
+      <c r="T3" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="O3" s="7"/>
-      <c r="P3" s="8" t="s">
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Q3" s="8" t="s">
+      <c r="X3" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="R3" s="5" t="s">
+      <c r="Y3" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="S3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="T3" s="5" t="s">
+      <c r="Z3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="U3" s="5" t="s">
+      <c r="AB3" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="V3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="W3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="X3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y3" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AC3" s="5"/>
+      <c r="AD3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG3" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>103</v>
       </c>
       <c r="B4" s="5">
         <v>3</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5">
+      <c r="E4" s="5"/>
+      <c r="F4" s="5">
         <v>84101</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>76</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="J4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="K4" s="5" t="s">
+      <c r="M4" s="5"/>
+      <c r="N4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="Q4" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="R4" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5" t="s">
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="P4" s="5" t="s">
+      <c r="W4" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="Q4" s="12" t="s">
+      <c r="X4" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="R4" s="5" t="s">
+      <c r="Y4" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="S4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="T4" s="5" t="s">
+      <c r="Z4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA4" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="U4" s="5" t="s">
+      <c r="AB4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="V4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="W4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="X4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y4" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AC4" s="5"/>
+      <c r="AD4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG4" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>103</v>
       </c>
       <c r="B5" s="5">
         <v>6</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="5"/>
+      <c r="D5" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5">
+      <c r="E5" s="5"/>
+      <c r="F5" s="5">
         <v>84010</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="L5" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="J5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>68</v>
-      </c>
+      <c r="M5" s="5"/>
       <c r="N5" s="5" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="O5" s="5"/>
       <c r="P5" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="Q5" s="12" t="s">
+      <c r="X5" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="R5" s="5" t="s">
+      <c r="Y5" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="S5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="T5" s="5" t="s">
+      <c r="Z5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA5" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="U5" s="5" t="s">
+      <c r="AB5" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="V5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="W5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="X5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y5" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG5" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>104</v>
       </c>
       <c r="B6" s="15">
         <v>5</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="15"/>
+      <c r="D6" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="R6" s="5" t="s">
+      <c r="E6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y6" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="S6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="T6" s="5" t="s">
+      <c r="Z6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA6" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="U6" s="5" t="s">
+      <c r="AB6" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="V6" s="5" t="s">
+      <c r="AC6" s="5"/>
+      <c r="AD6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE6" s="5"/>
+      <c r="AF6" s="5"/>
+      <c r="AG6" s="5"/>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" s="15">
+        <v>105</v>
+      </c>
+      <c r="B7" s="15">
+        <v>3</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="17">
+        <v>53704</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="H7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="K7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" t="s">
+        <v>108</v>
+      </c>
+      <c r="N7" t="s">
+        <v>8</v>
+      </c>
+      <c r="O7" t="s">
+        <v>110</v>
+      </c>
+      <c r="P7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>36</v>
+      </c>
+      <c r="R7" t="s">
+        <v>37</v>
+      </c>
+      <c r="S7" t="s">
+        <v>102</v>
+      </c>
+      <c r="T7" t="s">
+        <v>38</v>
+      </c>
+      <c r="U7" t="s">
+        <v>106</v>
+      </c>
+      <c r="W7" t="s">
+        <v>39</v>
+      </c>
+      <c r="X7" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA7" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB7" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC7" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="AD7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG7" s="5" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="E3:F3 H3 L3 P2:Q3"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="F3:I3 K3 Q3 W2:X3"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" display="random123@gmail.com"/>
-    <hyperlink ref="F3" r:id="rId2" display="random123@gmail.com"/>
-    <hyperlink ref="Q4" r:id="rId3"/>
-    <hyperlink ref="Q5" r:id="rId4"/>
-    <hyperlink ref="Q2" r:id="rId5"/>
+    <hyperlink ref="F3" r:id="rId1" display="random123@gmail.com"/>
+    <hyperlink ref="H3" r:id="rId2" display="random123@gmail.com"/>
+    <hyperlink ref="X4" r:id="rId3"/>
+    <hyperlink ref="X5" r:id="rId4"/>
+    <hyperlink ref="X2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
@@ -1870,20 +2173,28 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1891,23 +2202,71 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K1" t="s">
         <v>80</v>
       </c>
-      <c r="D1" t="s">
+      <c r="L1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>104</v>
       </c>
       <c r="B2" s="1">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
+      <c r="C2" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="D2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="K2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Recommitting Task 27 changes due to an out of date push
Changes made to PageProcess.java and Assertions.java
</commit_message>
<xml_diff>
--- a/resources/test_data/VM_TestData_Sample1.xlsx
+++ b/resources/test_data/VM_TestData_Sample1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\praneethm\git\VMSeleniumFramework\resources\test_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_2b36\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="11" documentId="11_30BFB98678587BF24C5D6650767FB1D240D0B996" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E2DB8347-7979-4BA9-9B73-57722ABD40B8}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="2055" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="2055" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LogInPage" sheetId="22" r:id="rId1"/>
@@ -30,7 +31,7 @@
     <definedName name="State">[1]Selectlists!$C$2:$C$52</definedName>
     <definedName name="waivsub">[1]Selectlists!$J$2:$J$6</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="113">
   <si>
     <t>TestCaseNumber</t>
   </si>
@@ -78,18 +79,39 @@
     <t>P@ssw0rd</t>
   </si>
   <si>
+    <t>VerifyUser</t>
+  </si>
+  <si>
     <t>NewSubmission</t>
   </si>
   <si>
+    <t>ServicePolicy</t>
+  </si>
+  <si>
+    <t>AreEqual&gt;Thomas Charles</t>
+  </si>
+  <si>
+    <t>VerifyCustomerAccountName1</t>
+  </si>
+  <si>
     <t>CustomerAccountName</t>
   </si>
   <si>
+    <t>SelectAndProceed1</t>
+  </si>
+  <si>
     <t>ZipCode</t>
   </si>
   <si>
+    <t>VerifyCity</t>
+  </si>
+  <si>
     <t>City</t>
   </si>
   <si>
+    <t>VerifyState</t>
+  </si>
+  <si>
     <t>State</t>
   </si>
   <si>
@@ -99,6 +121,9 @@
     <t>Apt</t>
   </si>
   <si>
+    <t>VerifyMailingAddress</t>
+  </si>
+  <si>
     <t>MailingAddress</t>
   </si>
   <si>
@@ -111,9 +136,15 @@
     <t>SubIndustryType</t>
   </si>
   <si>
+    <t>VerifySSN1</t>
+  </si>
+  <si>
     <t>SSN</t>
   </si>
   <si>
+    <t>FEIN</t>
+  </si>
+  <si>
     <t>BusinessPhone</t>
   </si>
   <si>
@@ -132,6 +163,9 @@
     <t>AgentName</t>
   </si>
   <si>
+    <t>VerifyColourofCS</t>
+  </si>
+  <si>
     <t>CreateSubmission</t>
   </si>
   <si>
@@ -216,18 +250,27 @@
     <t>JohnKristin</t>
   </si>
   <si>
+    <t>Salt Lake City</t>
+  </si>
+  <si>
     <t>Alaska</t>
   </si>
   <si>
     <t>Ameklari</t>
   </si>
   <si>
+    <t>Foreign Limited Liability Company</t>
+  </si>
+  <si>
     <t>32 - Manufacturing-Wood, paper, printing, chemical, plastics, non-metallic minerals</t>
   </si>
   <si>
     <t>321219 - Reconstituted Wood Product Manufacturing</t>
   </si>
   <si>
+    <t>21-3113154</t>
+  </si>
+  <si>
     <t>(565) 865 - 6856</t>
   </si>
   <si>
@@ -261,10 +304,25 @@
     <t>thomas@mailinator.com</t>
   </si>
   <si>
-    <t>Back</t>
-  </si>
-  <si>
-    <t>click</t>
+    <t>Charles Submission</t>
+  </si>
+  <si>
+    <t>IsEnable&gt;true</t>
+  </si>
+  <si>
+    <t>CheckMultipleValues&gt;Select||Madison||Maple Bluff</t>
+  </si>
+  <si>
+    <t>IsEnable&gt;false</t>
+  </si>
+  <si>
+    <t>IsSelected&gt;true</t>
+  </si>
+  <si>
+    <t>IsVisible&gt;true</t>
+  </si>
+  <si>
+    <t>CheckColor&gt;#48c157</t>
   </si>
   <si>
     <t>Search</t>
@@ -273,19 +331,25 @@
     <t>Actions</t>
   </si>
   <si>
-    <t>ServicePolicy</t>
-  </si>
-  <si>
-    <t>Salt Lake City</t>
-  </si>
-  <si>
-    <t>Foreign Limited Liability Company</t>
-  </si>
-  <si>
-    <t>FEIN</t>
-  </si>
-  <si>
-    <t>21-3113154</t>
+    <t>VerifyCustomerAccountID</t>
+  </si>
+  <si>
+    <t>VerifyCustomerSince</t>
+  </si>
+  <si>
+    <t>VerifyLegalEntityType</t>
+  </si>
+  <si>
+    <t>VerifySSN</t>
+  </si>
+  <si>
+    <t>VerifyPhone</t>
+  </si>
+  <si>
+    <t>VerifyEmailID</t>
+  </si>
+  <si>
+    <t>VerifyPhysicalAddress</t>
   </si>
   <si>
     <t>Submissions</t>
@@ -294,43 +358,7 @@
     <t>AddNewSubmission</t>
   </si>
   <si>
-    <t>Charles Submission</t>
-  </si>
-  <si>
-    <t>SelectAndProceed1</t>
-  </si>
-  <si>
-    <t>VerifyUser</t>
-  </si>
-  <si>
-    <t>AreEqual&gt;Thomas Charles</t>
-  </si>
-  <si>
-    <t>VerifyCustomerAccountID</t>
-  </si>
-  <si>
     <t>AreEqual&gt;ACC0000212</t>
-  </si>
-  <si>
-    <t>VerifyCustomerSince</t>
-  </si>
-  <si>
-    <t>VerifyLegalEntityType</t>
-  </si>
-  <si>
-    <t>VerifySSN</t>
-  </si>
-  <si>
-    <t>VerifyPhone</t>
-  </si>
-  <si>
-    <t>VerifyEmailID</t>
-  </si>
-  <si>
-    <t>VerifyPhysicalAddress</t>
-  </si>
-  <si>
-    <t>VerifyMailingAddress</t>
   </si>
   <si>
     <t>AreEqual&gt;09/04/2019</t>
@@ -355,52 +383,19 @@
 </t>
   </si>
   <si>
-    <t>VerifyCustomerAccountName1</t>
-  </si>
-  <si>
-    <t>IsEnable&gt;true</t>
-  </si>
-  <si>
-    <t>CheckMultipleValues&gt;Select||Madison||Maple Bluff</t>
-  </si>
-  <si>
-    <t>Verifycity1</t>
-  </si>
-  <si>
-    <t>Verifystate1</t>
-  </si>
-  <si>
-    <t>IsEnable&gt;false</t>
-  </si>
-  <si>
-    <t>VerifyMailingAddress1</t>
-  </si>
-  <si>
-    <t>IsSelected&gt;true</t>
-  </si>
-  <si>
-    <t>VerifyLegalEntityType1</t>
-  </si>
-  <si>
-    <t>IsVisible&gt;true</t>
-  </si>
-  <si>
-    <t>VerifySSN1</t>
-  </si>
-  <si>
-    <t>VerifyFEIN1</t>
-  </si>
-  <si>
-    <t>VerifyColourofCS</t>
-  </si>
-  <si>
-    <t>CheckColor&gt;#48c157</t>
+    <t>Back</t>
+  </si>
+  <si>
+    <t>click</t>
+  </si>
+  <si>
+    <t>VerifyFEIN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -605,7 +600,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -1270,7 +1265,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1409,10 +1404,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
@@ -1433,13 +1428,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>84</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>75</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1450,7 +1445,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -1523,11 +1518,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AG7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1571,97 +1566,97 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>101</v>
+        <v>14</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>83</v>
+        <v>16</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>104</v>
+        <v>18</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>105</v>
+        <v>20</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>107</v>
+        <v>24</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>111</v>
+        <v>29</v>
       </c>
       <c r="T1" s="5" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="U1" s="19" t="s">
         <v>112</v>
       </c>
       <c r="V1" s="14" t="s">
-        <v>78</v>
+        <v>31</v>
       </c>
       <c r="W1" s="5" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="X1" s="5" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="Y1" s="5" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="Z1" s="5" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="AA1" s="5" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="AB1" s="5" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="AC1" s="5" t="s">
-        <v>113</v>
+        <v>38</v>
       </c>
       <c r="AD1" s="5" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="AE1" s="6" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="AF1" s="6" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="AG1" s="5" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
@@ -1673,7 +1668,7 @@
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5">
@@ -1681,12 +1676,12 @@
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
@@ -1695,37 +1690,37 @@
       </c>
       <c r="O2" s="5"/>
       <c r="P2" s="5" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="S2" s="7"/>
       <c r="T2" s="7" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="U2" s="7"/>
       <c r="V2" s="7"/>
       <c r="W2" s="8" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="X2" s="9" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="Y2" s="5" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="Z2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="AA2" s="5" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="AB2" s="5" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="AC2" s="5"/>
       <c r="AD2" s="5" t="s">
@@ -1750,23 +1745,23 @@
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="10" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="11" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="11" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="I3" s="11"/>
       <c r="J3" s="5"/>
       <c r="K3" s="10" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5" t="s">
@@ -1774,37 +1769,37 @@
       </c>
       <c r="O3" s="5"/>
       <c r="P3" s="5" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="R3" s="7" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="S3" s="7"/>
       <c r="T3" s="7" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="U3" s="7"/>
       <c r="V3" s="7"/>
       <c r="W3" s="8" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="X3" s="8" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="Y3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA3" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="Z3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA3" s="5" t="s">
-        <v>42</v>
-      </c>
       <c r="AB3" s="5" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="AC3" s="5"/>
       <c r="AD3" s="5" t="s">
@@ -1829,7 +1824,7 @@
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5">
@@ -1837,15 +1832,15 @@
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="M4" s="5"/>
       <c r="N4" s="5" t="s">
@@ -1853,37 +1848,37 @@
       </c>
       <c r="O4" s="5"/>
       <c r="P4" s="5" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="S4" s="5"/>
       <c r="T4" s="5"/>
       <c r="U4" s="5"/>
       <c r="V4" s="5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="W4" s="5" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="X4" s="12" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="Y4" s="5" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="Z4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="AA4" s="5" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="AB4" s="5" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="AC4" s="5"/>
       <c r="AD4" s="5" t="s">
@@ -1908,7 +1903,7 @@
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5">
@@ -1916,15 +1911,15 @@
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="5" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="M5" s="5"/>
       <c r="N5" s="5" t="s">
@@ -1932,37 +1927,37 @@
       </c>
       <c r="O5" s="5"/>
       <c r="P5" s="5" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="R5" s="5" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="S5" s="5"/>
       <c r="T5" s="5" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="U5" s="5"/>
       <c r="V5" s="5"/>
       <c r="W5" s="5" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="X5" s="12" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="Y5" s="5" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="Z5" s="5" t="s">
         <v>8</v>
       </c>
       <c r="AA5" s="5" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="AB5" s="5" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="AC5" s="5"/>
       <c r="AD5" s="5" t="s">
@@ -1987,22 +1982,22 @@
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="15" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>8</v>
       </c>
       <c r="Y6" s="5" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="Z6" s="5" t="s">
         <v>8</v>
       </c>
       <c r="AA6" s="5" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="AB6" s="5" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="AC6" s="5"/>
       <c r="AD6" s="5" t="s">
@@ -2020,73 +2015,73 @@
         <v>3</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="F7" s="17">
         <v>53704</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="H7" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="I7" s="18" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="K7" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="M7" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="N7" t="s">
         <v>8</v>
       </c>
       <c r="O7" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="P7" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="Q7" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="R7" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="S7" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="T7" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="U7" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="W7" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="X7" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="Y7" s="5" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="Z7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="AA7" s="5" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="AB7" s="5" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="AC7" s="5" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="AD7" s="5" t="s">
         <v>8</v>
@@ -2103,14 +2098,14 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="F3:I3 K3 Q3 W2:X3"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="F3:I3 K3 Q3 W2:X3" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" display="random123@gmail.com"/>
-    <hyperlink ref="H3" r:id="rId2" display="random123@gmail.com"/>
-    <hyperlink ref="X4" r:id="rId3"/>
-    <hyperlink ref="X5" r:id="rId4"/>
-    <hyperlink ref="X2" r:id="rId5"/>
+    <hyperlink ref="F3" r:id="rId1" display="random123@gmail.com" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="H3" r:id="rId2" display="random123@gmail.com" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="X4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="X5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="X2" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
@@ -2118,7 +2113,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2140,13 +2135,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="E1" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2157,7 +2152,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -2172,7 +2167,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -2202,34 +2197,34 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="D1" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="E1" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="F1" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="G1" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="H1" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="I1" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="J1" t="s">
-        <v>94</v>
+        <v>24</v>
       </c>
       <c r="K1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="L1" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2240,28 +2235,28 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="D2" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="E2" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="J2" s="16" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="K2" t="s">
         <v>8</v>
@@ -2276,7 +2271,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2294,7 +2289,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>71</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2305,7 +2300,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>72</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2316,7 +2311,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>72</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2327,7 +2322,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>72</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor fixes to PageProcess and NewSubmissionPage
</commit_message>
<xml_diff>
--- a/resources/test_data/VM_TestData_Sample1.xlsx
+++ b/resources/test_data/VM_TestData_Sample1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_2b36\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="11_30BFB98678587BF24C5D6650767FB1D240D0B996" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E2DB8347-7979-4BA9-9B73-57722ABD40B8}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_30BFB98678587BF24C5D6650767FB1D240D0B996" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{511D9AB0-B33E-47E7-9C43-B584C64931EE}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="2055" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="2055" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LogInPage" sheetId="22" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <definedName name="State">[1]Selectlists!$C$2:$C$52</definedName>
     <definedName name="waivsub">[1]Selectlists!$J$2:$J$6</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="115">
   <si>
     <t>TestCaseNumber</t>
   </si>
@@ -103,13 +103,13 @@
     <t>ZipCode</t>
   </si>
   <si>
-    <t>VerifyCity</t>
+    <t>VerifyCity1</t>
   </si>
   <si>
     <t>City</t>
   </si>
   <si>
-    <t>VerifyState</t>
+    <t>VerifyState1</t>
   </si>
   <si>
     <t>State</t>
@@ -121,235 +121,244 @@
     <t>Apt</t>
   </si>
   <si>
+    <t>VerifyMailingAddress1</t>
+  </si>
+  <si>
+    <t>MailingAddress</t>
+  </si>
+  <si>
+    <t>VerifyLegalEntityType1</t>
+  </si>
+  <si>
+    <t>LegalEntityType</t>
+  </si>
+  <si>
+    <t>IndustryType</t>
+  </si>
+  <si>
+    <t>SubIndustryType</t>
+  </si>
+  <si>
+    <t>VerifySSN1</t>
+  </si>
+  <si>
+    <t>SSN</t>
+  </si>
+  <si>
+    <t>VerifyFEIN1</t>
+  </si>
+  <si>
+    <t>FEIN</t>
+  </si>
+  <si>
+    <t>BusinessPhone</t>
+  </si>
+  <si>
+    <t>EmailId</t>
+  </si>
+  <si>
+    <t>SelectProduct</t>
+  </si>
+  <si>
+    <t>CommercialAuto</t>
+  </si>
+  <si>
+    <t>AgencyName</t>
+  </si>
+  <si>
+    <t>AgentName</t>
+  </si>
+  <si>
+    <t>VerifyColourofCS</t>
+  </si>
+  <si>
+    <t>CreateSubmission</t>
+  </si>
+  <si>
+    <t>SelectUser</t>
+  </si>
+  <si>
+    <t>SelectAndProceed</t>
+  </si>
+  <si>
+    <t>CreateSubmission1</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>Madison</t>
+  </si>
+  <si>
+    <t>123 New Street</t>
+  </si>
+  <si>
+    <t>Individual</t>
+  </si>
+  <si>
+    <t>11 - Agriculture, Forestry, Fishing and Hunting</t>
+  </si>
+  <si>
+    <t>111160 - Rice Farming</t>
+  </si>
+  <si>
+    <t>654-98-7987</t>
+  </si>
+  <si>
+    <t>(654) 987 - 9798</t>
+  </si>
+  <si>
+    <t>jack123@gmail.com</t>
+  </si>
+  <si>
+    <t>Commercial Auto</t>
+  </si>
+  <si>
+    <t>pix3473-Pixel Groups</t>
+  </si>
+  <si>
+    <t>edw982347-Edward Bella</t>
+  </si>
+  <si>
+    <t>John miller</t>
+  </si>
+  <si>
+    <t>53004</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>jhgfugfgb</t>
+  </si>
+  <si>
+    <t>Zinkare zoth</t>
+  </si>
+  <si>
+    <t>42 -Wholesale Trade</t>
+  </si>
+  <si>
+    <t>423210 - Furniture Merchant Wholesalers</t>
+  </si>
+  <si>
+    <t>(121)212-1212</t>
+  </si>
+  <si>
+    <t>john@gmail.com</t>
+  </si>
+  <si>
+    <t>Commercial Property</t>
+  </si>
+  <si>
+    <t xml:space="preserve">edw982347-Edward Bella		</t>
+  </si>
+  <si>
+    <t>JohnKristin</t>
+  </si>
+  <si>
+    <t>Salt Lake City</t>
+  </si>
+  <si>
+    <t>Alaska</t>
+  </si>
+  <si>
+    <t>Ameklari</t>
+  </si>
+  <si>
+    <t>Foreign Limited Liability Company</t>
+  </si>
+  <si>
+    <t>32 - Manufacturing-Wood, paper, printing, chemical, plastics, non-metallic minerals</t>
+  </si>
+  <si>
+    <t>321219 - Reconstituted Wood Product Manufacturing</t>
+  </si>
+  <si>
+    <t>21-3113154</t>
+  </si>
+  <si>
+    <t>(565) 865 - 6856</t>
+  </si>
+  <si>
+    <t>ashdkjhskjdh@fshgdf.com</t>
+  </si>
+  <si>
+    <t>General Liability</t>
+  </si>
+  <si>
+    <t>Thomas Submission</t>
+  </si>
+  <si>
+    <t>Bountiful</t>
+  </si>
+  <si>
+    <t>86 East White Street Chicopee</t>
+  </si>
+  <si>
+    <t>77 S. Hartford Ave. South Portland</t>
+  </si>
+  <si>
+    <t>Association</t>
+  </si>
+  <si>
+    <t>111140 - Wheat Farming</t>
+  </si>
+  <si>
+    <t>(456) 489 - 7879</t>
+  </si>
+  <si>
+    <t>thomas@mailinator.com</t>
+  </si>
+  <si>
+    <t>Charles Submission</t>
+  </si>
+  <si>
+    <t>IsEnable&gt;true</t>
+  </si>
+  <si>
+    <t>CheckMultipleValues&gt;Select||Madison||Maple Bluff</t>
+  </si>
+  <si>
+    <t>IsEnable&gt;false</t>
+  </si>
+  <si>
+    <t>IsSelected&gt;true</t>
+  </si>
+  <si>
+    <t>IsVisible&gt;true</t>
+  </si>
+  <si>
+    <t>CheckColor&gt;#48c157</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>Actions</t>
+  </si>
+  <si>
+    <t>VerifyCustomerAccountID</t>
+  </si>
+  <si>
+    <t>VerifyCustomerSince</t>
+  </si>
+  <si>
+    <t>VerifyLegalEntityType</t>
+  </si>
+  <si>
+    <t>VerifySSN</t>
+  </si>
+  <si>
+    <t>VerifyPhone</t>
+  </si>
+  <si>
+    <t>VerifyEmailID</t>
+  </si>
+  <si>
+    <t>VerifyPhysicalAddress</t>
+  </si>
+  <si>
     <t>VerifyMailingAddress</t>
-  </si>
-  <si>
-    <t>MailingAddress</t>
-  </si>
-  <si>
-    <t>LegalEntityType</t>
-  </si>
-  <si>
-    <t>IndustryType</t>
-  </si>
-  <si>
-    <t>SubIndustryType</t>
-  </si>
-  <si>
-    <t>VerifySSN1</t>
-  </si>
-  <si>
-    <t>SSN</t>
-  </si>
-  <si>
-    <t>FEIN</t>
-  </si>
-  <si>
-    <t>BusinessPhone</t>
-  </si>
-  <si>
-    <t>EmailId</t>
-  </si>
-  <si>
-    <t>SelectProduct</t>
-  </si>
-  <si>
-    <t>CommercialAuto</t>
-  </si>
-  <si>
-    <t>AgencyName</t>
-  </si>
-  <si>
-    <t>AgentName</t>
-  </si>
-  <si>
-    <t>VerifyColourofCS</t>
-  </si>
-  <si>
-    <t>CreateSubmission</t>
-  </si>
-  <si>
-    <t>SelectUser</t>
-  </si>
-  <si>
-    <t>SelectAndProceed</t>
-  </si>
-  <si>
-    <t>CreateSubmission1</t>
-  </si>
-  <si>
-    <t>Jack</t>
-  </si>
-  <si>
-    <t>Madison</t>
-  </si>
-  <si>
-    <t>123 New Street</t>
-  </si>
-  <si>
-    <t>Individual</t>
-  </si>
-  <si>
-    <t>11 - Agriculture, Forestry, Fishing and Hunting</t>
-  </si>
-  <si>
-    <t>111160 - Rice Farming</t>
-  </si>
-  <si>
-    <t>654-98-7987</t>
-  </si>
-  <si>
-    <t>(654) 987 - 9798</t>
-  </si>
-  <si>
-    <t>jack123@gmail.com</t>
-  </si>
-  <si>
-    <t>Commercial Auto</t>
-  </si>
-  <si>
-    <t>pix3473-Pixel Groups</t>
-  </si>
-  <si>
-    <t>edw982347-Edward Bella</t>
-  </si>
-  <si>
-    <t>John miller</t>
-  </si>
-  <si>
-    <t>53004</t>
-  </si>
-  <si>
-    <t>Belgium</t>
-  </si>
-  <si>
-    <t>jhgfugfgb</t>
-  </si>
-  <si>
-    <t>Zinkare zoth</t>
-  </si>
-  <si>
-    <t>42 -Wholesale Trade</t>
-  </si>
-  <si>
-    <t>423210 - Furniture Merchant Wholesalers</t>
-  </si>
-  <si>
-    <t>(121)212-1212</t>
-  </si>
-  <si>
-    <t>john@gmail.com</t>
-  </si>
-  <si>
-    <t>Commercial Property</t>
-  </si>
-  <si>
-    <t xml:space="preserve">edw982347-Edward Bella		</t>
-  </si>
-  <si>
-    <t>JohnKristin</t>
-  </si>
-  <si>
-    <t>Salt Lake City</t>
-  </si>
-  <si>
-    <t>Alaska</t>
-  </si>
-  <si>
-    <t>Ameklari</t>
-  </si>
-  <si>
-    <t>Foreign Limited Liability Company</t>
-  </si>
-  <si>
-    <t>32 - Manufacturing-Wood, paper, printing, chemical, plastics, non-metallic minerals</t>
-  </si>
-  <si>
-    <t>321219 - Reconstituted Wood Product Manufacturing</t>
-  </si>
-  <si>
-    <t>21-3113154</t>
-  </si>
-  <si>
-    <t>(565) 865 - 6856</t>
-  </si>
-  <si>
-    <t>ashdkjhskjdh@fshgdf.com</t>
-  </si>
-  <si>
-    <t>General Liability</t>
-  </si>
-  <si>
-    <t>Thomas Submission</t>
-  </si>
-  <si>
-    <t>Bountiful</t>
-  </si>
-  <si>
-    <t>86 East White Street Chicopee</t>
-  </si>
-  <si>
-    <t>77 S. Hartford Ave. South Portland</t>
-  </si>
-  <si>
-    <t>Association</t>
-  </si>
-  <si>
-    <t>111140 - Wheat Farming</t>
-  </si>
-  <si>
-    <t>(456) 489 - 7879</t>
-  </si>
-  <si>
-    <t>thomas@mailinator.com</t>
-  </si>
-  <si>
-    <t>Charles Submission</t>
-  </si>
-  <si>
-    <t>IsEnable&gt;true</t>
-  </si>
-  <si>
-    <t>CheckMultipleValues&gt;Select||Madison||Maple Bluff</t>
-  </si>
-  <si>
-    <t>IsEnable&gt;false</t>
-  </si>
-  <si>
-    <t>IsSelected&gt;true</t>
-  </si>
-  <si>
-    <t>IsVisible&gt;true</t>
-  </si>
-  <si>
-    <t>CheckColor&gt;#48c157</t>
-  </si>
-  <si>
-    <t>Search</t>
-  </si>
-  <si>
-    <t>Actions</t>
-  </si>
-  <si>
-    <t>VerifyCustomerAccountID</t>
-  </si>
-  <si>
-    <t>VerifyCustomerSince</t>
-  </si>
-  <si>
-    <t>VerifyLegalEntityType</t>
-  </si>
-  <si>
-    <t>VerifySSN</t>
-  </si>
-  <si>
-    <t>VerifyPhone</t>
-  </si>
-  <si>
-    <t>VerifyEmailID</t>
-  </si>
-  <si>
-    <t>VerifyPhysicalAddress</t>
   </si>
   <si>
     <t>Submissions</t>
@@ -387,16 +396,13 @@
   </si>
   <si>
     <t>click</t>
-  </si>
-  <si>
-    <t>VerifyFEIN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1269,16 +1275,16 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:F6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1298,7 +1304,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="4">
         <v>101</v>
       </c>
@@ -1318,7 +1324,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="4">
         <v>102</v>
       </c>
@@ -1338,7 +1344,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="4">
         <v>103</v>
       </c>
@@ -1358,7 +1364,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="13">
         <v>104</v>
       </c>
@@ -1378,7 +1384,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="13">
         <v>105</v>
       </c>
@@ -1411,7 +1417,7 @@
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
@@ -1420,7 +1426,7 @@
     <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1437,7 +1443,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>101</v>
       </c>
@@ -1451,7 +1457,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>102</v>
       </c>
@@ -1463,7 +1469,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>103</v>
       </c>
@@ -1475,7 +1481,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>103</v>
       </c>
@@ -1488,7 +1494,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>104</v>
       </c>
@@ -1501,7 +1507,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>105</v>
       </c>
@@ -1521,11 +1527,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AG7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.140625" customWidth="1"/>
     <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
@@ -1558,7 +1564,7 @@
     <col min="33" max="33" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1602,64 +1608,64 @@
         <v>25</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>96</v>
+        <v>26</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="T1" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="U1" s="19" t="s">
-        <v>112</v>
+        <v>32</v>
       </c>
       <c r="V1" s="14" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="W1" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="X1" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="Y1" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Z1" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="AA1" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="AB1" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="AC1" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="AD1" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="AE1" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="AF1" s="6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="AG1" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33">
       <c r="A2" s="5">
         <v>101</v>
       </c>
@@ -1668,7 +1674,7 @@
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5">
@@ -1676,12 +1682,12 @@
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
@@ -1690,37 +1696,37 @@
       </c>
       <c r="O2" s="5"/>
       <c r="P2" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="S2" s="7"/>
       <c r="T2" s="7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="U2" s="7"/>
       <c r="V2" s="7"/>
       <c r="W2" s="8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="X2" s="9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="Y2" s="5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="Z2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="AA2" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AB2" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AC2" s="5"/>
       <c r="AD2" s="5" t="s">
@@ -1736,7 +1742,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33">
       <c r="A3" s="5">
         <v>102</v>
       </c>
@@ -1745,23 +1751,23 @@
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="11" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="11" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I3" s="11"/>
       <c r="J3" s="5"/>
       <c r="K3" s="10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5" t="s">
@@ -1769,37 +1775,37 @@
       </c>
       <c r="O3" s="5"/>
       <c r="P3" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="R3" s="7" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="S3" s="7"/>
       <c r="T3" s="7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="U3" s="7"/>
       <c r="V3" s="7"/>
       <c r="W3" s="8" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="X3" s="8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="Y3" s="5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="Z3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="AA3" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AB3" s="5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AC3" s="5"/>
       <c r="AD3" s="5" t="s">
@@ -1815,7 +1821,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33">
       <c r="A4" s="5">
         <v>103</v>
       </c>
@@ -1824,7 +1830,7 @@
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5">
@@ -1832,15 +1838,15 @@
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="M4" s="5"/>
       <c r="N4" s="5" t="s">
@@ -1848,37 +1854,37 @@
       </c>
       <c r="O4" s="5"/>
       <c r="P4" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="S4" s="5"/>
       <c r="T4" s="5"/>
       <c r="U4" s="5"/>
       <c r="V4" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="W4" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="X4" s="12" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="Y4" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="Z4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="AA4" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AB4" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AC4" s="5"/>
       <c r="AD4" s="5" t="s">
@@ -1894,7 +1900,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33">
       <c r="A5" s="5">
         <v>103</v>
       </c>
@@ -1903,7 +1909,7 @@
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5">
@@ -1911,15 +1917,15 @@
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="M5" s="5"/>
       <c r="N5" s="5" t="s">
@@ -1927,37 +1933,37 @@
       </c>
       <c r="O5" s="5"/>
       <c r="P5" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="R5" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="S5" s="5"/>
       <c r="T5" s="5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="U5" s="5"/>
       <c r="V5" s="5"/>
       <c r="W5" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="X5" s="12" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="Y5" s="5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="Z5" s="5" t="s">
         <v>8</v>
       </c>
       <c r="AA5" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AB5" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AC5" s="5"/>
       <c r="AD5" s="5" t="s">
@@ -1973,7 +1979,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33">
       <c r="A6" s="15">
         <v>104</v>
       </c>
@@ -1982,22 +1988,22 @@
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="15" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>8</v>
       </c>
       <c r="Y6" s="5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="Z6" s="5" t="s">
         <v>8</v>
       </c>
       <c r="AA6" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AB6" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AC6" s="5"/>
       <c r="AD6" s="5" t="s">
@@ -2007,7 +2013,7 @@
       <c r="AF6" s="5"/>
       <c r="AG6" s="5"/>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33">
       <c r="A7" s="15">
         <v>105</v>
       </c>
@@ -2015,73 +2021,73 @@
         <v>3</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F7" s="17">
         <v>53704</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="I7" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="K7" t="s">
+        <v>47</v>
+      </c>
+      <c r="M7" t="s">
+        <v>91</v>
+      </c>
+      <c r="N7" t="s">
+        <v>8</v>
+      </c>
+      <c r="O7" t="s">
+        <v>92</v>
+      </c>
+      <c r="P7" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>49</v>
+      </c>
+      <c r="R7" t="s">
+        <v>50</v>
+      </c>
+      <c r="S7" t="s">
         <v>88</v>
       </c>
-      <c r="K7" t="s">
-        <v>45</v>
-      </c>
-      <c r="M7" t="s">
-        <v>89</v>
-      </c>
-      <c r="N7" t="s">
-        <v>8</v>
-      </c>
-      <c r="O7" t="s">
+      <c r="T7" t="s">
+        <v>51</v>
+      </c>
+      <c r="U7" t="s">
         <v>90</v>
       </c>
-      <c r="P7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>47</v>
-      </c>
-      <c r="R7" t="s">
-        <v>48</v>
-      </c>
-      <c r="S7" t="s">
-        <v>86</v>
-      </c>
-      <c r="T7" t="s">
-        <v>49</v>
-      </c>
-      <c r="U7" t="s">
-        <v>88</v>
-      </c>
       <c r="W7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="X7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="Y7" s="5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="Z7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="AA7" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AB7" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AC7" s="5" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AD7" s="5" t="s">
         <v>8</v>
@@ -2120,14 +2126,14 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.28515625" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2138,13 +2144,13 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>104</v>
       </c>
@@ -2152,7 +2158,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -2174,7 +2180,7 @@
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
@@ -2189,7 +2195,7 @@
     <col min="12" max="12" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2197,37 +2203,37 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="F1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="G1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="H1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="I1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="J1" t="s">
-        <v>24</v>
+        <v>103</v>
       </c>
       <c r="K1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="L1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="14.25" customHeight="1">
       <c r="A2" s="1">
         <v>104</v>
       </c>
@@ -2235,28 +2241,28 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E2" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="J2" s="16" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="K2" t="s">
         <v>8</v>
@@ -2276,12 +2282,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2289,10 +2295,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="3">
         <v>101</v>
       </c>
@@ -2300,10 +2306,10 @@
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="3">
         <v>102</v>
       </c>
@@ -2311,10 +2317,10 @@
         <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="3">
         <v>103</v>
       </c>
@@ -2322,7 +2328,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Browser and BaseURL now set in config.properties
</commit_message>
<xml_diff>
--- a/resources/test_data/VM_TestData_Sample1.xlsx
+++ b/resources/test_data/VM_TestData_Sample1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22313"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_2b36\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{284550DA-19B3-4C7B-99A8-BC16CB819452}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{284550DA-19B3-4C7B-99A8-BC16CB819452}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CC1596CE-7320-47C0-BD47-B0CF208A0201}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="2055" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="2055" firstSheet="2" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LogInPage" sheetId="22" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="95">
   <si>
     <t>TestCaseNumber</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>P@ssw0rd</t>
+  </si>
+  <si>
+    <t>Enter</t>
   </si>
   <si>
     <t>VerifyUser</t>
@@ -1180,7 +1183,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:F6"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1226,7 +1229,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1246,7 +1249,7 @@
         <v>9</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1286,7 +1289,7 @@
         <v>9</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1306,7 +1309,7 @@
         <v>9</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1318,7 +1321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
@@ -1339,13 +1342,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1356,7 +1359,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -1432,7 +1435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AG7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -1477,97 +1480,97 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="T1" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="U1" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="V1" s="14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="W1" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="X1" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Y1" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Z1" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA1" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AB1" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AC1" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AD1" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AE1" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AF1" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AG1" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:33">
@@ -1579,7 +1582,7 @@
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5">
@@ -1587,12 +1590,12 @@
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
@@ -1601,37 +1604,37 @@
       </c>
       <c r="O2" s="5"/>
       <c r="P2" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="S2" s="7"/>
       <c r="T2" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="U2" s="7"/>
       <c r="V2" s="7"/>
       <c r="W2" s="8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="X2" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="Y2" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="Z2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="AA2" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AB2" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AC2" s="5"/>
       <c r="AD2" s="5" t="s">
@@ -1656,23 +1659,23 @@
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I3" s="11"/>
       <c r="J3" s="5"/>
       <c r="K3" s="10" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5" t="s">
@@ -1680,37 +1683,37 @@
       </c>
       <c r="O3" s="5"/>
       <c r="P3" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="R3" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="S3" s="7"/>
       <c r="T3" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="U3" s="7"/>
       <c r="V3" s="7"/>
       <c r="W3" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="X3" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Y3" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="Z3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="AA3" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AB3" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AC3" s="5"/>
       <c r="AD3" s="5" t="s">
@@ -1735,7 +1738,7 @@
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5">
@@ -1743,12 +1746,12 @@
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
@@ -1757,37 +1760,37 @@
       </c>
       <c r="O4" s="5"/>
       <c r="P4" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="R4" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="S4" s="7"/>
       <c r="T4" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="U4" s="7"/>
       <c r="V4" s="7"/>
       <c r="W4" s="8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="X4" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="Y4" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="Z4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="AA4" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AB4" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AC4" s="5"/>
       <c r="AD4" s="5" t="s">
@@ -1812,23 +1815,23 @@
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I5" s="11"/>
       <c r="J5" s="5"/>
       <c r="K5" s="10" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M5" s="5"/>
       <c r="N5" s="5" t="s">
@@ -1836,37 +1839,37 @@
       </c>
       <c r="O5" s="5"/>
       <c r="P5" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="R5" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="S5" s="7"/>
       <c r="T5" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="U5" s="7"/>
       <c r="V5" s="7"/>
       <c r="W5" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="X5" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Y5" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="Z5" s="5" t="s">
         <v>8</v>
       </c>
       <c r="AA5" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AB5" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AC5" s="5"/>
       <c r="AD5" s="5" t="s">
@@ -1891,7 +1894,7 @@
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>8</v>
@@ -1916,16 +1919,16 @@
       <c r="W6" s="6"/>
       <c r="X6" s="6"/>
       <c r="Y6" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="Z6" s="5" t="s">
         <v>8</v>
       </c>
       <c r="AA6" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AB6" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AC6" s="5"/>
       <c r="AD6" s="5" t="s">
@@ -1943,77 +1946,77 @@
         <v>3</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="15">
         <v>53704</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J7" s="6"/>
       <c r="K7" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L7" s="6"/>
       <c r="M7" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="R7" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="S7" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="T7" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="U7" s="6" t="s">
         <v>72</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="P7" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q7" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="R7" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="S7" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="T7" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="U7" s="6" t="s">
-        <v>71</v>
       </c>
       <c r="V7" s="6"/>
       <c r="W7" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="X7" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="Y7" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="Z7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="AA7" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AB7" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AC7" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AD7" s="5" t="s">
         <v>8</v>
@@ -2068,13 +2071,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2085,7 +2088,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -2130,34 +2133,34 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="L1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="14.25" customHeight="1">
@@ -2168,28 +2171,28 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K2" t="s">
         <v>8</v>
@@ -2222,7 +2225,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2233,7 +2236,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2244,7 +2247,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2255,7 +2258,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated New Test Data
</commit_message>
<xml_diff>
--- a/resources/test_data/VM_TestData_Sample1.xlsx
+++ b/resources/test_data/VM_TestData_Sample1.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22313"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_2b36\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\praneethm\git\VMSeleniumFramework\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{284550DA-19B3-4C7B-99A8-BC16CB819452}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CC1596CE-7320-47C0-BD47-B0CF208A0201}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="2055" firstSheet="2" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="2055" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LogInPage" sheetId="22" r:id="rId1"/>
@@ -31,7 +30,7 @@
     <definedName name="State">[1]Selectlists!$C$2:$C$52</definedName>
     <definedName name="waivsub">[1]Selectlists!$J$2:$J$6</definedName>
   </definedNames>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="112">
   <si>
     <t>TestCaseNumber</t>
   </si>
@@ -336,13 +335,64 @@
   </si>
   <si>
     <t>click</t>
+  </si>
+  <si>
+    <t>Keys.Enter</t>
+  </si>
+  <si>
+    <t>ControlKeys</t>
+  </si>
+  <si>
+    <t>124 New Street</t>
+  </si>
+  <si>
+    <t>12 - Agriculture, Forestry, Fishing and Hunting</t>
+  </si>
+  <si>
+    <t>654-98-7988</t>
+  </si>
+  <si>
+    <t>(654) 987 - 9799</t>
+  </si>
+  <si>
+    <t>Tab</t>
+  </si>
+  <si>
+    <t>Click $ Next</t>
+  </si>
+  <si>
+    <t>SelectLogin</t>
+  </si>
+  <si>
+    <t>SelectNext</t>
+  </si>
+  <si>
+    <t>SelectNewSubmission</t>
+  </si>
+  <si>
+    <t>Click $ New Submission</t>
+  </si>
+  <si>
+    <t>RandomName()</t>
+  </si>
+  <si>
+    <t>RandomNameWithNumbers()</t>
+  </si>
+  <si>
+    <t>RandomNumbers(11)</t>
+  </si>
+  <si>
+    <t>RandomEmail(&lt;gmail&gt;)</t>
+  </si>
+  <si>
+    <t>[654-98-7987]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -380,6 +430,27 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -389,7 +460,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -438,12 +509,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -484,6 +566,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -514,7 +608,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -1179,20 +1273,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1203,16 +1303,28 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="J1" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>101</v>
       </c>
@@ -1222,17 +1334,20 @@
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2"/>
+      <c r="I2" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>102</v>
       </c>
@@ -1242,17 +1357,20 @@
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="H3" s="2"/>
+      <c r="I3" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>103</v>
       </c>
@@ -1262,17 +1380,20 @@
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="H4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>104</v>
       </c>
@@ -1282,17 +1403,20 @@
       <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="H5" s="2"/>
+      <c r="I5" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>105</v>
       </c>
@@ -1302,39 +1426,127 @@
       <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="H6" s="21"/>
+      <c r="I6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
+    <row r="7" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="12">
+        <v>107</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>108</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>106</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>109</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G6" r:id="rId1"/>
+    <hyperlink ref="G8" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1345,13 +1557,16 @@
         <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>101</v>
       </c>
@@ -1361,11 +1576,12 @@
       <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>102</v>
       </c>
@@ -1373,11 +1589,12 @@
         <v>2</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>103</v>
       </c>
@@ -1385,11 +1602,12 @@
         <v>2</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>103</v>
       </c>
@@ -1397,12 +1615,13 @@
         <v>5</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="D5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>104</v>
       </c>
@@ -1411,18 +1630,69 @@
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="E6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>105</v>
       </c>
       <c r="B7" s="1">
         <v>2</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>107</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>108</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>106</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>109</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1432,14 +1702,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AG7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AI10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" customWidth="1"/>
     <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
@@ -1466,13 +1736,13 @@
     <col min="25" max="25" width="20" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="16" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="21.28515625" customWidth="1"/>
-    <col min="28" max="29" width="22.85546875" customWidth="1"/>
-    <col min="30" max="31" width="15.5703125" customWidth="1"/>
-    <col min="32" max="32" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="31" width="22.85546875" customWidth="1"/>
+    <col min="32" max="33" width="15.5703125" customWidth="1"/>
+    <col min="34" max="34" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1560,20 +1830,26 @@
       <c r="AC1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AD1" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="AE1" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="AE1" s="6" t="s">
+      <c r="AG1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="AF1" s="6" t="s">
+      <c r="AH1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="AG1" s="5" t="s">
+      <c r="AI1" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>101</v>
       </c>
@@ -1637,20 +1913,22 @@
         <v>57</v>
       </c>
       <c r="AC2" s="5"/>
-      <c r="AD2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AE2" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="AD2" s="5"/>
+      <c r="AE2" s="5"/>
       <c r="AF2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="AG2" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:33">
+      <c r="AH2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI2" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>102</v>
       </c>
@@ -1716,20 +1994,22 @@
         <v>68</v>
       </c>
       <c r="AC3" s="5"/>
-      <c r="AD3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AE3" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="AD3" s="5"/>
+      <c r="AE3" s="5"/>
       <c r="AF3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="AG3" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:33">
+      <c r="AH3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI3" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>103</v>
       </c>
@@ -1793,20 +2073,22 @@
         <v>57</v>
       </c>
       <c r="AC4" s="5"/>
-      <c r="AD4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AE4" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="AD4" s="5"/>
+      <c r="AE4" s="5"/>
       <c r="AF4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="AG4" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:33">
+      <c r="AH4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI4" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>103</v>
       </c>
@@ -1872,20 +2154,22 @@
         <v>68</v>
       </c>
       <c r="AC5" s="5"/>
-      <c r="AD5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AE5" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="AD5" s="5"/>
+      <c r="AE5" s="5"/>
       <c r="AF5" s="5" t="s">
         <v>8</v>
       </c>
       <c r="AG5" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:33">
+      <c r="AH5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI5" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>104</v>
       </c>
@@ -1931,14 +2215,16 @@
         <v>57</v>
       </c>
       <c r="AC6" s="5"/>
-      <c r="AD6" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="AD6" s="5"/>
       <c r="AE6" s="5"/>
-      <c r="AF6" s="5"/>
+      <c r="AF6" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="AG6" s="5"/>
-    </row>
-    <row r="7" spans="1:33">
+      <c r="AH6" s="5"/>
+      <c r="AI6" s="5"/>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>105</v>
       </c>
@@ -2018,30 +2304,251 @@
       <c r="AC7" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="AD7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AE7" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="AD7" s="5"/>
+      <c r="AE7" s="5"/>
       <c r="AF7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="AG7" s="5" t="s">
         <v>8</v>
       </c>
+      <c r="AH7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI7" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A8" s="18">
+        <v>107</v>
+      </c>
+      <c r="B8" s="15">
+        <v>3</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="15">
+        <v>53704</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="R8" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="T8" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="W8" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="X8" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y8" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA8" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB8" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD8" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="AE8" s="20" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="22">
+        <v>106</v>
+      </c>
+      <c r="B9" s="22">
+        <v>3</v>
+      </c>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22">
+        <v>53704</v>
+      </c>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q9" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="R9" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="S9" s="22"/>
+      <c r="T9" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="U9" s="22"/>
+      <c r="V9" s="22"/>
+      <c r="W9" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="X9" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y9" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z9" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA9" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB9" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC9" s="22"/>
+      <c r="AD9" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE9" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF9" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG9" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH9" s="1"/>
+      <c r="AI9" s="1"/>
+    </row>
+    <row r="10" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="22">
+        <v>109</v>
+      </c>
+      <c r="B10" s="22">
+        <v>3</v>
+      </c>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22">
+        <v>53704</v>
+      </c>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="O10" s="22"/>
+      <c r="P10" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q10" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="R10" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="S10" s="22"/>
+      <c r="T10" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="U10" s="22"/>
+      <c r="V10" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="W10" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="X10" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y10" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z10" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA10" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB10" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC10" s="22"/>
+      <c r="AD10" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE10" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF10" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG10" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH10" s="1"/>
+      <c r="AI10" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="F3:I3 K3 Q3 W2:X5 F5:I5 K5 Q5" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="F3:I3 K3 Q3 W2:X5 F5:I5 K5 Q5"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" display="random123@gmail.com" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="H3" r:id="rId2" display="random123@gmail.com" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="X2" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
-    <hyperlink ref="X4" r:id="rId4" xr:uid="{E26B484B-4383-46B5-A9DD-A9F40261C6F0}"/>
-    <hyperlink ref="F5" r:id="rId5" display="random123@gmail.com" xr:uid="{AA1CD9BD-A107-45B5-A12F-C6F47E7565F6}"/>
-    <hyperlink ref="H5" r:id="rId6" display="random123@gmail.com" xr:uid="{A7CBD975-BC9C-4366-B73D-B6D1D0A807A9}"/>
+    <hyperlink ref="F3" r:id="rId1" display="random123@gmail.com"/>
+    <hyperlink ref="H3" r:id="rId2" display="random123@gmail.com"/>
+    <hyperlink ref="X2" r:id="rId3"/>
+    <hyperlink ref="X4" r:id="rId4"/>
+    <hyperlink ref="F5" r:id="rId5" display="random123@gmail.com"/>
+    <hyperlink ref="H5" r:id="rId6" display="random123@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
@@ -2049,21 +2556,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.28515625" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2080,7 +2587,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>104</v>
       </c>
@@ -2103,14 +2610,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
@@ -2125,7 +2632,7 @@
     <col min="12" max="12" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2163,7 +2670,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="14.25" customHeight="1">
+    <row r="2" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>104</v>
       </c>
@@ -2207,17 +2714,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2228,7 +2737,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>101</v>
       </c>
@@ -2239,7 +2748,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>102</v>
       </c>
@@ -2250,7 +2759,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>103</v>
       </c>

</xml_diff>

<commit_message>
Fixed bugs: 58 & 54 (Test Case #'s: 108 and 106)
</commit_message>
<xml_diff>
--- a/resources/test_data/VM_TestData_Sample1.xlsx
+++ b/resources/test_data/VM_TestData_Sample1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22318"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\praneethm\git\VMSeleniumFramework\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D46DF327-2EA9-41C2-BBA5-936E2771012B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="2055" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="2055" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LogInPage" sheetId="22" r:id="rId1"/>
@@ -30,7 +31,7 @@
     <definedName name="State">[1]Selectlists!$C$2:$C$52</definedName>
     <definedName name="waivsub">[1]Selectlists!$J$2:$J$6</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="112">
   <si>
     <t>TestCaseNumber</t>
   </si>
@@ -57,33 +58,51 @@
     <t>UserName</t>
   </si>
   <si>
+    <t>SelectNext</t>
+  </si>
+  <si>
     <t>Next</t>
   </si>
   <si>
+    <t>Click</t>
+  </si>
+  <si>
     <t>Password</t>
   </si>
   <si>
+    <t>SelectLogin</t>
+  </si>
+  <si>
     <t>LogIn</t>
   </si>
   <si>
+    <t>ControlKeys</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
     <t>charles</t>
   </si>
   <si>
-    <t>Click</t>
-  </si>
-  <si>
     <t>P@ssw0rd</t>
   </si>
   <si>
     <t>Enter</t>
   </si>
   <si>
+    <t>Keys.Enter</t>
+  </si>
+  <si>
+    <t>Click $ Next</t>
+  </si>
+  <si>
     <t>VerifyUser</t>
   </si>
   <si>
+    <t>SelectNewSubmission</t>
+  </si>
+  <si>
     <t>NewSubmission</t>
   </si>
   <si>
@@ -93,6 +112,9 @@
     <t>AreEqual&gt;Thomas Charles</t>
   </si>
   <si>
+    <t>Click $ New Submission</t>
+  </si>
+  <si>
     <t>VerifyCustomerAccountName1</t>
   </si>
   <si>
@@ -274,6 +296,36 @@
   </si>
   <si>
     <t>CheckColor&gt;#48c157</t>
+  </si>
+  <si>
+    <t>124 New Street</t>
+  </si>
+  <si>
+    <t>12 - Agriculture, Forestry, Fishing and Hunting</t>
+  </si>
+  <si>
+    <t>654-98-7988</t>
+  </si>
+  <si>
+    <t>(654) 987 - 9799</t>
+  </si>
+  <si>
+    <t>Tab</t>
+  </si>
+  <si>
+    <t>RandomName()</t>
+  </si>
+  <si>
+    <t>RandomNameWithNumbers()</t>
+  </si>
+  <si>
+    <t>RandomNumbers(11)</t>
+  </si>
+  <si>
+    <t>RandomEmail(gmail.com)</t>
+  </si>
+  <si>
+    <t>[654-98-7987]</t>
   </si>
   <si>
     <t>Search</t>
@@ -335,64 +387,13 @@
   </si>
   <si>
     <t>click</t>
-  </si>
-  <si>
-    <t>Keys.Enter</t>
-  </si>
-  <si>
-    <t>ControlKeys</t>
-  </si>
-  <si>
-    <t>124 New Street</t>
-  </si>
-  <si>
-    <t>12 - Agriculture, Forestry, Fishing and Hunting</t>
-  </si>
-  <si>
-    <t>654-98-7988</t>
-  </si>
-  <si>
-    <t>(654) 987 - 9799</t>
-  </si>
-  <si>
-    <t>Tab</t>
-  </si>
-  <si>
-    <t>Click $ Next</t>
-  </si>
-  <si>
-    <t>SelectLogin</t>
-  </si>
-  <si>
-    <t>SelectNext</t>
-  </si>
-  <si>
-    <t>SelectNewSubmission</t>
-  </si>
-  <si>
-    <t>Click $ New Submission</t>
-  </si>
-  <si>
-    <t>RandomName()</t>
-  </si>
-  <si>
-    <t>RandomNameWithNumbers()</t>
-  </si>
-  <si>
-    <t>RandomNumbers(11)</t>
-  </si>
-  <si>
-    <t>RandomEmail(&lt;gmail&gt;)</t>
-  </si>
-  <si>
-    <t>[654-98-7987]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -608,7 +609,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -1273,14 +1274,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.5703125" customWidth="1"/>
@@ -1292,7 +1293,7 @@
     <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1303,97 +1304,97 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>104</v>
+        <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="J1" s="16" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="4">
         <v>101</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="4">
         <v>102</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="4">
         <v>103</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="12">
         <v>104</v>
       </c>
@@ -1401,22 +1402,22 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="12">
         <v>105</v>
       </c>
@@ -1424,22 +1425,22 @@
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="21" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H6" s="21"/>
       <c r="I6" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="16.5">
       <c r="A7" s="12">
         <v>107</v>
       </c>
@@ -1447,18 +1448,18 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="20" t="s">
-        <v>95</v>
+        <v>14</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="12">
         <v>108</v>
       </c>
@@ -1466,19 +1467,19 @@
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>102</v>
+        <v>15</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="I8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="12">
         <v>106</v>
       </c>
@@ -1486,19 +1487,19 @@
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G9" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="I9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="12">
         <v>109</v>
       </c>
@@ -1506,22 +1507,22 @@
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G10" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="I10" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G6" r:id="rId1"/>
-    <hyperlink ref="G8" r:id="rId2"/>
+    <hyperlink ref="G6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G8" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
@@ -1529,14 +1530,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
@@ -1546,7 +1547,7 @@
     <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1554,19 +1555,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>105</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>101</v>
       </c>
@@ -1574,14 +1575,14 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>102</v>
       </c>
@@ -1591,10 +1592,10 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>103</v>
       </c>
@@ -1604,10 +1605,10 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>103</v>
       </c>
@@ -1617,11 +1618,11 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>104</v>
       </c>
@@ -1632,10 +1633,10 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>105</v>
       </c>
@@ -1643,10 +1644,10 @@
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>107</v>
       </c>
@@ -1654,10 +1655,10 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>108</v>
       </c>
@@ -1665,10 +1666,10 @@
         <v>2</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
         <v>106</v>
       </c>
@@ -1676,13 +1677,10 @@
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
         <v>109</v>
       </c>
@@ -1690,10 +1688,10 @@
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F11" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1702,14 +1700,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AI10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="Y14" sqref="Y14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.140625" customWidth="1"/>
     <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
@@ -1742,7 +1740,7 @@
     <col min="35" max="35" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1750,106 +1748,106 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="T1" s="5" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="U1" s="5" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="V1" s="14" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="W1" s="5" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="X1" s="5" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="Y1" s="5" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="Z1" s="5" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="AA1" s="5" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="AB1" s="5" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="AC1" s="5" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="AD1" s="16" t="s">
-        <v>96</v>
+        <v>9</v>
       </c>
       <c r="AE1" s="16" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AF1" s="5" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="AG1" s="6" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="AH1" s="6" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="AI1" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35">
       <c r="A2" s="5">
         <v>101</v>
       </c>
@@ -1858,7 +1856,7 @@
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5">
@@ -1866,69 +1864,69 @@
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
       <c r="N2" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="O2" s="5"/>
       <c r="P2" s="5" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="S2" s="7"/>
       <c r="T2" s="7" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="U2" s="7"/>
       <c r="V2" s="7"/>
       <c r="W2" s="8" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="X2" s="9" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="Y2" s="5" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="Z2" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AA2" s="5" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="AB2" s="5" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="AC2" s="5"/>
       <c r="AD2" s="5"/>
       <c r="AE2" s="5"/>
       <c r="AF2" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AG2" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AH2" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AI2" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35">
       <c r="A3" s="5">
         <v>102</v>
       </c>
@@ -1937,79 +1935,79 @@
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="10" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="11" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="11" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="I3" s="11"/>
       <c r="J3" s="5"/>
       <c r="K3" s="10" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="O3" s="5"/>
       <c r="P3" s="5" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="R3" s="7" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="S3" s="7"/>
       <c r="T3" s="7" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="U3" s="7"/>
       <c r="V3" s="7"/>
       <c r="W3" s="8" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="X3" s="8" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="Y3" s="5" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="Z3" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AA3" s="5" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="AB3" s="5" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="AC3" s="5"/>
       <c r="AD3" s="5"/>
       <c r="AE3" s="5"/>
       <c r="AF3" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AG3" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AH3" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AI3" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35">
       <c r="A4" s="5">
         <v>103</v>
       </c>
@@ -2018,7 +2016,7 @@
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5">
@@ -2026,69 +2024,69 @@
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
       <c r="N4" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="O4" s="5"/>
       <c r="P4" s="5" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="R4" s="7" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="S4" s="7"/>
       <c r="T4" s="7" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="U4" s="7"/>
       <c r="V4" s="7"/>
       <c r="W4" s="8" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="X4" s="9" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="Y4" s="5" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="Z4" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AA4" s="5" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="AB4" s="5" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="AC4" s="5"/>
       <c r="AD4" s="5"/>
       <c r="AE4" s="5"/>
       <c r="AF4" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AG4" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AH4" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AI4" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35">
       <c r="A5" s="5">
         <v>103</v>
       </c>
@@ -2097,79 +2095,79 @@
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="10" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="11" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="I5" s="11"/>
       <c r="J5" s="5"/>
       <c r="K5" s="10" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="M5" s="5"/>
       <c r="N5" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="O5" s="5"/>
       <c r="P5" s="5" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="R5" s="7" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="S5" s="7"/>
       <c r="T5" s="7" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="U5" s="7"/>
       <c r="V5" s="7"/>
       <c r="W5" s="8" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="X5" s="8" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="Y5" s="5" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="Z5" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AA5" s="5" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="AB5" s="5" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="AC5" s="5"/>
       <c r="AD5" s="5"/>
       <c r="AE5" s="5"/>
       <c r="AF5" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AG5" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AH5" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AI5" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35">
       <c r="A6" s="15">
         <v>104</v>
       </c>
@@ -2178,10 +2176,10 @@
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="15" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -2203,28 +2201,28 @@
       <c r="W6" s="6"/>
       <c r="X6" s="6"/>
       <c r="Y6" s="5" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="Z6" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AA6" s="5" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="AB6" s="5" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="AC6" s="5"/>
       <c r="AD6" s="5"/>
       <c r="AE6" s="5"/>
       <c r="AF6" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AG6" s="5"/>
       <c r="AH6" s="5"/>
       <c r="AI6" s="5"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35">
       <c r="A7" s="15">
         <v>105</v>
       </c>
@@ -2232,94 +2230,94 @@
         <v>3</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="15">
         <v>53704</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="J7" s="6"/>
       <c r="K7" s="6" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="L7" s="6"/>
       <c r="M7" s="6" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="P7" s="6" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="Q7" s="6" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="S7" s="6" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="T7" s="6" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="U7" s="6" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="V7" s="6"/>
       <c r="W7" s="6" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="X7" s="6" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="Y7" s="5" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="Z7" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AA7" s="5" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="AB7" s="5" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="AC7" s="5" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="AD7" s="5"/>
       <c r="AE7" s="5"/>
       <c r="AF7" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AG7" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AH7" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AI7" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35">
       <c r="A8" s="18">
         <v>107</v>
       </c>
@@ -2327,58 +2325,58 @@
         <v>3</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="F8" s="15">
         <v>53704</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="P8" s="6" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="Q8" s="6" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="R8" s="6" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="T8" s="6" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="W8" s="6" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="X8" s="6" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="Y8" s="5" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="Z8" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AA8" s="5" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="AB8" s="5" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="AD8" s="16" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="AE8" s="20" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" ht="13.5" customHeight="1">
       <c r="A9" s="22">
         <v>106</v>
       </c>
@@ -2387,7 +2385,7 @@
       </c>
       <c r="C9" s="22"/>
       <c r="D9" s="22" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="E9" s="22"/>
       <c r="F9" s="22">
@@ -2395,69 +2393,69 @@
       </c>
       <c r="G9" s="22"/>
       <c r="H9" s="22" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="I9" s="22"/>
       <c r="J9" s="22"/>
       <c r="K9" s="22" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="L9" s="22"/>
       <c r="M9" s="22"/>
       <c r="N9" s="22" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="O9" s="22"/>
       <c r="P9" s="22" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="Q9" s="22" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="R9" s="22" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="S9" s="22"/>
       <c r="T9" s="22" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="U9" s="22"/>
       <c r="V9" s="22"/>
       <c r="W9" s="22" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="X9" s="22" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="Y9" s="22" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="Z9" s="22" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AA9" s="22" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="AB9" s="22" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="AC9" s="22"/>
       <c r="AD9" s="22" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AE9" s="22" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AF9" s="22" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AG9" s="22" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AH9" s="1"/>
       <c r="AI9" s="1"/>
     </row>
-    <row r="10" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" ht="13.5" customHeight="1">
       <c r="A10" s="22">
         <v>109</v>
       </c>
@@ -2466,7 +2464,7 @@
       </c>
       <c r="C10" s="22"/>
       <c r="D10" s="22" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="E10" s="22"/>
       <c r="F10" s="22">
@@ -2474,81 +2472,81 @@
       </c>
       <c r="G10" s="22"/>
       <c r="H10" s="22" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="I10" s="22"/>
       <c r="J10" s="22"/>
       <c r="K10" s="22" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="L10" s="22"/>
       <c r="M10" s="22"/>
       <c r="N10" s="22" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="O10" s="22"/>
       <c r="P10" s="22" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="Q10" s="22" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="R10" s="22" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="S10" s="22"/>
       <c r="T10" s="22" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="U10" s="22"/>
       <c r="V10" s="22" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="W10" s="22" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="X10" s="22" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="Y10" s="22" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="Z10" s="22" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AA10" s="22" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="AB10" s="22" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="AC10" s="22"/>
       <c r="AD10" s="22" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AE10" s="22" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AF10" s="22" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AG10" s="22" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AH10" s="1"/>
       <c r="AI10" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="F3:I3 K3 Q3 W2:X5 F5:I5 K5 Q5"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="F3:I3 K3 Q3 W2:X5 F5:I5 K5 Q5" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" display="random123@gmail.com"/>
-    <hyperlink ref="H3" r:id="rId2" display="random123@gmail.com"/>
-    <hyperlink ref="X2" r:id="rId3"/>
-    <hyperlink ref="X4" r:id="rId4"/>
-    <hyperlink ref="F5" r:id="rId5" display="random123@gmail.com"/>
-    <hyperlink ref="H5" r:id="rId6" display="random123@gmail.com"/>
+    <hyperlink ref="F3" r:id="rId1" display="random123@gmail.com" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="H3" r:id="rId2" display="random123@gmail.com" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="X2" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="X4" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="F5" r:id="rId5" display="random123@gmail.com" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="H5" r:id="rId6" display="random123@gmail.com" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
@@ -2556,21 +2554,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.28515625" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2578,16 +2576,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="E1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>104</v>
       </c>
@@ -2595,13 +2593,13 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -2610,14 +2608,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
@@ -2632,7 +2630,7 @@
     <col min="12" max="12" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2640,37 +2638,37 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="D1" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="E1" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="F1" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="G1" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="H1" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="I1" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="J1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="K1" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="L1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="14.25" customHeight="1">
       <c r="A2" s="1">
         <v>104</v>
       </c>
@@ -2678,34 +2676,34 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="D2" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="E2" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="K2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="L2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -2714,19 +2712,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2734,10 +2732,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="3">
         <v>101</v>
       </c>
@@ -2745,10 +2743,10 @@
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="3">
         <v>102</v>
       </c>
@@ -2756,10 +2754,10 @@
         <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="3">
         <v>103</v>
       </c>
@@ -2767,7 +2765,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Parallel Execution (Incomplete). Fix for bug #62.
</commit_message>
<xml_diff>
--- a/resources/test_data/VM_TestData_Sample1.xlsx
+++ b/resources/test_data/VM_TestData_Sample1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\praneethm\git\VMSeleniumFramework\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D46DF327-2EA9-41C2-BBA5-936E2771012B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_40E9362B34929B80EF67A5383EEB3898EAE03450" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{180D7F04-6A3F-44E0-85AC-1C854564C67E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="2055" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="2055" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LogInPage" sheetId="22" r:id="rId1"/>
@@ -393,6 +393,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
+  </numFmts>
   <fonts count="9">
     <font>
       <sz val="11"/>
@@ -526,7 +529,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -579,6 +582,13 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1533,7 +1543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -1703,8 +1713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AI10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Y14" sqref="Y14"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1892,7 +1902,7 @@
       </c>
       <c r="U2" s="7"/>
       <c r="V2" s="7"/>
-      <c r="W2" s="8" t="s">
+      <c r="W2" s="24" t="s">
         <v>60</v>
       </c>
       <c r="X2" s="9" t="s">
@@ -1973,7 +1983,7 @@
       </c>
       <c r="U3" s="7"/>
       <c r="V3" s="7"/>
-      <c r="W3" s="8" t="s">
+      <c r="W3" s="24" t="s">
         <v>72</v>
       </c>
       <c r="X3" s="8" t="s">
@@ -2052,7 +2062,7 @@
       </c>
       <c r="U4" s="7"/>
       <c r="V4" s="7"/>
-      <c r="W4" s="8" t="s">
+      <c r="W4" s="24" t="s">
         <v>60</v>
       </c>
       <c r="X4" s="9" t="s">
@@ -2133,7 +2143,7 @@
       </c>
       <c r="U5" s="7"/>
       <c r="V5" s="7"/>
-      <c r="W5" s="8" t="s">
+      <c r="W5" s="24" t="s">
         <v>72</v>
       </c>
       <c r="X5" s="8" t="s">
@@ -2198,7 +2208,7 @@
       <c r="T6" s="6"/>
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
-      <c r="W6" s="6"/>
+      <c r="W6" s="25"/>
       <c r="X6" s="6"/>
       <c r="Y6" s="5" t="s">
         <v>62</v>
@@ -2281,7 +2291,7 @@
         <v>79</v>
       </c>
       <c r="V7" s="6"/>
-      <c r="W7" s="6" t="s">
+      <c r="W7" s="25" t="s">
         <v>60</v>
       </c>
       <c r="X7" s="6" t="s">
@@ -2351,7 +2361,7 @@
       <c r="T8" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="W8" s="6" t="s">
+      <c r="W8" s="25" t="s">
         <v>86</v>
       </c>
       <c r="X8" s="6" t="s">
@@ -2421,7 +2431,7 @@
       </c>
       <c r="U9" s="22"/>
       <c r="V9" s="22"/>
-      <c r="W9" s="22" t="s">
+      <c r="W9" s="26" t="s">
         <v>90</v>
       </c>
       <c r="X9" s="22" t="s">
@@ -2502,7 +2512,7 @@
       <c r="V10" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="W10" s="22" t="s">
+      <c r="W10" s="26" t="s">
         <v>60</v>
       </c>
       <c r="X10" s="22" t="s">

</xml_diff>

<commit_message>
Updated Excel file for task 48
</commit_message>
<xml_diff>
--- a/resources/test_data/VM_TestData_Sample1.xlsx
+++ b/resources/test_data/VM_TestData_Sample1.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\praneethm\git\VMSeleniumFramework\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A72CD07-ED3C-4D4D-8D69-26337C142E9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="83" documentId="8_{2A72CD07-ED3C-4D4D-8D69-26337C142E9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D35010AA-C071-4248-8F19-9D75C12F41EB}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="2055" firstSheet="2" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="2055" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="LogInPage" sheetId="22" r:id="rId1"/>
-    <sheet name="IndexPage" sheetId="23" r:id="rId2"/>
-    <sheet name="NewSubmissionPage" sheetId="24" r:id="rId3"/>
-    <sheet name="ServicePolicy" sheetId="26" r:id="rId4"/>
-    <sheet name="CustomerInformationPage" sheetId="27" r:id="rId5"/>
-    <sheet name="SubmissionSummaryPage" sheetId="25" r:id="rId6"/>
+    <sheet name="HomePage" sheetId="28" r:id="rId1"/>
+    <sheet name="LogInPage" sheetId="22" r:id="rId2"/>
+    <sheet name="IndexPage" sheetId="23" r:id="rId3"/>
+    <sheet name="NewSubmissionPage" sheetId="24" r:id="rId4"/>
+    <sheet name="ServicePolicy" sheetId="26" r:id="rId5"/>
+    <sheet name="CustomerInformationPage" sheetId="27" r:id="rId6"/>
+    <sheet name="SubmissionSummaryPage" sheetId="25" r:id="rId7"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <definedNames>
     <definedName name="Abc">#REF!</definedName>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="112">
   <si>
     <t>TestCaseNumber</t>
   </si>
@@ -67,6 +68,18 @@
     <t>Click</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>charles</t>
+  </si>
+  <si>
+    <t>Keys.Enter</t>
+  </si>
+  <si>
+    <t>Click $ Next</t>
+  </si>
+  <si>
     <t>Password</t>
   </si>
   <si>
@@ -79,22 +92,10 @@
     <t>ControlKeys</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>charles</t>
-  </si>
-  <si>
     <t>P@ssw0rd</t>
   </si>
   <si>
     <t>Enter</t>
-  </si>
-  <si>
-    <t>Keys.Enter</t>
-  </si>
-  <si>
-    <t>Click $ Next</t>
   </si>
   <si>
     <t>VerifyUser</t>
@@ -464,7 +465,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -504,17 +505,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF000000"/>
       </left>
       <right style="thin">
@@ -534,11 +524,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -560,9 +546,6 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -571,23 +554,34 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1284,267 +1278,419 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A1CDF5E-0CC7-4AE9-8C27-E09EF38E63C9}">
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12" style="1" customWidth="1"/>
+    <col min="7" max="9" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="21">
+        <v>101</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="21">
+        <v>102</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="21">
+        <v>103</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="22">
+        <v>104</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="22">
+        <v>105</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="22">
+        <v>107</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="22">
+        <v>108</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="22">
+        <v>106</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="22">
+        <v>109</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1">
+        <v>110</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.5703125" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
     <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="21">
+        <v>101</v>
+      </c>
+      <c r="B2" s="4">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="4">
-        <v>101</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="4">
+      <c r="C2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="21">
         <v>102</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="4">
+      <c r="B3" s="4">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="21">
         <v>103</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="12">
+      <c r="B4" s="4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="22">
         <v>104</v>
       </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="12">
+      <c r="B5" s="4">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="22">
         <v>105</v>
       </c>
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="21"/>
-      <c r="I6" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="16.5">
-      <c r="A7" s="12">
+      <c r="B6" s="4">
+        <v>2</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="23"/>
+      <c r="E6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" ht="16.5">
+      <c r="A7" s="22">
         <v>107</v>
       </c>
-      <c r="B7" s="1">
-        <v>1</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="20" t="s">
+      <c r="B7" s="4">
+        <v>2</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="22">
+        <v>108</v>
+      </c>
+      <c r="B8" s="4">
+        <v>2</v>
+      </c>
+      <c r="C8" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="J7" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="12">
-        <v>108</v>
-      </c>
-      <c r="B8" s="1">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="22">
+        <v>106</v>
+      </c>
+      <c r="B9" s="4">
+        <v>2</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="12">
-        <v>106</v>
-      </c>
-      <c r="B9" s="1">
-        <v>1</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" t="s">
-        <v>5</v>
-      </c>
-      <c r="G9" t="s">
-        <v>12</v>
-      </c>
-      <c r="I9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="12">
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="22">
         <v>109</v>
       </c>
-      <c r="B10" s="1">
-        <v>1</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" t="s">
-        <v>5</v>
-      </c>
-      <c r="G10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I10" t="s">
-        <v>13</v>
+      <c r="B10" s="4">
+        <v>2</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1">
+        <v>110</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="G8" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C8" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1582,7 +1728,7 @@
         <v>101</v>
       </c>
       <c r="B2" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>20</v>
@@ -1597,7 +1743,7 @@
         <v>102</v>
       </c>
       <c r="B3" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -1610,7 +1756,7 @@
         <v>103</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -1623,7 +1769,7 @@
         <v>103</v>
       </c>
       <c r="B5" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -1637,7 +1783,7 @@
         <v>104</v>
       </c>
       <c r="B6" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -1649,7 +1795,7 @@
         <v>105</v>
       </c>
       <c r="B7" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7" t="s">
         <v>5</v>
@@ -1660,7 +1806,7 @@
         <v>107</v>
       </c>
       <c r="B8" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E8" t="s">
         <v>5</v>
@@ -1671,9 +1817,9 @@
         <v>108</v>
       </c>
       <c r="B9" s="1">
-        <v>2</v>
-      </c>
-      <c r="D9" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="15" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1682,7 +1828,7 @@
         <v>106</v>
       </c>
       <c r="B10" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E10" t="s">
         <v>5</v>
@@ -1693,7 +1839,7 @@
         <v>109</v>
       </c>
       <c r="B11" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E11" t="s">
         <v>5</v>
@@ -1704,12 +1850,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AI10"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1746,796 +1892,796 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="S1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="T1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="U1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="V1" s="14" t="s">
+      <c r="V1" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="W1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="X1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="Y1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="Z1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AA1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AB1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AC1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AD1" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="AE1" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="AF1" s="5" t="s">
+      <c r="AD1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF1" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AG1" s="6" t="s">
+      <c r="AG1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="AH1" s="6" t="s">
+      <c r="AH1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AI1" s="5" t="s">
+      <c r="AI1" s="3" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:35">
-      <c r="A2" s="5">
+      <c r="A2" s="3">
         <v>101</v>
       </c>
-      <c r="B2" s="5">
-        <v>3</v>
-      </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5" t="s">
+      <c r="B2" s="3">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3">
         <v>53704</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5" t="s">
+      <c r="G2" s="3"/>
+      <c r="H2" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5" t="s">
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5" t="s">
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="Q2" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="R2" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7" t="s">
+      <c r="S2" s="5"/>
+      <c r="T2" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7"/>
-      <c r="W2" s="24" t="s">
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="X2" s="9" t="s">
+      <c r="X2" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="Y2" s="5" t="s">
+      <c r="Y2" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="Z2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA2" s="5" t="s">
+      <c r="Z2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA2" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AB2" s="5" t="s">
+      <c r="AB2" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="AC2" s="5"/>
-      <c r="AD2" s="5"/>
-      <c r="AE2" s="5"/>
-      <c r="AF2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AH2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI2" s="5" t="s">
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:35">
-      <c r="A3" s="5">
+      <c r="A3" s="3">
         <v>102</v>
       </c>
-      <c r="B3" s="5">
-        <v>3</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="10" t="s">
+      <c r="B3" s="3">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="11" t="s">
+      <c r="E3" s="3"/>
+      <c r="F3" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11" t="s">
+      <c r="G3" s="9"/>
+      <c r="H3" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="I3" s="11"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="10" t="s">
+      <c r="I3" s="9"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5" t="s">
+      <c r="M3" s="3"/>
+      <c r="N3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="Q3" s="5" t="s">
+      <c r="Q3" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="R3" s="7" t="s">
+      <c r="R3" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7" t="s">
+      <c r="S3" s="5"/>
+      <c r="T3" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7"/>
-      <c r="W3" s="24" t="s">
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="X3" s="8" t="s">
+      <c r="X3" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="Y3" s="5" t="s">
+      <c r="Y3" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="Z3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA3" s="5" t="s">
+      <c r="Z3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA3" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AB3" s="5" t="s">
+      <c r="AB3" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="AC3" s="5"/>
-      <c r="AD3" s="5"/>
-      <c r="AE3" s="5"/>
-      <c r="AF3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AH3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI3" s="5" t="s">
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
+      <c r="AE3" s="3"/>
+      <c r="AF3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:35">
-      <c r="A4" s="5">
+      <c r="A4" s="3">
         <v>103</v>
       </c>
-      <c r="B4" s="5">
-        <v>3</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5" t="s">
+      <c r="B4" s="3">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5">
+      <c r="E4" s="3"/>
+      <c r="F4" s="3">
         <v>53704</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5" t="s">
+      <c r="G4" s="3"/>
+      <c r="H4" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5" t="s">
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5" t="s">
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="Q4" s="5" t="s">
+      <c r="Q4" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="R4" s="7" t="s">
+      <c r="R4" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7" t="s">
+      <c r="S4" s="5"/>
+      <c r="T4" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="U4" s="7"/>
-      <c r="V4" s="7"/>
-      <c r="W4" s="24" t="s">
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="X4" s="9" t="s">
+      <c r="X4" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="Y4" s="5" t="s">
+      <c r="Y4" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="Z4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA4" s="5" t="s">
+      <c r="Z4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA4" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AB4" s="5" t="s">
+      <c r="AB4" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="AC4" s="5"/>
-      <c r="AD4" s="5"/>
-      <c r="AE4" s="5"/>
-      <c r="AF4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AH4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI4" s="5" t="s">
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="3"/>
+      <c r="AE4" s="3"/>
+      <c r="AF4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:35">
-      <c r="A5" s="5">
+      <c r="A5" s="3">
         <v>103</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="3">
+        <v>7</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="I5" s="9"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="X5" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y5" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB5" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="3"/>
+      <c r="AE5" s="3"/>
+      <c r="AF5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI5" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35">
+      <c r="A6" s="12">
+        <v>104</v>
+      </c>
+      <c r="B6" s="12">
         <v>6</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="I5" s="11"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5" t="s">
+      <c r="C6" s="12"/>
+      <c r="D6" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+      <c r="W6" s="18"/>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB6" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG6" s="3"/>
+      <c r="AH6" s="3"/>
+      <c r="AI6" s="3"/>
+    </row>
+    <row r="7" spans="1:35">
+      <c r="A7" s="12">
+        <v>105</v>
+      </c>
+      <c r="B7" s="12">
+        <v>4</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="12">
+        <v>53704</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="P7" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="Q5" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="R5" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7" t="s">
+      <c r="Q7" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="T7" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
-      <c r="W5" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="X5" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="Y5" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA5" s="5" t="s">
+      <c r="U7" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="V7" s="4"/>
+      <c r="W7" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="X7" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y7" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA7" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AB5" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="AC5" s="5"/>
-      <c r="AD5" s="5"/>
-      <c r="AE5" s="5"/>
-      <c r="AF5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AH5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI5" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:35">
-      <c r="A6" s="15">
-        <v>104</v>
-      </c>
-      <c r="B6" s="15">
-        <v>5</v>
-      </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="6"/>
-      <c r="U6" s="6"/>
-      <c r="V6" s="6"/>
-      <c r="W6" s="25"/>
-      <c r="X6" s="6"/>
-      <c r="Y6" s="5" t="s">
+      <c r="AB7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC7" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD7" s="3"/>
+      <c r="AE7" s="3"/>
+      <c r="AF7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI7" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35">
+      <c r="A8" s="14">
+        <v>107</v>
+      </c>
+      <c r="B8" s="12">
+        <v>4</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="12">
+        <v>53704</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="R8" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="T8" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="W8" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="X8" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y8" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="Z6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA6" s="5" t="s">
+      <c r="Z8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA8" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AB6" s="5" t="s">
+      <c r="AB8" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="AC6" s="5"/>
-      <c r="AD6" s="5"/>
-      <c r="AE6" s="5"/>
-      <c r="AF6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG6" s="5"/>
-      <c r="AH6" s="5"/>
-      <c r="AI6" s="5"/>
-    </row>
-    <row r="7" spans="1:35">
-      <c r="A7" s="15">
-        <v>105</v>
-      </c>
-      <c r="B7" s="15">
-        <v>3</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="15">
+      <c r="AD8" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE8" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" ht="13.5" customHeight="1">
+      <c r="A9" s="16">
+        <v>106</v>
+      </c>
+      <c r="B9" s="16">
+        <v>4</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16">
         <v>53704</v>
       </c>
-      <c r="G7" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="H7" s="6" t="s">
+      <c r="G9" s="16"/>
+      <c r="H9" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="I7" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="P7" s="6" t="s">
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="Q7" s="6" t="s">
+      <c r="Q9" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="R7" s="6" t="s">
+      <c r="R9" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="S7" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="T7" s="6" t="s">
+      <c r="S9" s="16"/>
+      <c r="T9" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="U7" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="V7" s="6"/>
-      <c r="W7" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="X7" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y7" s="5" t="s">
+      <c r="U9" s="16"/>
+      <c r="V9" s="16"/>
+      <c r="W9" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="X9" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y9" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="Z7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA7" s="5" t="s">
+      <c r="Z9" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA9" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="AB7" s="5" t="s">
+      <c r="AB9" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="AC7" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD7" s="5"/>
-      <c r="AE7" s="5"/>
-      <c r="AF7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AH7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI7" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:35">
-      <c r="A8" s="18">
-        <v>107</v>
-      </c>
-      <c r="B8" s="15">
-        <v>3</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" s="15">
-        <v>53704</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="N8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="P8" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q8" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="R8" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="T8" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="W8" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="X8" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y8" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA8" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="AB8" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="AD8" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE8" s="20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:35" ht="13.5" customHeight="1">
-      <c r="A9" s="22">
-        <v>106</v>
-      </c>
-      <c r="B9" s="22">
-        <v>3</v>
-      </c>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22">
-        <v>53704</v>
-      </c>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="O9" s="22"/>
-      <c r="P9" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q9" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="R9" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="S9" s="22"/>
-      <c r="T9" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="U9" s="22"/>
-      <c r="V9" s="22"/>
-      <c r="W9" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="X9" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y9" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z9" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA9" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="AB9" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="AC9" s="22"/>
-      <c r="AD9" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="AE9" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="AF9" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG9" s="22" t="s">
+      <c r="AC9" s="16"/>
+      <c r="AD9" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE9" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF9" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG9" s="16" t="s">
         <v>5</v>
       </c>
       <c r="AH9" s="1"/>
       <c r="AI9" s="1"/>
     </row>
     <row r="10" spans="1:35" ht="13.5" customHeight="1">
-      <c r="A10" s="22">
+      <c r="A10" s="16">
         <v>109</v>
       </c>
-      <c r="B10" s="22">
-        <v>3</v>
-      </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22" t="s">
+      <c r="B10" s="16">
+        <v>4</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22">
+      <c r="E10" s="16"/>
+      <c r="F10" s="16">
         <v>53704</v>
       </c>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22" t="s">
+      <c r="G10" s="16"/>
+      <c r="H10" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22" t="s">
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22" t="s">
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="Q10" s="22" t="s">
+      <c r="Q10" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="R10" s="22" t="s">
+      <c r="R10" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="S10" s="22"/>
-      <c r="T10" s="22" t="s">
+      <c r="S10" s="16"/>
+      <c r="T10" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="U10" s="22"/>
-      <c r="V10" s="22" t="s">
+      <c r="U10" s="16"/>
+      <c r="V10" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="W10" s="26" t="s">
+      <c r="W10" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="X10" s="22" t="s">
+      <c r="X10" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="Y10" s="22" t="s">
+      <c r="Y10" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="Z10" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA10" s="22" t="s">
+      <c r="Z10" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA10" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="AB10" s="22" t="s">
+      <c r="AB10" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="AC10" s="22"/>
-      <c r="AD10" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="AE10" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="AF10" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG10" s="22" t="s">
+      <c r="AC10" s="16"/>
+      <c r="AD10" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE10" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF10" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG10" s="16" t="s">
         <v>5</v>
       </c>
       <c r="AH10" s="1"/>
@@ -2558,12 +2704,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2595,7 +2741,7 @@
         <v>104</v>
       </c>
       <c r="B2" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
         <v>53</v>
@@ -2612,12 +2758,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2678,7 +2824,7 @@
         <v>104</v>
       </c>
       <c r="B2" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>103</v>
@@ -2689,19 +2835,19 @@
       <c r="E2" t="s">
         <v>105</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="10" t="s">
         <v>109</v>
       </c>
       <c r="K2" t="s">
@@ -2716,7 +2862,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -2730,46 +2876,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>101</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>102</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>103</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>4</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed Bug 82: Fixed functionality of ControlKeys
</commit_message>
<xml_diff>
--- a/resources/test_data/VM_TestData_Sample1.xlsx
+++ b/resources/test_data/VM_TestData_Sample1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22318"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\praneethm\git\VMSeleniumFramework\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A72CD07-ED3C-4D4D-8D69-26337C142E9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{2A72CD07-ED3C-4D4D-8D69-26337C142E9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{795BAC45-F079-49B0-A8BA-2351EC938744}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="2055" firstSheet="2" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="2055" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LogInPage" sheetId="22" r:id="rId1"/>
@@ -39,7 +39,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -47,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="113">
   <si>
     <t>TestCaseNumber</t>
   </si>
@@ -64,27 +66,30 @@
     <t>Next</t>
   </si>
   <si>
+    <t>ControlKeys</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>SelectLogin</t>
+  </si>
+  <si>
+    <t>LogIn</t>
+  </si>
+  <si>
+    <t>ControlKeys2</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>charles</t>
+  </si>
+  <si>
     <t>Click</t>
   </si>
   <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>SelectLogin</t>
-  </si>
-  <si>
-    <t>LogIn</t>
-  </si>
-  <si>
-    <t>ControlKeys</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>charles</t>
-  </si>
-  <si>
     <t>P@ssw0rd</t>
   </si>
   <si>
@@ -310,7 +315,7 @@
     <t>(654) 987 - 9799</t>
   </si>
   <si>
-    <t>Tab</t>
+    <t>Tab, Return</t>
   </si>
   <si>
     <t>RandomName()</t>
@@ -1288,7 +1293,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1297,7 +1302,7 @@
     <col min="2" max="2" width="6.5703125" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
     <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
@@ -1347,15 +1352,15 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1370,15 +1375,15 @@
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1393,15 +1398,15 @@
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1416,15 +1421,15 @@
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1439,15 +1444,15 @@
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="21" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H6" s="21"/>
       <c r="I6" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="16.5">
@@ -1463,10 +1468,13 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="17" t="s">
         <v>14</v>
-      </c>
-      <c r="J7" s="17" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1480,13 +1488,13 @@
         <v>11</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I8" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1500,13 +1508,13 @@
         <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1520,13 +1528,13 @@
         <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1543,7 +1551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -1565,16 +1573,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1585,11 +1593,11 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1602,7 +1610,7 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1615,7 +1623,7 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1628,7 +1636,7 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F5" s="1"/>
     </row>
@@ -1652,7 +1660,7 @@
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1663,7 +1671,7 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1674,7 +1682,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1685,7 +1693,7 @@
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1696,7 +1704,7 @@
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1706,10 +1714,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AI10"/>
+  <dimension ref="A1:AH10"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AE1" sqref="AE1:AE1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1739,13 +1747,13 @@
     <col min="25" max="25" width="20" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="16" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="21.28515625" customWidth="1"/>
-    <col min="28" max="31" width="22.85546875" customWidth="1"/>
-    <col min="32" max="33" width="15.5703125" customWidth="1"/>
-    <col min="34" max="34" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="30" width="22.85546875" customWidth="1"/>
+    <col min="31" max="32" width="15.5703125" customWidth="1"/>
+    <col min="33" max="33" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:34">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1753,106 +1761,103 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="T1" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="U1" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="V1" s="14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="W1" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="X1" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Y1" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Z1" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AA1" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AB1" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AC1" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AD1" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="AE1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="AF1" s="5" t="s">
-        <v>49</v>
+      <c r="AE1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF1" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="AG1" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="AH1" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AI1" s="5" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="2" spans="1:35">
+      <c r="AH1" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34">
       <c r="A2" s="5">
         <v>101</v>
       </c>
@@ -1861,7 +1866,7 @@
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5">
@@ -1869,69 +1874,68 @@
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
       <c r="N2" s="5" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="O2" s="5"/>
       <c r="P2" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="S2" s="7"/>
       <c r="T2" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="U2" s="7"/>
       <c r="V2" s="7"/>
       <c r="W2" s="24" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="X2" s="9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Y2" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="Z2" s="5" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="AA2" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AB2" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AC2" s="5"/>
       <c r="AD2" s="5"/>
-      <c r="AE2" s="5"/>
+      <c r="AE2" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="AF2" s="5" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="AG2" s="5" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="AH2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI2" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34">
       <c r="A3" s="5">
         <v>102</v>
       </c>
@@ -1940,79 +1944,78 @@
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="11" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I3" s="11"/>
       <c r="J3" s="5"/>
       <c r="K3" s="10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="O3" s="5"/>
       <c r="P3" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="R3" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="S3" s="7"/>
       <c r="T3" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="U3" s="7"/>
       <c r="V3" s="7"/>
       <c r="W3" s="24" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="X3" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="Y3" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="Z3" s="5" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="AA3" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AB3" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AC3" s="5"/>
       <c r="AD3" s="5"/>
-      <c r="AE3" s="5"/>
+      <c r="AE3" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="AF3" s="5" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="AG3" s="5" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="AH3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI3" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34">
       <c r="A4" s="5">
         <v>103</v>
       </c>
@@ -2021,7 +2024,7 @@
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5">
@@ -2029,69 +2032,68 @@
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
       <c r="N4" s="5" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="O4" s="5"/>
       <c r="P4" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="R4" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="S4" s="7"/>
       <c r="T4" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="U4" s="7"/>
       <c r="V4" s="7"/>
       <c r="W4" s="24" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="X4" s="9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Y4" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="Z4" s="5" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="AA4" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AB4" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AC4" s="5"/>
       <c r="AD4" s="5"/>
-      <c r="AE4" s="5"/>
+      <c r="AE4" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="AF4" s="5" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="AG4" s="5" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="AH4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI4" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34">
       <c r="A5" s="5">
         <v>103</v>
       </c>
@@ -2100,79 +2102,78 @@
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I5" s="11"/>
       <c r="J5" s="5"/>
       <c r="K5" s="10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="M5" s="5"/>
       <c r="N5" s="5" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="O5" s="5"/>
       <c r="P5" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="R5" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="S5" s="7"/>
       <c r="T5" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="U5" s="7"/>
       <c r="V5" s="7"/>
       <c r="W5" s="24" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="X5" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="Y5" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="Z5" s="5" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="AA5" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AB5" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AC5" s="5"/>
       <c r="AD5" s="5"/>
-      <c r="AE5" s="5"/>
+      <c r="AE5" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="AF5" s="5" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="AG5" s="5" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="AH5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI5" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34">
       <c r="A6" s="15">
         <v>104</v>
       </c>
@@ -2181,10 +2182,10 @@
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="15" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -2206,28 +2207,27 @@
       <c r="W6" s="25"/>
       <c r="X6" s="6"/>
       <c r="Y6" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="Z6" s="5" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="AA6" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AB6" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AC6" s="5"/>
       <c r="AD6" s="5"/>
-      <c r="AE6" s="5"/>
-      <c r="AF6" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="AE6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF6" s="5"/>
       <c r="AG6" s="5"/>
       <c r="AH6" s="5"/>
-      <c r="AI6" s="5"/>
-    </row>
-    <row r="7" spans="1:35">
+    </row>
+    <row r="7" spans="1:34">
       <c r="A7" s="15">
         <v>105</v>
       </c>
@@ -2235,94 +2235,93 @@
         <v>3</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="15">
         <v>53704</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J7" s="6"/>
       <c r="K7" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L7" s="6"/>
       <c r="M7" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="R7" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="S7" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="T7" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="U7" s="6" t="s">
         <v>80</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="P7" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q7" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="R7" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="S7" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="T7" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="U7" s="6" t="s">
-        <v>79</v>
       </c>
       <c r="V7" s="6"/>
       <c r="W7" s="25" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="X7" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Y7" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="Z7" s="5" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="AA7" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AB7" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AC7" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AD7" s="5"/>
-      <c r="AE7" s="5"/>
+      <c r="AE7" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="AF7" s="5" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="AG7" s="5" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="AH7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI7" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34">
       <c r="A8" s="18">
         <v>107</v>
       </c>
@@ -2330,58 +2329,55 @@
         <v>3</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F8" s="15">
         <v>53704</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="P8" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q8" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="R8" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="T8" s="6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="W8" s="25" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="X8" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Y8" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="Z8" s="5" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="AA8" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AB8" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AD8" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE8" s="20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:35" ht="13.5" customHeight="1">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" ht="13.5" customHeight="1">
       <c r="A9" s="22">
         <v>106</v>
       </c>
@@ -2390,7 +2386,7 @@
       </c>
       <c r="C9" s="22"/>
       <c r="D9" s="22" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E9" s="22"/>
       <c r="F9" s="22">
@@ -2398,69 +2394,66 @@
       </c>
       <c r="G9" s="22"/>
       <c r="H9" s="22" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I9" s="22"/>
       <c r="J9" s="22"/>
       <c r="K9" s="22" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L9" s="22"/>
       <c r="M9" s="22"/>
       <c r="N9" s="22" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="O9" s="22"/>
       <c r="P9" s="22" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q9" s="22" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="R9" s="22" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="S9" s="22"/>
       <c r="T9" s="22" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="U9" s="22"/>
       <c r="V9" s="22"/>
       <c r="W9" s="26" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="X9" s="22" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="Y9" s="22" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="Z9" s="22" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="AA9" s="22" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AB9" s="22" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AC9" s="22"/>
       <c r="AD9" s="22" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="AE9" s="22" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="AF9" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG9" s="22" t="s">
-        <v>5</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="AG9" s="1"/>
       <c r="AH9" s="1"/>
-      <c r="AI9" s="1"/>
-    </row>
-    <row r="10" spans="1:35" ht="13.5" customHeight="1">
+    </row>
+    <row r="10" spans="1:34" ht="13.5" customHeight="1">
       <c r="A10" s="22">
         <v>109</v>
       </c>
@@ -2469,7 +2462,7 @@
       </c>
       <c r="C10" s="22"/>
       <c r="D10" s="22" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E10" s="22"/>
       <c r="F10" s="22">
@@ -2477,69 +2470,66 @@
       </c>
       <c r="G10" s="22"/>
       <c r="H10" s="22" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I10" s="22"/>
       <c r="J10" s="22"/>
       <c r="K10" s="22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L10" s="22"/>
       <c r="M10" s="22"/>
       <c r="N10" s="22" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="O10" s="22"/>
       <c r="P10" s="22" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q10" s="22" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="R10" s="22" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="S10" s="22"/>
       <c r="T10" s="22" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="U10" s="22"/>
       <c r="V10" s="22" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="W10" s="26" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="X10" s="22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Y10" s="22" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="Z10" s="22" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="AA10" s="22" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AB10" s="22" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AC10" s="22"/>
       <c r="AD10" s="22" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="AE10" s="22" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="AF10" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG10" s="22" t="s">
-        <v>5</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="AG10" s="1"/>
       <c r="AH10" s="1"/>
-      <c r="AI10" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -2581,13 +2571,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2598,13 +2588,13 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -2616,7 +2606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
@@ -2643,34 +2633,34 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="L1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="14.25" customHeight="1">
@@ -2681,34 +2671,34 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="L2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -2737,7 +2727,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2748,7 +2738,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2759,7 +2749,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2770,7 +2760,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified exceptional handling and test data for no code branch
</commit_message>
<xml_diff>
--- a/resources/test_data/VM_TestData_Sample1.xlsx
+++ b/resources/test_data/VM_TestData_Sample1.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22410"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\praneethm\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\praneethm\git\VMSeleniumFramework\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{11AB9E4E-DF5C-4F03-A346-F783E06B7410}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="2055" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="2055"/>
   </bookViews>
   <sheets>
     <sheet name="LogInPage" sheetId="22" r:id="rId1"/>
@@ -33,7 +32,7 @@
     <definedName name="State">[1]Selectlists!$C$2:$C$52</definedName>
     <definedName name="waivsub">[1]Selectlists!$J$2:$J$6</definedName>
   </definedNames>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -51,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="228">
   <si>
     <t>TestCaseNumber</t>
   </si>
@@ -703,16 +702,52 @@
   </si>
   <si>
     <t>Submit</t>
+  </si>
+  <si>
+    <t>//a[@ng-click=\"CustomerAndPolicySearch()\"]</t>
+  </si>
+  <si>
+    <t>//button[@class=\"btn btn-success pull-right\"]</t>
+  </si>
+  <si>
+    <t>//input[@id='PrimaryAccountState']</t>
+  </si>
+  <si>
+    <t>//input[@id='IDphysical_aptsuit']</t>
+  </si>
+  <si>
+    <t>//span[contains(text(),'SSN')]</t>
+  </si>
+  <si>
+    <t>//span[contains(text(),'FEIN')]</t>
+  </si>
+  <si>
+    <t>//*[@id='IdfeinNumber']</t>
+  </si>
+  <si>
+    <t>//input[@ng-model='CustomerSearchCriteria.AccountName']</t>
+  </si>
+  <si>
+    <t>//button[@ng-click=\"customerSearch();\"]</t>
+  </si>
+  <si>
+    <t>(//a[@class='vam-table-tdArrow'])[2]</t>
+  </si>
+  <si>
+    <t>//li[@ng-click=\"setCustomerAccountDetailsTab('submissions')\"]</t>
+  </si>
+  <si>
+    <t>//a[@ng-click=\"CreateNewSubmission()\"]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1023,7 +1058,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -1688,14 +1723,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.5703125" customWidth="1"/>
@@ -1709,7 +1744,7 @@
     <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1741,7 +1776,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
@@ -1763,7 +1798,7 @@
       </c>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="23">
         <v>101</v>
       </c>
@@ -1787,7 +1822,7 @@
       </c>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="23">
         <v>102</v>
       </c>
@@ -1811,7 +1846,7 @@
       </c>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="23">
         <v>103</v>
       </c>
@@ -1835,7 +1870,7 @@
       </c>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="24">
         <v>104</v>
       </c>
@@ -1859,7 +1894,7 @@
       </c>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="24">
         <v>105</v>
       </c>
@@ -1883,7 +1918,7 @@
       </c>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="24">
         <v>107</v>
       </c>
@@ -1905,7 +1940,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="24">
         <v>108</v>
       </c>
@@ -1929,7 +1964,7 @@
       </c>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="24">
         <v>106</v>
       </c>
@@ -1953,7 +1988,7 @@
       </c>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="24">
         <v>109</v>
       </c>
@@ -1977,7 +2012,7 @@
       </c>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="24">
         <v>110</v>
       </c>
@@ -2008,24 +2043,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="32" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.42578125" customWidth="1"/>
     <col min="5" max="5" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2048,7 +2083,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -2060,9 +2095,12 @@
       <c r="E2" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="F2" t="s">
+        <v>216</v>
+      </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>101</v>
       </c>
@@ -2077,7 +2115,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>102</v>
       </c>
@@ -2090,7 +2128,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>103</v>
       </c>
@@ -2103,7 +2141,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>103</v>
       </c>
@@ -2117,7 +2155,7 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>104</v>
       </c>
@@ -2131,7 +2169,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>105</v>
       </c>
@@ -2142,7 +2180,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>107</v>
       </c>
@@ -2153,7 +2191,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>108</v>
       </c>
@@ -2164,7 +2202,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>106</v>
       </c>
@@ -2175,7 +2213,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>109</v>
       </c>
@@ -2186,7 +2224,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>110</v>
       </c>
@@ -2197,7 +2235,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
     </row>
@@ -2207,23 +2245,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH13"/>
   <sheetViews>
-    <sheetView topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AJ2" sqref="AJ2"/>
+    <sheetView topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AD17" sqref="AD17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.28515625" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="49.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="9" customWidth="1"/>
+    <col min="8" max="8" width="27.7109375" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5.28515625" customWidth="1"/>
@@ -2237,7 +2275,7 @@
     <col min="19" max="19" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.5703125" customWidth="1"/>
     <col min="23" max="23" width="16.42578125" customWidth="1"/>
     <col min="24" max="24" width="23.5703125" customWidth="1"/>
     <col min="25" max="25" width="20" bestFit="1" customWidth="1"/>
@@ -2249,7 +2287,7 @@
     <col min="34" max="34" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2353,34 +2391,46 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:34">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="14"/>
-      <c r="D2" s="4"/>
+      <c r="D2" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="E2" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F2" s="4"/>
+      <c r="F2" s="4" t="s">
+        <v>217</v>
+      </c>
       <c r="G2" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="H2" s="4"/>
+      <c r="H2" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="I2" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="J2" s="4"/>
+      <c r="J2" s="4" t="s">
+        <v>218</v>
+      </c>
       <c r="K2" s="4"/>
       <c r="L2" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="M2" s="4"/>
+      <c r="M2" s="4" t="s">
+        <v>219</v>
+      </c>
       <c r="N2" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="O2" s="4"/>
+      <c r="O2" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="P2" s="4" t="s">
         <v>65</v>
       </c>
@@ -2390,12 +2440,18 @@
       <c r="R2" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="S2" s="4"/>
+      <c r="S2" s="4" t="s">
+        <v>220</v>
+      </c>
       <c r="T2" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="U2" s="4"/>
-      <c r="V2" s="12"/>
+      <c r="U2" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="V2" s="12" t="s">
+        <v>222</v>
+      </c>
       <c r="W2" s="4" t="s">
         <v>69</v>
       </c>
@@ -2414,7 +2470,9 @@
       <c r="AB2" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="AC2" s="4"/>
+      <c r="AC2" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="AD2" s="16"/>
       <c r="AE2" s="4" t="s">
         <v>75</v>
@@ -2429,7 +2487,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:34">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>101</v>
       </c>
@@ -2507,7 +2565,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:34">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>102</v>
       </c>
@@ -2587,7 +2645,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:34">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>103</v>
       </c>
@@ -2665,7 +2723,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:34">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>103</v>
       </c>
@@ -2745,7 +2803,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:34">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>104</v>
       </c>
@@ -2799,7 +2857,7 @@
       <c r="AG7" s="4"/>
       <c r="AH7" s="4"/>
     </row>
-    <row r="8" spans="1:34">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>105</v>
       </c>
@@ -2891,7 +2949,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:34">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>107</v>
       </c>
@@ -2948,7 +3006,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:34" ht="13.5" customHeight="1">
+    <row r="10" spans="1:34" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18">
         <v>106</v>
       </c>
@@ -3022,7 +3080,7 @@
       <c r="AG10" s="1"/>
       <c r="AH10" s="1"/>
     </row>
-    <row r="11" spans="1:34" ht="13.5" customHeight="1">
+    <row r="11" spans="1:34" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18">
         <v>109</v>
       </c>
@@ -3098,7 +3156,7 @@
       <c r="AG11" s="1"/>
       <c r="AH11" s="1"/>
     </row>
-    <row r="12" spans="1:34">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="22">
         <v>108</v>
       </c>
@@ -3175,7 +3233,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:34">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="22">
         <v>110</v>
       </c>
@@ -3189,16 +3247,16 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="G4:J4 L4 Q4 W3:X6 G6:J6 L6 Q6 W12:X12" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="G4:J4 L4 Q4 W3:X6 G6:J6 L6 Q6 W12:X12"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G4" r:id="rId1" display="random123@gmail.com" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="I4" r:id="rId2" display="random123@gmail.com" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="X3" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="X5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="G6" r:id="rId5" display="random123@gmail.com" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
-    <hyperlink ref="I6" r:id="rId6" display="random123@gmail.com" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
-    <hyperlink ref="X12" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="G4" r:id="rId1" display="random123@gmail.com"/>
+    <hyperlink ref="I4" r:id="rId2" display="random123@gmail.com"/>
+    <hyperlink ref="X3" r:id="rId3"/>
+    <hyperlink ref="X5" r:id="rId4"/>
+    <hyperlink ref="G6" r:id="rId5" display="random123@gmail.com"/>
+    <hyperlink ref="I6" r:id="rId6" display="random123@gmail.com"/>
+    <hyperlink ref="X12" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
@@ -3206,21 +3264,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.28515625" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3237,20 +3295,34 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>104</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B3" s="1">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>78</v>
       </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3260,14 +3332,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:L2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
@@ -3282,7 +3354,7 @@
     <col min="12" max="12" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3320,41 +3392,52 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A2" s="1">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" t="s">
+        <v>226</v>
+      </c>
+      <c r="L2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>104</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B3" s="1">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>128</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
         <v>129</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F3" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G3" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H3" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I3" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J3" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="K2" t="s">
-        <v>5</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="K3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3364,14 +3447,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A101A3F-5E55-48C4-A581-5C9FEB4521BA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" customWidth="1"/>
@@ -3412,7 +3495,7 @@
     <col min="38" max="38" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
@@ -3528,7 +3611,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:38">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>9</v>
       </c>
@@ -3642,7 +3725,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="3" spans="1:38">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="30">
         <v>112</v>
       </c>
@@ -3691,7 +3774,7 @@
       <c r="AK3" s="37"/>
       <c r="AL3" s="38"/>
     </row>
-    <row r="4" spans="1:38">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>113</v>
       </c>
@@ -3803,26 +3886,26 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J4" r:id="rId1" xr:uid="{41FC0B67-1D6A-4701-83A0-CB716B0700BA}"/>
+    <hyperlink ref="J4" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3833,7 +3916,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -3842,7 +3925,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>101</v>
       </c>
@@ -3853,7 +3936,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>102</v>
       </c>
@@ -3864,7 +3947,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>103</v>
       </c>
@@ -3881,19 +3964,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3907,7 +3990,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>111</v>
       </c>

</xml_diff>

<commit_message>
updated test data for 101,102,103 and code
</commit_message>
<xml_diff>
--- a/resources/test_data/VM_TestData_Sample1.xlsx
+++ b/resources/test_data/VM_TestData_Sample1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="2055"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="2055" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="LogInPage" sheetId="22" r:id="rId1"/>
@@ -18,8 +18,8 @@
     <sheet name="ServicePolicy" sheetId="26" r:id="rId4"/>
     <sheet name="CustomerInformationPage" sheetId="27" r:id="rId5"/>
     <sheet name="PracticeAutomationPage" sheetId="29" r:id="rId6"/>
-    <sheet name="SubmissionSummaryPage" sheetId="25" r:id="rId7"/>
-    <sheet name="Iframepage" sheetId="28" r:id="rId8"/>
+    <sheet name="Iframepage" sheetId="28" r:id="rId7"/>
+    <sheet name="SubmissionSummaryPage" sheetId="25" r:id="rId8"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId9"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="215">
   <si>
     <t>TestCaseNumber</t>
   </si>
@@ -280,12 +280,6 @@
     <t>//*[@ng-click='accountproceed()']</t>
   </si>
   <si>
-    <t>//input[@name=\"Duplicate\"]</t>
-  </si>
-  <si>
-    <t>//*[@id=\"existingAccountpopup\"]/div/div/div[3]/button</t>
-  </si>
-  <si>
     <t>Jack</t>
   </si>
   <si>
@@ -406,58 +400,12 @@
     <t>Actions</t>
   </si>
   <si>
-    <t>VerifyCustomerAccountID</t>
-  </si>
-  <si>
-    <t>VerifyCustomerSince</t>
-  </si>
-  <si>
-    <t>VerifySSN</t>
-  </si>
-  <si>
-    <t>VerifyPhone</t>
-  </si>
-  <si>
-    <t>VerifyEmailID</t>
-  </si>
-  <si>
-    <t>VerifyPhysicalAddress</t>
-  </si>
-  <si>
-    <t>VerifyMailingAddress</t>
-  </si>
-  <si>
     <t>Submissions</t>
   </si>
   <si>
     <t>AddNewSubmission</t>
   </si>
   <si>
-    <t>AreEqual&gt;ACC0000212</t>
-  </si>
-  <si>
-    <t>AreEqual&gt;09/04/2019</t>
-  </si>
-  <si>
-    <t>AreEqual&gt;Individual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AreEqual&gt;65-4987879
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AreEqual&gt;(654) 987 - 9798
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AreEqual&gt;jack@gmail.com
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AreEqual&gt;123 New Street, Madison, WI- 53704
-</t>
-  </si>
-  <si>
     <t>uid</t>
   </si>
   <si>
@@ -704,9 +652,6 @@
     <t>Submit</t>
   </si>
   <si>
-    <t>//a[@ng-click=\"CustomerAndPolicySearch()\"]</t>
-  </si>
-  <si>
     <t>//button[@class=\"btn btn-success pull-right\"]</t>
   </si>
   <si>
@@ -728,16 +673,28 @@
     <t>//input[@ng-model='CustomerSearchCriteria.AccountName']</t>
   </si>
   <si>
-    <t>//button[@ng-click=\"customerSearch();\"]</t>
-  </si>
-  <si>
     <t>(//a[@class='vam-table-tdArrow'])[2]</t>
   </si>
   <si>
-    <t>//li[@ng-click=\"setCustomerAccountDetailsTab('submissions')\"]</t>
-  </si>
-  <si>
-    <t>//a[@ng-click=\"CreateNewSubmission()\"]</t>
+    <t>//input[@value=2]</t>
+  </si>
+  <si>
+    <t>//*[@id="existingAccountpopup"]/div/div/div[3]/button</t>
+  </si>
+  <si>
+    <t>(121)212-1213</t>
+  </si>
+  <si>
+    <t>//a[@ng-click="CustomerAndPolicySearch()"]</t>
+  </si>
+  <si>
+    <t>//*[@id="div1"]/div/button</t>
+  </si>
+  <si>
+    <t>//*[@id="submissionsTab"]</t>
+  </si>
+  <si>
+    <t>//*[@ng-click="CreateNewSubmission()"]</t>
   </si>
 </sst>
 </file>
@@ -1726,8 +1683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2096,7 +2053,7 @@
         <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="G2" s="1"/>
     </row>
@@ -2248,8 +2205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH13"/>
   <sheetViews>
-    <sheetView topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AD17" sqref="AD17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AC7" sqref="AC7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2404,7 +2361,7 @@
         <v>60</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>61</v>
@@ -2416,14 +2373,14 @@
         <v>62</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
       <c r="K2" s="4"/>
       <c r="L2" s="4" t="s">
         <v>63</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>219</v>
+        <v>202</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>64</v>
@@ -2441,16 +2398,16 @@
         <v>67</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
       <c r="T2" s="4" t="s">
         <v>68</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>221</v>
+        <v>204</v>
       </c>
       <c r="V2" s="12" t="s">
-        <v>222</v>
+        <v>205</v>
       </c>
       <c r="W2" s="4" t="s">
         <v>69</v>
@@ -2478,10 +2435,10 @@
         <v>75</v>
       </c>
       <c r="AF2" s="5" t="s">
-        <v>76</v>
+        <v>208</v>
       </c>
       <c r="AG2" s="5" t="s">
-        <v>77</v>
+        <v>209</v>
       </c>
       <c r="AH2" s="4" t="s">
         <v>75</v>
@@ -2497,7 +2454,7 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4">
@@ -2505,12 +2462,12 @@
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="M3" s="4"/>
       <c r="N3" s="4" t="s">
@@ -2518,37 +2475,37 @@
       </c>
       <c r="O3" s="4"/>
       <c r="P3" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="R3" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="R3" s="6" t="s">
-        <v>83</v>
       </c>
       <c r="S3" s="6"/>
       <c r="T3" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="U3" s="6"/>
       <c r="V3" s="6"/>
       <c r="W3" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="X3" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y3" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="X3" s="8" t="s">
+      <c r="Z3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA3" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="Y3" s="4" t="s">
+      <c r="AB3" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="Z3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA3" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="AB3" s="4" t="s">
-        <v>89</v>
       </c>
       <c r="AC3" s="4"/>
       <c r="AD3" s="4"/>
@@ -2575,60 +2532,60 @@
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H4" s="10"/>
       <c r="I4" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J4" s="10"/>
       <c r="K4" s="4"/>
       <c r="L4" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="O4" s="4"/>
       <c r="P4" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="R4" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="S4" s="6"/>
       <c r="T4" s="6" t="s">
-        <v>84</v>
+        <v>107</v>
       </c>
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
       <c r="W4" s="19" t="s">
+        <v>210</v>
+      </c>
+      <c r="X4" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y4" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="X4" s="7" t="s">
+      <c r="Z4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA4" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB4" s="4" t="s">
         <v>98</v>
-      </c>
-      <c r="Y4" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="Z4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA4" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="AB4" s="4" t="s">
-        <v>100</v>
       </c>
       <c r="AC4" s="4"/>
       <c r="AD4" s="4"/>
@@ -2655,7 +2612,7 @@
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4">
@@ -2663,12 +2620,12 @@
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="M5" s="4"/>
       <c r="N5" s="4" t="s">
@@ -2676,37 +2633,37 @@
       </c>
       <c r="O5" s="4"/>
       <c r="P5" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="R5" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="Q5" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="R5" s="6" t="s">
-        <v>83</v>
       </c>
       <c r="S5" s="6"/>
       <c r="T5" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="U5" s="6"/>
       <c r="V5" s="6"/>
       <c r="W5" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="X5" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y5" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="X5" s="8" t="s">
+      <c r="Z5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA5" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="Y5" s="4" t="s">
+      <c r="AB5" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="Z5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA5" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="AB5" s="4" t="s">
-        <v>89</v>
       </c>
       <c r="AC5" s="4"/>
       <c r="AD5" s="4"/>
@@ -2733,60 +2690,60 @@
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H6" s="10"/>
       <c r="I6" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J6" s="10"/>
       <c r="K6" s="4"/>
       <c r="L6" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="N6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="O6" s="4"/>
       <c r="P6" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="R6" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="S6" s="6"/>
       <c r="T6" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
       <c r="W6" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="X6" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y6" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="X6" s="7" t="s">
+      <c r="Z6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA6" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB6" s="4" t="s">
         <v>98</v>
-      </c>
-      <c r="Y6" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="Z6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA6" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="AB6" s="4" t="s">
-        <v>100</v>
       </c>
       <c r="AC6" s="4"/>
       <c r="AD6" s="4"/>
@@ -2813,7 +2770,7 @@
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
       <c r="E7" s="13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>5</v>
@@ -2837,16 +2794,16 @@
       <c r="W7" s="20"/>
       <c r="X7" s="5"/>
       <c r="Y7" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA7" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB7" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="Z7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA7" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="AB7" s="4" t="s">
-        <v>89</v>
       </c>
       <c r="AC7" s="4"/>
       <c r="AD7" s="4"/>
@@ -2866,74 +2823,74 @@
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="13">
         <v>53704</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="M8" s="5"/>
       <c r="N8" s="5" t="s">
         <v>5</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="P8" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q8" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="R8" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="Q8" s="5" t="s">
+      <c r="S8" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="T8" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="R8" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="S8" s="5" t="s">
+      <c r="U8" s="5" t="s">
         <v>102</v>
-      </c>
-      <c r="T8" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="U8" s="5" t="s">
-        <v>104</v>
       </c>
       <c r="V8" s="5"/>
       <c r="W8" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="X8" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y8" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="X8" s="5" t="s">
+      <c r="Z8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA8" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="Y8" s="4" t="s">
+      <c r="AB8" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="Z8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA8" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="AB8" s="4" t="s">
-        <v>89</v>
-      </c>
       <c r="AC8" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="AD8" s="4"/>
       <c r="AE8" s="4" t="s">
@@ -2958,49 +2915,49 @@
       </c>
       <c r="C9" s="22"/>
       <c r="E9" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G9" s="13">
         <v>53704</v>
       </c>
       <c r="I9" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P9" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="Q9" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="R9" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="T9" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="N9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="P9" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q9" s="5" t="s">
+      <c r="W9" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="R9" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="T9" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="W9" s="20" t="s">
-        <v>110</v>
-      </c>
       <c r="X9" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y9" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA9" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="Y9" s="4" t="s">
+      <c r="AB9" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="Z9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA9" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="AB9" s="4" t="s">
-        <v>89</v>
       </c>
       <c r="AD9" s="17" t="s">
         <v>18</v>
@@ -3016,7 +2973,7 @@
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
       <c r="E10" s="18" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F10" s="18"/>
       <c r="G10" s="18">
@@ -3024,12 +2981,12 @@
       </c>
       <c r="H10" s="18"/>
       <c r="I10" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J10" s="18"/>
       <c r="K10" s="18"/>
       <c r="L10" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M10" s="18"/>
       <c r="N10" s="18" t="s">
@@ -3037,37 +2994,37 @@
       </c>
       <c r="O10" s="18"/>
       <c r="P10" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q10" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="R10" s="18" t="s">
         <v>81</v>
-      </c>
-      <c r="Q10" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="R10" s="18" t="s">
-        <v>83</v>
       </c>
       <c r="S10" s="18"/>
       <c r="T10" s="18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="U10" s="18"/>
       <c r="V10" s="18"/>
       <c r="W10" s="21" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="X10" s="18" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="Y10" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z10" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA10" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB10" s="18" t="s">
         <v>87</v>
-      </c>
-      <c r="Z10" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA10" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="AB10" s="18" t="s">
-        <v>89</v>
       </c>
       <c r="AC10" s="18"/>
       <c r="AD10" s="18"/>
@@ -3090,7 +3047,7 @@
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
       <c r="E11" s="18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F11" s="18"/>
       <c r="G11" s="18">
@@ -3098,12 +3055,12 @@
       </c>
       <c r="H11" s="18"/>
       <c r="I11" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J11" s="18"/>
       <c r="K11" s="18"/>
       <c r="L11" s="18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="M11" s="18"/>
       <c r="N11" s="18" t="s">
@@ -3111,39 +3068,39 @@
       </c>
       <c r="O11" s="18"/>
       <c r="P11" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q11" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="R11" s="18" t="s">
         <v>81</v>
-      </c>
-      <c r="Q11" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="R11" s="18" t="s">
-        <v>83</v>
       </c>
       <c r="S11" s="18"/>
       <c r="T11" s="18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="U11" s="18"/>
       <c r="V11" s="18" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="W11" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="X11" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y11" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="X11" s="18" t="s">
+      <c r="Z11" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA11" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="Y11" s="18" t="s">
+      <c r="AB11" s="18" t="s">
         <v>87</v>
-      </c>
-      <c r="Z11" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA11" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="AB11" s="18" t="s">
-        <v>89</v>
       </c>
       <c r="AC11" s="18"/>
       <c r="AD11" s="18"/>
@@ -3166,7 +3123,7 @@
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4">
@@ -3174,49 +3131,49 @@
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="M12" s="4"/>
       <c r="N12" s="4" t="s">
         <v>5</v>
       </c>
       <c r="P12" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="R12" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="Q12" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="R12" s="6" t="s">
-        <v>83</v>
       </c>
       <c r="S12" s="6"/>
       <c r="T12" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="U12" s="6"/>
       <c r="V12" s="6"/>
       <c r="W12" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="X12" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y12" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="X12" s="8" t="s">
+      <c r="Z12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA12" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="Y12" s="4" t="s">
+      <c r="AB12" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="Z12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA12" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="AB12" s="4" t="s">
-        <v>89</v>
       </c>
       <c r="AC12" s="4"/>
       <c r="AD12" s="4"/>
@@ -3242,7 +3199,7 @@
       </c>
       <c r="C13" s="4"/>
       <c r="E13" s="22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -3268,7 +3225,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3289,10 +3246,10 @@
         <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -3300,13 +3257,13 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>223</v>
+        <v>206</v>
       </c>
       <c r="D2" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="E2" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -3317,7 +3274,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -3333,10 +3290,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3354,7 +3311,7 @@
     <col min="12" max="12" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3362,84 +3319,41 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G1" t="s">
-        <v>121</v>
-      </c>
-      <c r="H1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I1" t="s">
-        <v>123</v>
-      </c>
-      <c r="J1" t="s">
-        <v>124</v>
-      </c>
-      <c r="K1" t="s">
-        <v>125</v>
-      </c>
-      <c r="L1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K2" t="s">
-        <v>226</v>
-      </c>
-      <c r="L2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>104</v>
       </c>
       <c r="B3" s="1">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>127</v>
+      <c r="C3" t="s">
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E3" t="s">
-        <v>129</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="K3" t="s">
-        <v>5</v>
-      </c>
-      <c r="L3" t="s">
-        <v>5</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3503,112 +3417,112 @@
         <v>1</v>
       </c>
       <c r="C1" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="I1" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="J1" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="K1" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="L1" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="M1" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="N1" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="O1" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="P1" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q1" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="R1" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="S1" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="T1" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="U1" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="V1" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="W1" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="X1" s="34" t="s">
         <v>139</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="Y1" s="34" t="s">
         <v>140</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="Z1" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="K1" s="28" t="s">
+      <c r="AA1" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="L1" s="31" t="s">
+      <c r="AB1" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="M1" s="34" t="s">
+      <c r="AC1" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="N1" s="34" t="s">
+      <c r="AD1" s="34" t="s">
         <v>145</v>
       </c>
-      <c r="O1" s="34" t="s">
+      <c r="AE1" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="P1" s="34" t="s">
+      <c r="AF1" s="34" t="s">
         <v>147</v>
       </c>
-      <c r="Q1" s="34" t="s">
+      <c r="AG1" s="34" t="s">
         <v>148</v>
       </c>
-      <c r="R1" s="34" t="s">
+      <c r="AH1" s="34" t="s">
         <v>149</v>
       </c>
-      <c r="S1" s="34" t="s">
+      <c r="AI1" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="T1" s="34" t="s">
+      <c r="AJ1" s="34" t="s">
         <v>151</v>
       </c>
-      <c r="U1" s="34" t="s">
+      <c r="AK1" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="V1" s="34" t="s">
+      <c r="AL1" s="31" t="s">
         <v>153</v>
-      </c>
-      <c r="W1" s="34" t="s">
-        <v>154</v>
-      </c>
-      <c r="X1" s="34" t="s">
-        <v>155</v>
-      </c>
-      <c r="Y1" s="34" t="s">
-        <v>156</v>
-      </c>
-      <c r="Z1" s="34" t="s">
-        <v>157</v>
-      </c>
-      <c r="AA1" s="34" t="s">
-        <v>158</v>
-      </c>
-      <c r="AB1" s="34" t="s">
-        <v>159</v>
-      </c>
-      <c r="AC1" s="34" t="s">
-        <v>160</v>
-      </c>
-      <c r="AD1" s="34" t="s">
-        <v>161</v>
-      </c>
-      <c r="AE1" s="34" t="s">
-        <v>162</v>
-      </c>
-      <c r="AF1" s="34" t="s">
-        <v>163</v>
-      </c>
-      <c r="AG1" s="34" t="s">
-        <v>164</v>
-      </c>
-      <c r="AH1" s="34" t="s">
-        <v>165</v>
-      </c>
-      <c r="AI1" s="34" t="s">
-        <v>166</v>
-      </c>
-      <c r="AJ1" s="34" t="s">
-        <v>167</v>
-      </c>
-      <c r="AK1" s="34" t="s">
-        <v>168</v>
-      </c>
-      <c r="AL1" s="31" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
@@ -3617,112 +3531,112 @@
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="M2" s="5" t="s">
         <v>12</v>
       </c>
       <c r="N2" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="W2" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="X2" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="Y2" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="Z2" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="AA2" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="AB2" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="AC2" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="AD2" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="AE2" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="O2" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="P2" s="5" t="s">
+      <c r="AF2" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="AG2" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="AH2" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="AI2" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="AJ2" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="AK2" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="AL2" s="5" t="s">
         <v>187</v>
-      </c>
-      <c r="W2" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="X2" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="Y2" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="Z2" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="AA2" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="AB2" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="AC2" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="AD2" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="AE2" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="AF2" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="AG2" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="AH2" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="AI2" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="AJ2" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="AK2" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="AL2" s="5" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
@@ -3733,13 +3647,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="D3" s="36" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="E3" s="36" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="F3" s="16"/>
       <c r="H3" s="37"/>
@@ -3785,31 +3699,31 @@
       <c r="D4" s="5"/>
       <c r="E4" s="29"/>
       <c r="F4" s="29" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="G4" s="32" t="s">
-        <v>208</v>
+        <v>192</v>
       </c>
       <c r="H4" s="29" t="s">
-        <v>209</v>
+        <v>193</v>
       </c>
       <c r="I4" s="32">
         <v>3</v>
       </c>
       <c r="J4" s="33" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="K4" s="29" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="L4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="M4" s="29" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="N4" s="29" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="O4" s="29" t="s">
         <v>5</v>
@@ -3893,6 +3807,52 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>111</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -3913,7 +3873,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3922,7 +3882,7 @@
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3933,7 +3893,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3944,7 +3904,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3955,53 +3915,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>206</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>214</v>
-      </c>
-      <c r="D1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>111</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update for the Task 96
</commit_message>
<xml_diff>
--- a/resources/test_data/VM_TestData_Sample1.xlsx
+++ b/resources/test_data/VM_TestData_Sample1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\praneethm\git\VMSeleniumFramework\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB668017-213A-4EDB-AFEF-04A2EF534A24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{FB668017-213A-4EDB-AFEF-04A2EF534A24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{77CF52C2-2C3D-4786-9BA6-19BE29884707}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="2055" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="2055" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LogInPage" sheetId="22" r:id="rId1"/>
@@ -33,7 +33,7 @@
     <definedName name="State">[1]Selectlists!$C$2:$C$52</definedName>
     <definedName name="waivsub">[1]Selectlists!$J$2:$J$6</definedName>
   </definedNames>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="223">
   <si>
     <t>TestCaseNumber</t>
   </si>
@@ -86,9 +86,6 @@
     <t>Xpath</t>
   </si>
   <si>
-    <t>//*[@id='UserName']</t>
-  </si>
-  <si>
     <t>//*[@id='UserName']//following::button</t>
   </si>
   <si>
@@ -711,6 +708,12 @@
   </si>
   <si>
     <t>//*[@class='btn btn-blue']</t>
+  </si>
+  <si>
+    <t>Selector</t>
+  </si>
+  <si>
+    <t>id=UserName</t>
   </si>
 </sst>
 </file>
@@ -720,7 +723,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1713,25 +1716,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5703125" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="5" max="5" width="38.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.41015625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.58984375" customWidth="1"/>
+    <col min="3" max="3" width="20.3125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" customWidth="1"/>
+    <col min="5" max="5" width="38.3359375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.64453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.37109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37.26171875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1763,101 +1766,101 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>10</v>
+        <v>219</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5" t="s">
-        <v>11</v>
+        <v>220</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="23">
         <v>101</v>
       </c>
       <c r="B3" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="23">
         <v>102</v>
       </c>
       <c r="B4" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="23">
         <v>103</v>
       </c>
       <c r="B5" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="24">
         <v>104</v>
       </c>
@@ -1865,23 +1868,23 @@
         <v>1</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="24">
         <v>105</v>
       </c>
@@ -1889,23 +1892,23 @@
         <v>1</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H7" s="25"/>
       <c r="I7" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="24">
         <v>107</v>
       </c>
@@ -1913,23 +1916,23 @@
         <v>1</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="26" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="24">
         <v>108</v>
       </c>
@@ -1937,23 +1940,23 @@
         <v>1</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H9" s="5"/>
       <c r="I9" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="24">
         <v>106</v>
       </c>
@@ -1961,23 +1964,23 @@
         <v>1</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="24">
         <v>109</v>
       </c>
@@ -1985,23 +1988,23 @@
         <v>1</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="24">
         <v>110</v>
       </c>
@@ -2009,19 +2012,19 @@
         <v>1</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J12" s="5"/>
     </row>
@@ -2035,21 +2038,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="32" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" customWidth="1"/>
-    <col min="5" max="5" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.41015625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.41015625" customWidth="1"/>
+    <col min="3" max="3" width="32.015625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.48046875" customWidth="1"/>
+    <col min="5" max="5" width="38.203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.98828125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2057,39 +2058,39 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
         <v>27</v>
       </c>
-      <c r="F2" t="s">
-        <v>28</v>
-      </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>101</v>
       </c>
@@ -2097,14 +2098,14 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>102</v>
       </c>
@@ -2114,10 +2115,10 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>103</v>
       </c>
@@ -2127,10 +2128,10 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>103</v>
       </c>
@@ -2140,11 +2141,11 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>104</v>
       </c>
@@ -2155,10 +2156,10 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>105</v>
       </c>
@@ -2166,10 +2167,10 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>107</v>
       </c>
@@ -2177,10 +2178,10 @@
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>108</v>
       </c>
@@ -2188,10 +2189,10 @@
         <v>2</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>106</v>
       </c>
@@ -2199,10 +2200,10 @@
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>109</v>
       </c>
@@ -2210,10 +2211,10 @@
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>110</v>
       </c>
@@ -2221,10 +2222,10 @@
         <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="F14" s="1"/>
@@ -2238,46 +2239,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AI13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" customWidth="1"/>
-    <col min="7" max="7" width="9" customWidth="1"/>
+    <col min="1" max="1" width="16.41015625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.24609375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.125" customWidth="1"/>
+    <col min="4" max="4" width="22.46484375" customWidth="1"/>
+    <col min="5" max="5" width="9.4140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.1015625" customWidth="1"/>
+    <col min="7" max="7" width="9.01171875" customWidth="1"/>
     <col min="8" max="8" width="27.7109375" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5078125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.28515625" customWidth="1"/>
-    <col min="12" max="12" width="28" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="38.28515625" customWidth="1"/>
-    <col min="18" max="18" width="19.7109375" customWidth="1"/>
-    <col min="19" max="19" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.24609375" customWidth="1"/>
+    <col min="12" max="12" width="27.98046875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.8359375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.7890625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29.59375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="38.3359375" customWidth="1"/>
+    <col min="18" max="18" width="19.7734375" customWidth="1"/>
+    <col min="19" max="19" width="13.31640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.43359375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.5703125" customWidth="1"/>
-    <col min="23" max="23" width="16.42578125" customWidth="1"/>
-    <col min="24" max="24" width="23.5703125" customWidth="1"/>
-    <col min="25" max="25" width="20" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="21.28515625" customWidth="1"/>
-    <col min="28" max="30" width="22.85546875" customWidth="1"/>
-    <col min="31" max="32" width="15.5703125" customWidth="1"/>
-    <col min="34" max="34" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.5078125" customWidth="1"/>
+    <col min="23" max="23" width="16.41015625" customWidth="1"/>
+    <col min="24" max="24" width="23.5390625" customWidth="1"/>
+    <col min="25" max="25" width="20.04296875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.0078125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="21.25390625" customWidth="1"/>
+    <col min="28" max="30" width="22.8671875" customWidth="1"/>
+    <col min="31" max="32" width="15.6015625" customWidth="1"/>
+    <col min="34" max="34" width="17.62109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="18.4296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2285,205 +2284,205 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="F1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="V1" s="12" t="s">
+      <c r="W1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AD1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AF1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="AF1" s="5" t="s">
+      <c r="AG1" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="AG1" s="5" t="s">
+      <c r="AH1" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="AH1" s="5" t="s">
+      <c r="AI1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="AI1" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35">
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E2" s="14"/>
       <c r="F2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>68</v>
       </c>
       <c r="K2" s="4"/>
       <c r="L2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q2" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="P2" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q2" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="T2" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="U2" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="V2" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="V2" s="12" t="s">
+      <c r="W2" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="X2" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="Y2" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Z2" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="AA2" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AB2" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AC2" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="AC2" s="4" t="s">
-        <v>85</v>
       </c>
       <c r="AD2" s="16"/>
       <c r="AE2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF2" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="AF2" s="5" t="s">
+      <c r="AG2" t="s">
         <v>86</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="AH2" s="5" t="s">
-        <v>88</v>
-      </c>
       <c r="AI2" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>101</v>
       </c>
@@ -2492,7 +2491,7 @@
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -2501,67 +2500,67 @@
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M3" s="4"/>
       <c r="N3" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O3" s="4"/>
       <c r="P3" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q3" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="R3" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="R3" s="6" t="s">
-        <v>94</v>
       </c>
       <c r="S3" s="6"/>
       <c r="T3" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="U3" s="6"/>
       <c r="V3" s="6"/>
       <c r="W3" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="X3" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="X3" s="8" t="s">
+      <c r="Y3" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="Y3" s="4" t="s">
+      <c r="Z3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA3" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="Z3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA3" s="4" t="s">
+      <c r="AB3" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="AB3" s="4" t="s">
-        <v>100</v>
       </c>
       <c r="AC3" s="4"/>
       <c r="AD3" s="4"/>
       <c r="AE3" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AF3" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AH3" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI3" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>102</v>
       </c>
@@ -2570,78 +2569,78 @@
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H4" s="10"/>
       <c r="I4" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J4" s="10"/>
       <c r="K4" s="4"/>
       <c r="L4" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="M4" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="M4" s="4" t="s">
-        <v>105</v>
-      </c>
       <c r="N4" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O4" s="4"/>
       <c r="P4" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q4" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="R4" s="6" t="s">
         <v>106</v>
-      </c>
-      <c r="R4" s="6" t="s">
-        <v>107</v>
       </c>
       <c r="S4" s="6"/>
       <c r="T4" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
       <c r="W4" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="X4" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="X4" s="7" t="s">
+      <c r="Y4" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="Y4" s="4" t="s">
+      <c r="Z4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA4" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB4" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="Z4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA4" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="AB4" s="4" t="s">
-        <v>112</v>
       </c>
       <c r="AC4" s="4"/>
       <c r="AD4" s="4"/>
       <c r="AE4" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AF4" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AH4" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI4" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>103</v>
       </c>
@@ -2650,7 +2649,7 @@
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -2659,67 +2658,67 @@
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M5" s="4"/>
       <c r="N5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O5" s="4"/>
       <c r="P5" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q5" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="Q5" s="4" t="s">
+      <c r="R5" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="R5" s="6" t="s">
-        <v>94</v>
       </c>
       <c r="S5" s="6"/>
       <c r="T5" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="U5" s="6"/>
       <c r="V5" s="6"/>
       <c r="W5" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="X5" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="X5" s="8" t="s">
+      <c r="Y5" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="Y5" s="4" t="s">
+      <c r="Z5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA5" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="Z5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA5" s="4" t="s">
+      <c r="AB5" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="AB5" s="4" t="s">
-        <v>100</v>
       </c>
       <c r="AC5" s="4"/>
       <c r="AD5" s="4"/>
       <c r="AE5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AF5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AH5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI5" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>103</v>
       </c>
@@ -2728,78 +2727,78 @@
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H6" s="10"/>
       <c r="I6" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J6" s="10"/>
       <c r="K6" s="4"/>
       <c r="L6" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="M6" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="M6" s="4" t="s">
-        <v>105</v>
-      </c>
       <c r="N6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O6" s="4"/>
       <c r="P6" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q6" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="R6" s="6" t="s">
         <v>106</v>
-      </c>
-      <c r="R6" s="6" t="s">
-        <v>107</v>
       </c>
       <c r="S6" s="6"/>
       <c r="T6" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
       <c r="W6" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="X6" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y6" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="Y6" s="4" t="s">
+      <c r="Z6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA6" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB6" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="Z6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA6" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="AB6" s="4" t="s">
-        <v>112</v>
       </c>
       <c r="AC6" s="4"/>
       <c r="AD6" s="4"/>
       <c r="AE6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AF6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AH6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI6" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A7" s="13">
         <v>104</v>
       </c>
@@ -2808,11 +2807,11 @@
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -2833,27 +2832,27 @@
       <c r="W7" s="20"/>
       <c r="X7" s="5"/>
       <c r="Y7" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA7" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="Z7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA7" s="4" t="s">
+      <c r="AB7" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="AB7" s="4" t="s">
-        <v>100</v>
       </c>
       <c r="AC7" s="4"/>
       <c r="AD7" s="4"/>
       <c r="AE7" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AF7" s="4"/>
       <c r="AH7" s="4"/>
       <c r="AI7" s="4"/>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A8" s="13">
         <v>105</v>
       </c>
@@ -2861,10 +2860,10 @@
         <v>3</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E8" s="13"/>
       <c r="F8" s="5"/>
@@ -2872,78 +2871,78 @@
         <v>53704</v>
       </c>
       <c r="H8" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="J8" s="13" t="s">
         <v>116</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="J8" s="13" t="s">
-        <v>117</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M8" s="5"/>
       <c r="N8" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P8" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q8" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="Q8" s="5" t="s">
+      <c r="R8" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="R8" s="5" t="s">
+      <c r="S8" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="T8" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="S8" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="T8" s="5" t="s">
-        <v>95</v>
       </c>
       <c r="U8" s="5"/>
       <c r="V8" s="5"/>
       <c r="W8" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="X8" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="X8" s="5" t="s">
+      <c r="Y8" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="Y8" s="4" t="s">
+      <c r="Z8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA8" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="Z8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA8" s="4" t="s">
+      <c r="AB8" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="AB8" s="4" t="s">
-        <v>100</v>
-      </c>
       <c r="AC8" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AD8" s="4"/>
       <c r="AE8" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AF8" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AH8" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI8" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A9" s="15">
         <v>107</v>
       </c>
@@ -2951,56 +2950,56 @@
         <v>3</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E9" s="22"/>
       <c r="G9" s="13">
         <v>53704</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L9" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q9" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="N9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="P9" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q9" s="5" t="s">
+      <c r="R9" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="T9" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="W9" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="R9" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="T9" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="W9" s="20" t="s">
-        <v>122</v>
-      </c>
       <c r="X9" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y9" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="Y9" s="4" t="s">
+      <c r="Z9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA9" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="Z9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA9" s="4" t="s">
+      <c r="AB9" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="AB9" s="4" t="s">
-        <v>100</v>
-      </c>
       <c r="AD9" s="17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:35" ht="13.5" customHeight="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="18">
         <v>106</v>
       </c>
@@ -3009,7 +3008,7 @@
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E10" s="18"/>
       <c r="F10" s="18"/>
@@ -3018,68 +3017,68 @@
       </c>
       <c r="H10" s="18"/>
       <c r="I10" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J10" s="18"/>
       <c r="K10" s="18"/>
       <c r="L10" s="18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M10" s="18"/>
       <c r="N10" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O10" s="18"/>
       <c r="P10" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q10" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="Q10" s="18" t="s">
+      <c r="R10" s="18" t="s">
         <v>93</v>
-      </c>
-      <c r="R10" s="18" t="s">
-        <v>94</v>
       </c>
       <c r="S10" s="18"/>
       <c r="T10" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U10" s="18"/>
       <c r="V10" s="18"/>
       <c r="W10" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="X10" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="X10" s="18" t="s">
-        <v>127</v>
-      </c>
       <c r="Y10" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z10" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA10" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="Z10" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA10" s="18" t="s">
+      <c r="AB10" s="18" t="s">
         <v>99</v>
-      </c>
-      <c r="AB10" s="18" t="s">
-        <v>100</v>
       </c>
       <c r="AC10" s="18"/>
       <c r="AD10" s="18"/>
       <c r="AE10" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AF10" s="18"/>
       <c r="AG10" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AH10" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI10" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:35" ht="13.5" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="18">
         <v>109</v>
       </c>
@@ -3088,7 +3087,7 @@
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E11" s="18"/>
       <c r="F11" s="18"/>
@@ -3097,65 +3096,65 @@
       </c>
       <c r="H11" s="18"/>
       <c r="I11" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J11" s="18"/>
       <c r="K11" s="18"/>
       <c r="L11" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M11" s="18"/>
       <c r="N11" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O11" s="18"/>
       <c r="P11" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q11" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="Q11" s="18" t="s">
+      <c r="R11" s="18" t="s">
         <v>93</v>
-      </c>
-      <c r="R11" s="18" t="s">
-        <v>94</v>
       </c>
       <c r="S11" s="18"/>
       <c r="T11" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="U11" s="18"/>
       <c r="V11" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="W11" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="X11" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="X11" s="18" t="s">
+      <c r="Y11" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="Y11" s="18" t="s">
+      <c r="Z11" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA11" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="Z11" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA11" s="18" t="s">
+      <c r="AB11" s="18" t="s">
         <v>99</v>
-      </c>
-      <c r="AB11" s="18" t="s">
-        <v>100</v>
       </c>
       <c r="AC11" s="18"/>
       <c r="AD11" s="18"/>
       <c r="AE11" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AF11" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AH11" s="1"/>
       <c r="AI11" s="1"/>
     </row>
-    <row r="12" spans="1:35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A12" s="22">
         <v>108</v>
       </c>
@@ -3164,7 +3163,7 @@
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -3173,66 +3172,66 @@
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M12" s="4"/>
       <c r="N12" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P12" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q12" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="Q12" s="4" t="s">
+      <c r="R12" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="R12" s="6" t="s">
-        <v>94</v>
       </c>
       <c r="S12" s="6"/>
       <c r="T12" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="U12" s="6"/>
       <c r="V12" s="6"/>
       <c r="W12" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="X12" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="X12" s="8" t="s">
+      <c r="Y12" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="Y12" s="4" t="s">
+      <c r="Z12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA12" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="Z12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA12" s="4" t="s">
+      <c r="AB12" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="AB12" s="4" t="s">
-        <v>100</v>
       </c>
       <c r="AC12" s="4"/>
       <c r="AD12" s="4"/>
       <c r="AE12" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AF12" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AH12" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI12" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A13" s="22">
         <v>110</v>
       </c>
@@ -3240,10 +3239,10 @@
         <v>3</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -3268,18 +3267,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.27734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33984375" customWidth="1"/>
+    <col min="3" max="3" width="22.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3287,30 +3284,30 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" t="s">
         <v>129</v>
       </c>
-      <c r="E1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D2" t="s">
         <v>131</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>132</v>
       </c>
-      <c r="E2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>104</v>
       </c>
@@ -3318,13 +3315,13 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -3336,26 +3333,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.27734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.48046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.04296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.71484375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.10546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.31640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.4453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.97265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.1015625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3363,24 +3358,24 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" t="s">
         <v>134</v>
       </c>
-      <c r="D1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" t="s">
         <v>136</v>
       </c>
-      <c r="D2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="14.25" customHeight="1">
+    </row>
+    <row r="3" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>104</v>
       </c>
@@ -3388,10 +3383,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
@@ -3408,52 +3403,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AL4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" customWidth="1"/>
-    <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="25" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" customWidth="1"/>
-    <col min="9" max="9" width="28.42578125" customWidth="1"/>
-    <col min="10" max="10" width="16" customWidth="1"/>
-    <col min="11" max="11" width="21.42578125" customWidth="1"/>
-    <col min="12" max="12" width="20.140625" customWidth="1"/>
-    <col min="13" max="13" width="19.140625" customWidth="1"/>
-    <col min="14" max="14" width="24.28515625" customWidth="1"/>
-    <col min="15" max="15" width="26.28515625" customWidth="1"/>
-    <col min="16" max="16" width="23.5703125" customWidth="1"/>
-    <col min="17" max="17" width="25.140625" customWidth="1"/>
-    <col min="18" max="18" width="30" customWidth="1"/>
-    <col min="19" max="19" width="27.140625" customWidth="1"/>
-    <col min="20" max="20" width="26.85546875" customWidth="1"/>
-    <col min="21" max="21" width="25" customWidth="1"/>
-    <col min="22" max="22" width="32.7109375" customWidth="1"/>
-    <col min="23" max="23" width="25.28515625" customWidth="1"/>
-    <col min="24" max="24" width="24.42578125" customWidth="1"/>
-    <col min="25" max="25" width="27.5703125" customWidth="1"/>
-    <col min="26" max="26" width="24.140625" customWidth="1"/>
-    <col min="27" max="27" width="33.5703125" customWidth="1"/>
-    <col min="28" max="28" width="29.140625" customWidth="1"/>
-    <col min="29" max="29" width="32.85546875" customWidth="1"/>
-    <col min="30" max="30" width="28.5703125" customWidth="1"/>
-    <col min="31" max="31" width="28" customWidth="1"/>
-    <col min="32" max="32" width="23.85546875" customWidth="1"/>
-    <col min="33" max="33" width="22.85546875" customWidth="1"/>
-    <col min="34" max="34" width="21.5703125" customWidth="1"/>
-    <col min="35" max="35" width="38.85546875" customWidth="1"/>
-    <col min="36" max="36" width="35.42578125" customWidth="1"/>
-    <col min="37" max="37" width="30.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.9296875" customWidth="1"/>
+    <col min="3" max="3" width="14.796875" customWidth="1"/>
+    <col min="4" max="4" width="20.84765625" customWidth="1"/>
+    <col min="5" max="5" width="20.04296875" customWidth="1"/>
+    <col min="6" max="6" width="25.01953125" customWidth="1"/>
+    <col min="7" max="7" width="20.4453125" customWidth="1"/>
+    <col min="8" max="8" width="20.58203125" customWidth="1"/>
+    <col min="9" max="9" width="28.3828125" customWidth="1"/>
+    <col min="10" max="10" width="16.0078125" customWidth="1"/>
+    <col min="11" max="11" width="21.38671875" customWidth="1"/>
+    <col min="12" max="12" width="20.17578125" customWidth="1"/>
+    <col min="13" max="13" width="19.1015625" customWidth="1"/>
+    <col min="14" max="14" width="24.34765625" customWidth="1"/>
+    <col min="15" max="15" width="26.23046875" customWidth="1"/>
+    <col min="16" max="16" width="23.5390625" customWidth="1"/>
+    <col min="17" max="17" width="25.15234375" customWidth="1"/>
+    <col min="18" max="18" width="29.99609375" customWidth="1"/>
+    <col min="19" max="19" width="27.171875" customWidth="1"/>
+    <col min="20" max="20" width="26.90234375" customWidth="1"/>
+    <col min="21" max="21" width="25.01953125" customWidth="1"/>
+    <col min="22" max="22" width="32.6875" customWidth="1"/>
+    <col min="23" max="23" width="25.2890625" customWidth="1"/>
+    <col min="24" max="24" width="24.48046875" customWidth="1"/>
+    <col min="25" max="25" width="27.57421875" customWidth="1"/>
+    <col min="26" max="26" width="24.078125" customWidth="1"/>
+    <col min="27" max="27" width="33.62890625" customWidth="1"/>
+    <col min="28" max="28" width="29.19140625" customWidth="1"/>
+    <col min="29" max="29" width="32.8203125" customWidth="1"/>
+    <col min="30" max="30" width="28.515625" customWidth="1"/>
+    <col min="31" max="31" width="27.98046875" customWidth="1"/>
+    <col min="32" max="32" width="23.80859375" customWidth="1"/>
+    <col min="33" max="33" width="22.8671875" customWidth="1"/>
+    <col min="34" max="34" width="21.5234375" customWidth="1"/>
+    <col min="35" max="35" width="38.875" customWidth="1"/>
+    <col min="36" max="36" width="35.37890625" customWidth="1"/>
+    <col min="37" max="37" width="30.1328125" customWidth="1"/>
     <col min="38" max="38" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
@@ -3461,229 +3454,229 @@
         <v>1</v>
       </c>
       <c r="C1" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" s="27" t="s">
         <v>138</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="E1" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="F1" s="27" t="s">
         <v>140</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="G1" s="27" t="s">
         <v>141</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="H1" s="27" t="s">
         <v>142</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="I1" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="J1" s="27" t="s">
         <v>144</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="K1" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="K1" s="28" t="s">
+      <c r="L1" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="L1" s="31" t="s">
+      <c r="M1" s="34" t="s">
         <v>147</v>
       </c>
-      <c r="M1" s="34" t="s">
+      <c r="N1" s="34" t="s">
         <v>148</v>
       </c>
-      <c r="N1" s="34" t="s">
+      <c r="O1" s="34" t="s">
         <v>149</v>
       </c>
-      <c r="O1" s="34" t="s">
+      <c r="P1" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="P1" s="34" t="s">
+      <c r="Q1" s="34" t="s">
         <v>151</v>
       </c>
-      <c r="Q1" s="34" t="s">
+      <c r="R1" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="R1" s="34" t="s">
+      <c r="S1" s="34" t="s">
         <v>153</v>
       </c>
-      <c r="S1" s="34" t="s">
+      <c r="T1" s="34" t="s">
         <v>154</v>
       </c>
-      <c r="T1" s="34" t="s">
+      <c r="U1" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="U1" s="34" t="s">
+      <c r="V1" s="34" t="s">
         <v>156</v>
       </c>
-      <c r="V1" s="34" t="s">
+      <c r="W1" s="34" t="s">
         <v>157</v>
       </c>
-      <c r="W1" s="34" t="s">
+      <c r="X1" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="X1" s="34" t="s">
+      <c r="Y1" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="Y1" s="34" t="s">
+      <c r="Z1" s="34" t="s">
         <v>160</v>
       </c>
-      <c r="Z1" s="34" t="s">
+      <c r="AA1" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="AA1" s="34" t="s">
+      <c r="AB1" s="34" t="s">
         <v>162</v>
       </c>
-      <c r="AB1" s="34" t="s">
+      <c r="AC1" s="34" t="s">
         <v>163</v>
       </c>
-      <c r="AC1" s="34" t="s">
+      <c r="AD1" s="34" t="s">
         <v>164</v>
       </c>
-      <c r="AD1" s="34" t="s">
+      <c r="AE1" s="34" t="s">
         <v>165</v>
       </c>
-      <c r="AE1" s="34" t="s">
+      <c r="AF1" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="AF1" s="34" t="s">
+      <c r="AG1" s="34" t="s">
         <v>167</v>
       </c>
-      <c r="AG1" s="34" t="s">
+      <c r="AH1" s="34" t="s">
         <v>168</v>
       </c>
-      <c r="AH1" s="34" t="s">
+      <c r="AI1" s="34" t="s">
         <v>169</v>
       </c>
-      <c r="AI1" s="34" t="s">
+      <c r="AJ1" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="AJ1" s="34" t="s">
+      <c r="AK1" s="34" t="s">
         <v>171</v>
       </c>
-      <c r="AK1" s="34" t="s">
+      <c r="AL1" s="31" t="s">
         <v>172</v>
       </c>
-      <c r="AL1" s="31" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="2" spans="1:38">
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="M2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2" s="5" t="s">
+      <c r="O2" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="P2" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="O2" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="P2" s="5" t="s">
+      <c r="Q2" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="R2" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="S2" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="T2" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="U2" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="V2" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="W2" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="W2" s="5" t="s">
+      <c r="X2" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="X2" s="5" t="s">
+      <c r="Y2" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="Y2" s="5" t="s">
+      <c r="Z2" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="Z2" s="5" t="s">
+      <c r="AA2" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="AA2" s="5" t="s">
+      <c r="AB2" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="AB2" s="5" t="s">
+      <c r="AC2" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="AC2" s="5" t="s">
+      <c r="AD2" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="AD2" s="5" t="s">
+      <c r="AE2" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="AE2" s="5" t="s">
+      <c r="AF2" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="AF2" s="5" t="s">
+      <c r="AG2" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="AG2" s="5" t="s">
+      <c r="AH2" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="AH2" s="5" t="s">
+      <c r="AI2" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="AI2" s="5" t="s">
+      <c r="AJ2" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="AJ2" s="5" t="s">
+      <c r="AK2" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="AK2" s="5" t="s">
+      <c r="AL2" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="AL2" s="5" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="3" spans="1:38">
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A3" s="30">
         <v>112</v>
       </c>
@@ -3691,13 +3684,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="36" t="s">
+        <v>207</v>
+      </c>
+      <c r="D3" s="36" t="s">
         <v>208</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="E3" s="36" t="s">
         <v>209</v>
-      </c>
-      <c r="E3" s="36" t="s">
-        <v>210</v>
       </c>
       <c r="F3" s="16"/>
       <c r="H3" s="37"/>
@@ -3732,7 +3725,7 @@
       <c r="AK3" s="37"/>
       <c r="AL3" s="38"/>
     </row>
-    <row r="4" spans="1:38">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>113</v>
       </c>
@@ -3743,103 +3736,103 @@
       <c r="D4" s="5"/>
       <c r="E4" s="29"/>
       <c r="F4" s="29" t="s">
+        <v>210</v>
+      </c>
+      <c r="G4" s="32" t="s">
         <v>211</v>
       </c>
-      <c r="G4" s="32" t="s">
+      <c r="H4" s="29" t="s">
         <v>212</v>
-      </c>
-      <c r="H4" s="29" t="s">
-        <v>213</v>
       </c>
       <c r="I4" s="32">
         <v>3</v>
       </c>
       <c r="J4" s="33" t="s">
+        <v>213</v>
+      </c>
+      <c r="K4" s="29" t="s">
         <v>214</v>
       </c>
-      <c r="K4" s="29" t="s">
-        <v>215</v>
-      </c>
       <c r="L4" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M4" s="29" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="N4" s="29" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O4" s="29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P4" s="29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q4" s="29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R4" s="29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S4" s="29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T4" s="29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U4" s="29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="V4" s="29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="W4" s="29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="X4" s="29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Y4" s="29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Z4" s="29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AA4" s="29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AB4" s="29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AC4" s="29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AD4" s="29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AE4" s="29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AF4" s="29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AG4" s="29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AH4" s="29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI4" s="29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AJ4" s="29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AK4" s="29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AL4" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -3854,16 +3847,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.27734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3871,13 +3862,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D1" t="s">
         <v>216</v>
       </c>
-      <c r="D1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>111</v>
       </c>
@@ -3888,7 +3879,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -3904,12 +3895,12 @@
       <selection activeCell="B6" sqref="B6:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3917,19 +3908,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>101</v>
       </c>
@@ -3937,10 +3928,10 @@
         <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>102</v>
       </c>
@@ -3948,10 +3939,10 @@
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>103</v>
       </c>
@@ -3959,10 +3950,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="39">
         <v>106</v>
       </c>
@@ -3970,7 +3961,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created a new row to implement ExplicitWaits
</commit_message>
<xml_diff>
--- a/resources/test_data/VM_TestData_Sample1.xlsx
+++ b/resources/test_data/VM_TestData_Sample1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\praneethm\git\VMSeleniumFramework\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{FB668017-213A-4EDB-AFEF-04A2EF534A24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6E6CAD2D-9228-4913-BD95-B19399908B50}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{FB668017-213A-4EDB-AFEF-04A2EF534A24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{39077E56-2A1E-43F1-8384-97C5027CFF02}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="2055" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="222">
   <si>
     <t>TestCaseNumber</t>
   </si>
@@ -711,6 +711,9 @@
   </si>
   <si>
     <t>Locators</t>
+  </si>
+  <si>
+    <t>ExplicitWait</t>
   </si>
 </sst>
 </file>
@@ -782,7 +785,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -927,12 +930,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF505050"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF505050"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF505050"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF505050"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1013,6 +1031,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1711,10 +1733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1786,32 +1808,22 @@
       <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="23">
-        <v>101</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>14</v>
-      </c>
+      <c r="A3" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
       <c r="D3" s="5"/>
-      <c r="E3" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="E3" s="5"/>
       <c r="F3" s="5"/>
-      <c r="G3" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="G3" s="5"/>
       <c r="H3" s="5"/>
-      <c r="I3" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="I3" s="5"/>
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="23">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B4" s="23" t="s">
         <v>13</v>
@@ -1835,7 +1847,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="23">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B5" s="23" t="s">
         <v>13</v>
@@ -1853,16 +1865,16 @@
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="24">
-        <v>104</v>
-      </c>
-      <c r="B6" s="4">
-        <v>1</v>
+      <c r="A6" s="23">
+        <v>103</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>13</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>14</v>
@@ -1877,13 +1889,13 @@
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="24">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B7" s="4">
         <v>1</v>
@@ -1899,7 +1911,7 @@
       <c r="G7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="25"/>
+      <c r="H7" s="5"/>
       <c r="I7" s="5" t="s">
         <v>17</v>
       </c>
@@ -1907,7 +1919,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="24">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B8" s="4">
         <v>1</v>
@@ -1916,22 +1928,22 @@
         <v>14</v>
       </c>
       <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="26" t="s">
-        <v>17</v>
-      </c>
+      <c r="E8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="5"/>
       <c r="G8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="26" t="s">
+      <c r="H8" s="25"/>
+      <c r="I8" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="24">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B9" s="4">
         <v>1</v>
@@ -1939,23 +1951,23 @@
       <c r="C9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="D9" s="5"/>
       <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="F9" s="26" t="s">
+        <v>17</v>
+      </c>
       <c r="G9" s="5" t="s">
         <v>16</v>
       </c>
       <c r="H9" s="5"/>
-      <c r="I9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="26" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="24">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B10" s="4">
         <v>1</v>
@@ -1963,23 +1975,23 @@
       <c r="C10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="D10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5" t="s">
         <v>16</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="24">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B11" s="4">
         <v>1</v>
@@ -1997,13 +2009,13 @@
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="24">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B12" s="4">
         <v>1</v>
@@ -2024,6 +2036,30 @@
         <v>15</v>
       </c>
       <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="24">
+        <v>110</v>
+      </c>
+      <c r="B13" s="4">
+        <v>1</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2033,10 +2069,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2049,7 +2085,7 @@
     <col min="6" max="6" width="43.98828125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2072,7 +2108,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>219</v>
       </c>
@@ -2089,37 +2125,38 @@
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>101</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>102</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
@@ -2130,48 +2167,50 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>103</v>
       </c>
       <c r="B6" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B7" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B8" s="1">
         <v>2</v>
       </c>
-      <c r="E8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B9" s="1">
         <v>2</v>
@@ -2180,31 +2219,31 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B10" s="1">
         <v>2</v>
       </c>
-      <c r="D10" s="17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B11" s="1">
         <v>2</v>
       </c>
-      <c r="E11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D11" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B12" s="1">
         <v>2</v>
@@ -2213,9 +2252,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B13" s="1">
         <v>2</v>
@@ -2224,10 +2263,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="F14" s="1"/>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>110</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="F15" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2236,10 +2286,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AI13"/>
+  <dimension ref="A1:AI14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2484,111 +2534,45 @@
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
-        <v>101</v>
-      </c>
-      <c r="B3" s="4">
-        <v>3</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4">
-        <v>53704</v>
-      </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="R3" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="X3" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="Y3" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA3" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="AB3" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="AC3" s="4"/>
-      <c r="AD3" s="4"/>
-      <c r="AE3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AH3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AI3" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="A3" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B4" s="4">
         <v>3</v>
       </c>
       <c r="C4" s="4"/>
-      <c r="D4" s="9" t="s">
-        <v>99</v>
+      <c r="D4" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="J4" s="10"/>
+      <c r="G4" s="4">
+        <v>53704</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="J4" s="4"/>
       <c r="K4" s="4"/>
-      <c r="L4" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>103</v>
-      </c>
+      <c r="L4" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M4" s="4"/>
       <c r="N4" s="4" t="s">
         <v>15</v>
       </c>
@@ -2597,25 +2581,25 @@
         <v>90</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="R4" s="6" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="S4" s="6"/>
       <c r="T4" s="6" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
       <c r="W4" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="X4" s="7" t="s">
-        <v>108</v>
+        <v>94</v>
+      </c>
+      <c r="X4" s="8" t="s">
+        <v>95</v>
       </c>
       <c r="Y4" s="4" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="Z4" s="4" t="s">
         <v>15</v>
@@ -2624,7 +2608,7 @@
         <v>97</v>
       </c>
       <c r="AB4" s="4" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="AC4" s="4"/>
       <c r="AD4" s="4"/>
@@ -2643,30 +2627,32 @@
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B5" s="4">
         <v>3</v>
       </c>
       <c r="C5" s="4"/>
-      <c r="D5" s="4" t="s">
-        <v>87</v>
+      <c r="D5" s="9" t="s">
+        <v>99</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="4">
-        <v>53704</v>
-      </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="J5" s="4"/>
+      <c r="G5" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="J5" s="10"/>
       <c r="K5" s="4"/>
-      <c r="L5" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M5" s="4"/>
+      <c r="L5" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>103</v>
+      </c>
       <c r="N5" s="4" t="s">
         <v>15</v>
       </c>
@@ -2675,25 +2661,25 @@
         <v>90</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="R5" s="6" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="S5" s="6"/>
       <c r="T5" s="6" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="U5" s="6"/>
       <c r="V5" s="6"/>
       <c r="W5" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="X5" s="8" t="s">
-        <v>95</v>
+        <v>107</v>
+      </c>
+      <c r="X5" s="7" t="s">
+        <v>108</v>
       </c>
       <c r="Y5" s="4" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="Z5" s="4" t="s">
         <v>15</v>
@@ -2702,7 +2688,7 @@
         <v>97</v>
       </c>
       <c r="AB5" s="4" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="AC5" s="4"/>
       <c r="AD5" s="4"/>
@@ -2724,29 +2710,27 @@
         <v>103</v>
       </c>
       <c r="B6" s="4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C6" s="4"/>
-      <c r="D6" s="9" t="s">
-        <v>99</v>
+      <c r="D6" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
-      <c r="G6" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="J6" s="10"/>
+      <c r="G6" s="4">
+        <v>53704</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="J6" s="4"/>
       <c r="K6" s="4"/>
-      <c r="L6" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>103</v>
-      </c>
+      <c r="L6" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M6" s="4"/>
       <c r="N6" s="4" t="s">
         <v>15</v>
       </c>
@@ -2755,10 +2739,10 @@
         <v>90</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="R6" s="6" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="S6" s="6"/>
       <c r="T6" s="6" t="s">
@@ -2767,13 +2751,13 @@
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
       <c r="W6" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="X6" s="7" t="s">
-        <v>108</v>
+        <v>94</v>
+      </c>
+      <c r="X6" s="8" t="s">
+        <v>95</v>
       </c>
       <c r="Y6" s="4" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="Z6" s="4" t="s">
         <v>15</v>
@@ -2782,7 +2766,7 @@
         <v>97</v>
       </c>
       <c r="AB6" s="4" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="AC6" s="4"/>
       <c r="AD6" s="4"/>
@@ -2800,40 +2784,60 @@
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A7" s="13">
+      <c r="A7" s="4">
+        <v>103</v>
+      </c>
+      <c r="B7" s="4">
+        <v>6</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="J7" s="10"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q7" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="13">
-        <v>5</v>
-      </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="E7" s="13"/>
-      <c r="F7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
-      <c r="T7" s="5"/>
-      <c r="U7" s="5"/>
-      <c r="V7" s="5"/>
-      <c r="W7" s="20"/>
-      <c r="X7" s="5"/>
+      <c r="R7" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="X7" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="Y7" s="4" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="Z7" s="4" t="s">
         <v>15</v>
@@ -2842,78 +2846,56 @@
         <v>97</v>
       </c>
       <c r="AB7" s="4" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="AC7" s="4"/>
       <c r="AD7" s="4"/>
       <c r="AE7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AF7" s="4"/>
-      <c r="AH7" s="4"/>
-      <c r="AI7" s="4"/>
+      <c r="AF7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI7" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A8" s="13">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B8" s="13">
-        <v>3</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>113</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C8" s="13"/>
       <c r="D8" s="13" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="E8" s="13"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="13">
-        <v>53704</v>
-      </c>
-      <c r="H8" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="J8" s="13" t="s">
-        <v>115</v>
-      </c>
+      <c r="F8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
       <c r="K8" s="5"/>
-      <c r="L8" s="5" t="s">
-        <v>89</v>
-      </c>
+      <c r="L8" s="5"/>
       <c r="M8" s="5"/>
-      <c r="N8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="O8" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="P8" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q8" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="R8" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="S8" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="T8" s="5" t="s">
-        <v>93</v>
-      </c>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
       <c r="U8" s="5"/>
       <c r="V8" s="5"/>
-      <c r="W8" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="X8" s="5" t="s">
-        <v>95</v>
-      </c>
+      <c r="W8" s="20"/>
+      <c r="X8" s="5"/>
       <c r="Y8" s="4" t="s">
         <v>96</v>
       </c>
@@ -2926,60 +2908,72 @@
       <c r="AB8" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="AC8" s="4" t="s">
-        <v>117</v>
-      </c>
+      <c r="AC8" s="4"/>
       <c r="AD8" s="4"/>
       <c r="AE8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AF8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AH8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AI8" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="AF8" s="4"/>
+      <c r="AH8" s="4"/>
+      <c r="AI8" s="4"/>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A9" s="15">
-        <v>107</v>
+      <c r="A9" s="13">
+        <v>105</v>
       </c>
       <c r="B9" s="13">
         <v>3</v>
       </c>
+      <c r="C9" s="13" t="s">
+        <v>113</v>
+      </c>
       <c r="D9" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="E9" s="22"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="5"/>
       <c r="G9" s="13">
         <v>53704</v>
       </c>
+      <c r="H9" s="13" t="s">
+        <v>114</v>
+      </c>
       <c r="I9" s="5" t="s">
         <v>88</v>
       </c>
+      <c r="J9" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="K9" s="5"/>
       <c r="L9" s="5" t="s">
-        <v>118</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="M9" s="5"/>
       <c r="N9" s="5" t="s">
         <v>15</v>
+      </c>
+      <c r="O9" s="5" t="s">
+        <v>116</v>
       </c>
       <c r="P9" s="5" t="s">
         <v>90</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
       <c r="R9" s="5" t="s">
         <v>92</v>
       </c>
+      <c r="S9" s="5" t="s">
+        <v>113</v>
+      </c>
       <c r="T9" s="5" t="s">
-        <v>106</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
       <c r="W9" s="20" t="s">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="X9" s="5" t="s">
         <v>95</v>
@@ -2996,99 +2990,90 @@
       <c r="AB9" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="AD9" s="17" t="s">
+      <c r="AC9" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="AD9" s="4"/>
+      <c r="AE9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI9" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A10" s="15">
+        <v>107</v>
+      </c>
+      <c r="B10" s="13">
+        <v>3</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="E10" s="22"/>
+      <c r="G10" s="13">
+        <v>53704</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q10" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="T10" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="W10" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="X10" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y10" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA10" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB10" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD10" s="17" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="18">
-        <v>106</v>
-      </c>
-      <c r="B10" s="18">
-        <v>3</v>
-      </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18">
-        <v>53704</v>
-      </c>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q10" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="R10" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="S10" s="18"/>
-      <c r="T10" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="U10" s="18"/>
-      <c r="V10" s="18"/>
-      <c r="W10" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="X10" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="Y10" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z10" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA10" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="AB10" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="AC10" s="18"/>
-      <c r="AD10" s="18"/>
-      <c r="AE10" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF10" s="18"/>
-      <c r="AG10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AH10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AI10" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="18">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B11" s="18">
         <v>3</v>
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="18" t="s">
-        <v>87</v>
+        <v>121</v>
       </c>
       <c r="E11" s="18"/>
       <c r="F11" s="18"/>
@@ -3102,7 +3087,7 @@
       <c r="J11" s="18"/>
       <c r="K11" s="18"/>
       <c r="L11" s="18" t="s">
-        <v>89</v>
+        <v>122</v>
       </c>
       <c r="M11" s="18"/>
       <c r="N11" s="18" t="s">
@@ -3120,17 +3105,15 @@
       </c>
       <c r="S11" s="18"/>
       <c r="T11" s="18" t="s">
-        <v>93</v>
+        <v>123</v>
       </c>
       <c r="U11" s="18"/>
-      <c r="V11" s="18" t="s">
-        <v>126</v>
-      </c>
+      <c r="V11" s="18"/>
       <c r="W11" s="21" t="s">
-        <v>94</v>
+        <v>124</v>
       </c>
       <c r="X11" s="18" t="s">
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="Y11" s="18" t="s">
         <v>96</v>
@@ -3149,115 +3132,196 @@
       <c r="AE11" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="AF11" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="AH11" s="1"/>
-      <c r="AI11" s="1"/>
-    </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A12" s="22">
-        <v>108</v>
-      </c>
-      <c r="B12" s="4">
+      <c r="AF11" s="18"/>
+      <c r="AG11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI11" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="18">
+        <v>109</v>
+      </c>
+      <c r="B12" s="18">
         <v>3</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4" t="s">
+      <c r="C12" s="18"/>
+      <c r="D12" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4">
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18">
         <v>53704</v>
       </c>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4" t="s">
+      <c r="H12" s="18"/>
+      <c r="I12" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4" t="s">
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="P12" s="4" t="s">
+      <c r="M12" s="18"/>
+      <c r="N12" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="O12" s="18"/>
+      <c r="P12" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="Q12" s="4" t="s">
+      <c r="Q12" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="R12" s="6" t="s">
+      <c r="R12" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="S12" s="6"/>
-      <c r="T12" s="6" t="s">
+      <c r="S12" s="18"/>
+      <c r="T12" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="U12" s="6"/>
-      <c r="V12" s="6"/>
-      <c r="W12" s="19" t="s">
+      <c r="U12" s="18"/>
+      <c r="V12" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="W12" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="X12" s="8" t="s">
+      <c r="X12" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="Y12" s="4" t="s">
+      <c r="Y12" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="Z12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA12" s="4" t="s">
+      <c r="Z12" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA12" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="AB12" s="4" t="s">
+      <c r="AB12" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="AC12" s="4"/>
-      <c r="AD12" s="4"/>
-      <c r="AE12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AH12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AI12" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="AC12" s="18"/>
+      <c r="AD12" s="18"/>
+      <c r="AE12" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF12" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH12" s="1"/>
+      <c r="AI12" s="1"/>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A13" s="22">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B13" s="4">
         <v>3</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="C13" s="4"/>
+      <c r="D13" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4">
+        <v>53704</v>
+      </c>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="R13" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6"/>
+      <c r="W13" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="X13" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y13" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA13" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB13" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC13" s="4"/>
+      <c r="AD13" s="4"/>
+      <c r="AE13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI13" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A14" s="22">
+        <v>110</v>
+      </c>
+      <c r="B14" s="4">
+        <v>3</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="E14" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="G4:J4 L4 Q4 W3:X6 G6:J6 L6 Q6 W12:X12" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="G5:J5 L5 Q5 W4:X7 G7:J7 L7 Q7 W13:X13" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G4" r:id="rId1" display="random123@gmail.com" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="I4" r:id="rId2" display="random123@gmail.com" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="X3" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="X5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="G6" r:id="rId5" display="random123@gmail.com" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
-    <hyperlink ref="I6" r:id="rId6" display="random123@gmail.com" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
-    <hyperlink ref="X12" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="G5" r:id="rId1" display="random123@gmail.com" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="I5" r:id="rId2" display="random123@gmail.com" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="X4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="X6" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="G7" r:id="rId5" display="random123@gmail.com" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="I7" r:id="rId6" display="random123@gmail.com" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="X13" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
@@ -3266,10 +3330,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3279,7 +3343,7 @@
     <col min="3" max="3" width="22.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3296,7 +3360,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>219</v>
       </c>
@@ -3310,20 +3374,34 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>104</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B4" s="1">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>87</v>
       </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -3334,10 +3412,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3380,24 +3458,38 @@
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>104</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B4" s="1">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3406,7 +3498,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:AL4"/>
+  <dimension ref="A1:AL5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -3684,167 +3776,181 @@
       </c>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A3" s="30">
+      <c r="A3" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A4" s="30">
         <v>112</v>
       </c>
-      <c r="B3" s="35">
+      <c r="B4" s="35">
         <v>1</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C4" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D4" s="36" t="s">
         <v>207</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="E4" s="36" t="s">
         <v>208</v>
       </c>
-      <c r="F3" s="16"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37"/>
-      <c r="S3" s="37"/>
-      <c r="T3" s="37"/>
-      <c r="U3" s="37"/>
-      <c r="V3" s="37"/>
-      <c r="W3" s="37"/>
-      <c r="X3" s="37"/>
-      <c r="Y3" s="37"/>
-      <c r="Z3" s="37"/>
-      <c r="AA3" s="37"/>
-      <c r="AB3" s="37"/>
-      <c r="AC3" s="37"/>
-      <c r="AD3" s="37"/>
-      <c r="AE3" s="37"/>
-      <c r="AF3" s="37"/>
-      <c r="AG3" s="37"/>
-      <c r="AH3" s="37"/>
-      <c r="AI3" s="37"/>
-      <c r="AJ3" s="37"/>
-      <c r="AK3" s="37"/>
-      <c r="AL3" s="38"/>
-    </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
+      <c r="F4" s="16"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="37"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="37"/>
+      <c r="S4" s="37"/>
+      <c r="T4" s="37"/>
+      <c r="U4" s="37"/>
+      <c r="V4" s="37"/>
+      <c r="W4" s="37"/>
+      <c r="X4" s="37"/>
+      <c r="Y4" s="37"/>
+      <c r="Z4" s="37"/>
+      <c r="AA4" s="37"/>
+      <c r="AB4" s="37"/>
+      <c r="AC4" s="37"/>
+      <c r="AD4" s="37"/>
+      <c r="AE4" s="37"/>
+      <c r="AF4" s="37"/>
+      <c r="AG4" s="37"/>
+      <c r="AH4" s="37"/>
+      <c r="AI4" s="37"/>
+      <c r="AJ4" s="37"/>
+      <c r="AK4" s="37"/>
+      <c r="AL4" s="38"/>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
         <v>113</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B5" s="4">
         <v>1</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29" t="s">
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29" t="s">
         <v>209</v>
       </c>
-      <c r="G4" s="32" t="s">
+      <c r="G5" s="32" t="s">
         <v>210</v>
       </c>
-      <c r="H4" s="29" t="s">
+      <c r="H5" s="29" t="s">
         <v>211</v>
       </c>
-      <c r="I4" s="32">
+      <c r="I5" s="32">
         <v>3</v>
       </c>
-      <c r="J4" s="33" t="s">
+      <c r="J5" s="33" t="s">
         <v>212</v>
       </c>
-      <c r="K4" s="29" t="s">
+      <c r="K5" s="29" t="s">
         <v>213</v>
       </c>
-      <c r="L4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M4" s="29" t="s">
+      <c r="L5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M5" s="29" t="s">
         <v>207</v>
       </c>
-      <c r="N4" s="29" t="s">
+      <c r="N5" s="29" t="s">
         <v>207</v>
       </c>
-      <c r="O4" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="P4" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q4" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="R4" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="S4" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="T4" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="U4" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="V4" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="W4" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="X4" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y4" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z4" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA4" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="AB4" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC4" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD4" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="AE4" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF4" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG4" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="AH4" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="AI4" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="AJ4" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="AK4" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="AL4" s="5" t="s">
+      <c r="O5" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="P5" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q5" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="R5" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="S5" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="T5" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="U5" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="V5" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="W5" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="X5" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y5" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z5" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA5" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB5" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC5" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD5" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE5" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF5" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG5" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH5" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI5" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ5" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="AK5" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="AL5" s="5" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J4" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="J5" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3852,42 +3958,173 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.27734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="40" t="s">
         <v>214</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="40" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="40" t="s">
+        <v>219</v>
+      </c>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="40" t="s">
+        <v>220</v>
+      </c>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="41">
         <v>111</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B4" s="41">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C4" s="41">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="D4" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3896,10 +4133,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="XEK1" workbookViewId="0">
+      <selection activeCell="XFD3" sqref="XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3907,7 +4144,7 @@
     <col min="1" max="1" width="17.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3918,7 +4155,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>219</v>
       </c>
@@ -3927,20 +4164,23 @@
         <v>217</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
         <v>101</v>
-      </c>
-      <c r="B3" s="3">
-        <v>4</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
-        <v>102</v>
       </c>
       <c r="B4" s="3">
         <v>4</v>
@@ -3949,9 +4189,9 @@
         <v>208</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B5" s="3">
         <v>4</v>
@@ -3960,14 +4200,25 @@
         <v>208</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="39">
-        <v>106</v>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>103</v>
       </c>
       <c r="B6" s="3">
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="39">
+        <v>106</v>
+      </c>
+      <c r="B7" s="3">
+        <v>4</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>208</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added explicit wait to fix ElementClickIntercepted on SelectUser
</commit_message>
<xml_diff>
--- a/resources/test_data/VM_TestData_Sample1.xlsx
+++ b/resources/test_data/VM_TestData_Sample1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\praneethm\git\VMSeleniumFramework\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C5DD6AE7-A56F-4F0F-924B-A0C72DC33448}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{787A4407-52FA-43A7-8478-23EE79F688B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="2055" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="2055" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LogInPage" sheetId="22" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="224">
   <si>
     <t>TestCaseNumber</t>
   </si>
@@ -327,6 +327,9 @@
   </si>
   <si>
     <t>//*[@id="existingAccountpopup"]/div/div/div[3]/button</t>
+  </si>
+  <si>
+    <t>Sleep=4000</t>
   </si>
   <si>
     <t>Jack</t>
@@ -2310,8 +2313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AI14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="Y14" sqref="Y14"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AF18" sqref="AF18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2568,6 +2571,9 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
+      <c r="AF3" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="4" spans="1:35">
       <c r="A4" s="4">
@@ -2578,7 +2584,7 @@
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -2587,12 +2593,12 @@
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="M4" s="4"/>
       <c r="N4" s="4" t="s">
@@ -2600,37 +2606,37 @@
       </c>
       <c r="O4" s="4"/>
       <c r="P4" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="R4" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="S4" s="6"/>
       <c r="T4" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
       <c r="W4" s="19" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="X4" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="Y4" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="Z4" s="4" t="s">
         <v>18</v>
       </c>
       <c r="AA4" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AB4" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AC4" s="4"/>
       <c r="AD4" s="4"/>
@@ -2656,61 +2662,61 @@
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="10" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="J5" s="10"/>
       <c r="K5" s="4"/>
       <c r="L5" s="9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="N5" s="4" t="s">
         <v>18</v>
       </c>
       <c r="O5" s="4"/>
       <c r="P5" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="R5" s="6" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="S5" s="6"/>
       <c r="T5" s="6" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="U5" s="6"/>
       <c r="V5" s="6"/>
       <c r="W5" s="19" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="X5" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="Y5" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="Z5" s="4" t="s">
         <v>18</v>
       </c>
       <c r="AA5" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AB5" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="AC5" s="4"/>
       <c r="AD5" s="4"/>
@@ -2736,7 +2742,7 @@
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -2745,12 +2751,12 @@
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="M6" s="4"/>
       <c r="N6" s="4" t="s">
@@ -2758,37 +2764,37 @@
       </c>
       <c r="O6" s="4"/>
       <c r="P6" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="R6" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="S6" s="6"/>
       <c r="T6" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
       <c r="W6" s="19" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="X6" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="Y6" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="Z6" s="4" t="s">
         <v>18</v>
       </c>
       <c r="AA6" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AB6" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AC6" s="4"/>
       <c r="AD6" s="4"/>
@@ -2814,61 +2820,61 @@
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="10" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="J7" s="10"/>
       <c r="K7" s="4"/>
       <c r="L7" s="9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="N7" s="4" t="s">
         <v>18</v>
       </c>
       <c r="O7" s="4"/>
       <c r="P7" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="S7" s="6"/>
       <c r="T7" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="U7" s="6"/>
       <c r="V7" s="6"/>
       <c r="W7" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="X7" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y7" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA7" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB7" s="4" t="s">
         <v>116</v>
-      </c>
-      <c r="X7" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="Y7" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="Z7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="AA7" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="AB7" s="4" t="s">
-        <v>115</v>
       </c>
       <c r="AC7" s="4"/>
       <c r="AD7" s="4"/>
@@ -2894,7 +2900,7 @@
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="13" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E8" s="13"/>
       <c r="F8" s="4" t="s">
@@ -2919,16 +2925,16 @@
       <c r="W8" s="20"/>
       <c r="X8" s="5"/>
       <c r="Y8" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="Z8" s="4" t="s">
         <v>18</v>
       </c>
       <c r="AA8" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AB8" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AC8" s="4"/>
       <c r="AD8" s="4"/>
@@ -2947,10 +2953,10 @@
         <v>3</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="5"/>
@@ -2958,62 +2964,62 @@
         <v>53704</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="K9" s="5"/>
       <c r="L9" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="M9" s="5"/>
       <c r="N9" s="5" t="s">
         <v>18</v>
       </c>
       <c r="O9" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="P9" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="R9" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="S9" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="T9" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="U9" s="5"/>
       <c r="V9" s="5"/>
       <c r="W9" s="20" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="X9" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="Y9" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="Z9" s="4" t="s">
         <v>18</v>
       </c>
       <c r="AA9" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AB9" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AC9" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="AD9" s="4"/>
       <c r="AE9" s="4" t="s">
@@ -3037,50 +3043,50 @@
         <v>3</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E10" s="22"/>
       <c r="G10" s="13">
         <v>53704</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="N10" s="5" t="s">
         <v>18</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q10" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="R10" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="T10" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="W10" s="20" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="X10" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="Y10" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="Z10" s="4" t="s">
         <v>18</v>
       </c>
       <c r="AA10" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AB10" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AD10" s="17" t="s">
         <v>20</v>
@@ -3095,7 +3101,7 @@
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="18" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E11" s="18"/>
       <c r="F11" s="18"/>
@@ -3104,12 +3110,12 @@
       </c>
       <c r="H11" s="18"/>
       <c r="I11" s="18" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J11" s="18"/>
       <c r="K11" s="18"/>
       <c r="L11" s="18" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="M11" s="18"/>
       <c r="N11" s="18" t="s">
@@ -3117,37 +3123,37 @@
       </c>
       <c r="O11" s="18"/>
       <c r="P11" s="18" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q11" s="18" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="R11" s="18" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="S11" s="18"/>
       <c r="T11" s="18" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="U11" s="18"/>
       <c r="V11" s="18"/>
       <c r="W11" s="21" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="X11" s="18" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="Y11" s="18" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="Z11" s="18" t="s">
         <v>18</v>
       </c>
       <c r="AA11" s="18" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AB11" s="18" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AC11" s="18"/>
       <c r="AD11" s="18"/>
@@ -3174,7 +3180,7 @@
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="18" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
@@ -3183,12 +3189,12 @@
       </c>
       <c r="H12" s="18"/>
       <c r="I12" s="18" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J12" s="18"/>
       <c r="K12" s="18"/>
       <c r="L12" s="18" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="M12" s="18"/>
       <c r="N12" s="18" t="s">
@@ -3196,39 +3202,39 @@
       </c>
       <c r="O12" s="18"/>
       <c r="P12" s="18" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q12" s="18" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="R12" s="18" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="S12" s="18"/>
       <c r="T12" s="18" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="U12" s="18"/>
       <c r="V12" s="18" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="W12" s="21" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="X12" s="18" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="Y12" s="18" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="Z12" s="18" t="s">
         <v>18</v>
       </c>
       <c r="AA12" s="18" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AB12" s="18" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AC12" s="18"/>
       <c r="AD12" s="18"/>
@@ -3250,7 +3256,7 @@
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -3259,49 +3265,49 @@
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="M13" s="4"/>
       <c r="N13" s="4" t="s">
         <v>18</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q13" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="R13" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="S13" s="6"/>
       <c r="T13" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="U13" s="6"/>
       <c r="V13" s="6"/>
       <c r="W13" s="19" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="X13" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="Y13" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="Z13" s="4" t="s">
         <v>18</v>
       </c>
       <c r="AA13" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AB13" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AC13" s="4"/>
       <c r="AD13" s="4"/>
@@ -3326,7 +3332,7 @@
         <v>3</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E14" t="s">
         <v>18</v>
@@ -3376,10 +3382,10 @@
         <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -3387,13 +3393,13 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -3418,7 +3424,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D4" t="s">
         <v>18</v>
@@ -3463,10 +3469,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -3474,10 +3480,10 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -3575,112 +3581,112 @@
         <v>1</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F1" s="27" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G1" s="27" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H1" s="27" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I1" s="27" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J1" s="27" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="K1" s="28" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="L1" s="31" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="M1" s="34" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="N1" s="34" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="O1" s="34" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="P1" s="34" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="Q1" s="34" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="R1" s="34" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="S1" s="34" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="T1" s="34" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="U1" s="34" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="V1" s="34" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="W1" s="34" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="X1" s="34" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="Y1" s="34" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Z1" s="34" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="AA1" s="34" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="AB1" s="34" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AC1" s="34" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="AD1" s="34" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="AE1" s="34" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="AF1" s="34" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="AG1" s="34" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="AH1" s="34" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="AI1" s="34" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="AJ1" s="34" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="AK1" s="34" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AL1" s="31" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:38">
@@ -3689,112 +3695,112 @@
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="M2" s="5" t="s">
         <v>13</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="V2" s="5" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="W2" s="5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="X2" s="5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="Y2" s="5" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="Z2" s="5" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="AA2" s="5" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="AB2" s="5" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="AC2" s="5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="AD2" s="5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AE2" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="AF2" s="5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="AG2" s="5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="AH2" s="5" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="AI2" s="5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="AJ2" s="5" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="AK2" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="AL2" s="5" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:38">
@@ -3819,13 +3825,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E4" s="36" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F4" s="16"/>
       <c r="H4" s="37"/>
@@ -3871,31 +3877,31 @@
       <c r="D5" s="5"/>
       <c r="E5" s="29"/>
       <c r="F5" s="29" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G5" s="32" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H5" s="29" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="I5" s="32">
         <v>3</v>
       </c>
       <c r="J5" s="33" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="K5" s="29" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="L5" s="5" t="s">
         <v>18</v>
       </c>
       <c r="M5" s="29" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="N5" s="29" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="O5" s="29" t="s">
         <v>18</v>
@@ -3999,10 +4005,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="40" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D1" s="40" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
@@ -4174,7 +4180,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -4183,7 +4189,7 @@
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -4208,7 +4214,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -4219,7 +4225,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -4230,7 +4236,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -4241,7 +4247,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>